<commit_message>
Make windows bat and linux sh file to run pipeline.
</commit_message>
<xml_diff>
--- a/analyze_nhej/libinfo.xlsx
+++ b/analyze_nhej/libinfo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\analyze_nhej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D0C665C-CA95-46E5-ADC1-419AEDC8F03A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE94EBC-C2E5-44BA-964F-B18EB30A3E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1537" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="189">
   <si>
     <t>yjl217</t>
   </si>
@@ -652,6 +652,12 @@
   <si>
     <t>universal_layout_legend_pos_x</t>
   </si>
+  <si>
+    <t>full_command_main</t>
+  </si>
+  <si>
+    <t>full_command_graph</t>
+  </si>
 </sst>
 </file>
 
@@ -771,6 +777,12 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FFD19645-61C4-4244-A560-0232B787F38C}"/>
   </cellStyles>
   <dxfs count="200">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1488,12 +1500,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1984,44 +1990,44 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="98">
   <autoFilter ref="A1:M41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="13">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="95"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="94">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="97"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="96">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="93">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="95">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="92">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="94">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="91">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="93">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="90">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="92">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="89">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="91">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="88">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="90">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="87">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="89">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="86">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="88">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="85">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="87">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="84">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="86">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="83">
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="85">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2034,40 +2040,40 @@
   <autoFilter ref="A43:M55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
-    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="82">
+    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="84">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="81">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="83">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="80">
+    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="82">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="79">
+    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="81">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="78">
+    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="80">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="77">
+    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="79">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="76">
+    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="78">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="75">
+    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="77">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="74">
+    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="76">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="73">
+    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="75">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="72">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="74">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="71">
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="73">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2076,36 +2082,36 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="72">
   <autoFilter ref="A3:I4" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="69"/>
-    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="68">
+    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="71"/>
+    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="70">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="67">
+    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="69">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="66">
+    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="68">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="65">
+    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="67">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 12 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="33" xr3:uid="{8FF7E83A-9135-4A64-965C-48368A6C0367}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="64">
+    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="66">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="63">
+    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="65">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="62">
+    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="64">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2114,32 +2120,32 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="63">
   <autoFilter ref="A7:I9" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="60"/>
-    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="59">
+    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="62"/>
+    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="61">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="58">
+    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="60">
       <calculatedColumnFormula>IF(table_6_4[[#This Row],[hguide]]="A",NA(), IF(var_6_layout = "universal", "1 1 1 1 1 1", NA()))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="57">
+    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="59">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="56">
+    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="58">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" xr3:uid="{5BD83012-469D-4202-9584-AA182CDF11F9}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="55">
+    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="57">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="54">
+    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="56">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="53">
+    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="55">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2148,36 +2154,36 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="54" headerRowBorderDxfId="53" tableBorderDxfId="52">
   <autoFilter ref="A12:I13" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0F421990-E775-4F35-92AF-6BA19E0E8AEE}" name="index"/>
-    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="49">
+    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="51">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="48">
+    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="50">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0,4, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="47">
+    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="49">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="46">
+    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="48">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{E0783723-9246-4BF6-A5DA-E000EA1E5E87}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="45">
+    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="47">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="44">
+    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="46">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="43">
+    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="45">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2186,44 +2192,44 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:R42" totalsRowShown="0" headerRowDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:R42" totalsRowShown="0" headerRowDxfId="44">
   <autoFilter ref="A2:R42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="18">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="41"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="40">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="43"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="42">
       <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="39">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="41">
       <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="38">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="40">
       <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="37">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="39">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="36">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="38">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="35">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="37">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="34">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="36">
       <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="33">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="35">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="32">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="34">
       <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="31">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="33">
       <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="30">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="32">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="29">
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="31">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
       OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
       IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
@@ -2235,19 +2241,19 @@
       )
   )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="28">
+    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="30">
       <calculatedColumnFormula>AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="27">
+    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="29">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 13 --range_y -22 22 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 13 --range_y -18 25 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 13 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 13 --range_y -20 16 ", NA())))), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{891739FF-B093-4EE5-A0A2-20948C58CB96}" name="universal_layout_legend_pos_x" dataDxfId="26">
+    <tableColumn id="17" xr3:uid="{891739FF-B093-4EE5-A0A2-20948C58CB96}" name="universal_layout_legend_pos_x" dataDxfId="28">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 12, IF(table_7_1[[#This Row],[hguide]]="A", 12, IF(table_7_1[[#This Row],[hguide]]="B", 12, IF(table_7_1[[#This Row],[hguide]]="CD", 12, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="25">
+    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="27">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/individual/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="24">
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="26">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], IF(NOT(ISNA(table_7_1[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_1[[#This Row],[universal_layout_legend_pos_x]], "")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2256,38 +2262,38 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:K60" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:K60" totalsRowShown="0" headerRowDxfId="25">
   <autoFilter ref="A44:K60" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="23">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="20">
+    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="22">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="19">
+    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="18">
+    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="20">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="17">
+    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="19">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="16">
+    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="18">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="15">
+    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="17">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_legend_pos_x" dataDxfId="14">
+    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_legend_pos_x" dataDxfId="16">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_legend_pos_x]:[universal_layout_legend_pos_x]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="13">
+    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="15">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="14">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], IF(NOT(ISNA(table_7_2[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_2[[#This Row],[universal_layout_legend_pos_x]], "")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2296,38 +2302,38 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:K64" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:K64" totalsRowShown="0" headerRowDxfId="13">
   <autoFilter ref="A62:K64" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="11">
       <calculatedColumnFormula>OFFSET(table_4_2[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="10">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="7">
+    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="6">
+    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="8">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="7">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="6">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="3">
+    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="5">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_legend_pos_x" dataDxfId="2">
+    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_legend_pos_x" dataDxfId="4">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_legend_pos_x]:[universal_layout_legend_pos_x]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="1">
+    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], IF(NOT(ISNA(table_7_3[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_3[[#This Row],[universal_layout_legend_pos_x]], "")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2632,28 +2638,28 @@
     <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="116">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="115">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="1">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="114">
+    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="115">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="113">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="0">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="112">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="114">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_2[[#This Row],[treatment_1]], "_", table_4_2[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="111">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="113">
       <calculatedColumnFormula>SUBSTITUTE(table_4_2[[#This Row],[dir_1]], table_4_2[[#This Row],[treatment_1]], table_4_2[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="110">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="112">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_2[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_2[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_2[[#This Row],[dir_out]], " --subst_type ", table_4_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="109">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="111">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_2[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2662,38 +2668,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="110">
   <autoFilter ref="A25:K33" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="107"/>
-    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="106">
+    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="109"/>
+    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="108">
       <calculatedColumnFormula>OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="105">
+    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="107">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="104">
+    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="106">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="103">
+    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="105">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="102">
+    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="104">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="101">
+    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="103">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_3[[#This Row],[treatment_1]], "_", table_4_3[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="100">
+    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="102">
       <calculatedColumnFormula>SUBSTITUTE(table_4_3[[#This Row],[dir_1]], table_4_3[[#This Row],[treatment_1]], table_4_3[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="99">
+    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="101">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="98">
+    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="100">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_3[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_3[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_3[[#This Row],[dir_out]], " --subst_type ", table_4_3[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="97">
+    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="99">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_3[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_3[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3067,7 +3073,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5334D33C-3E16-4C4F-BA76-1F06B33FAC0B}">
   <dimension ref="A1:D108"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -4705,10 +4711,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F1EACD-27DC-4973-8E3A-9162F610D9C4}">
-  <dimension ref="A1:O173"/>
+  <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B157" workbookViewId="0">
-      <selection activeCell="M98" sqref="M98"/>
+    <sheetView topLeftCell="B169" workbookViewId="0">
+      <selection activeCell="B176" sqref="B176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14064,6 +14070,188 @@
         <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl283_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl283_KO_sgB_R2_cmv_nodsb.tsv --min_length 130 -dsb 46 --quiet</v>
       </c>
     </row>
+    <row r="175" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B175" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="176" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B176" t="str">
+        <f>_xlfn.TEXTJOIN(CHAR(10), TRUE, table_1[command_filter_nhej])</f>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl217_R1_2DSBs.sam -ref ref_seq/2DSB_R1_sense.fa -o libraries_2/yjl217_WT_sgAB_R1_sense.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl218_R1_2DSBs.sam -ref ref_seq/2DSB_R1_sense.fa -o libraries_2/yjl218_WT_sgAB_R1_sense.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl219_R1_2DSBs.sam -ref ref_seq/2DSB_R1_sense.fa -o libraries_2/yjl219_WT_sgAB_R1_sense.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl220_R1_2DSBs.sam -ref ref_seq/2DSB_R1_sense.fa -o libraries_2/yjl220_WT_sgAB_R1_sense.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl221_R1_2DSBs.sam -ref ref_seq/2DSB_R1_branch.fa -o libraries_2/yjl221_WT_sgAB_R1_branch.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl222_R1_2DSBs.sam -ref ref_seq/2DSB_R1_branch.fa -o libraries_2/yjl222_WT_sgAB_R1_branch.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl223_R1_2DSBs.sam -ref ref_seq/2DSB_R1_branch.fa -o libraries_2/yjl223_WT_sgAB_R1_branch.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl224_R1_2DSBs.sam -ref ref_seq/2DSB_R1_branch.fa -o libraries_2/yjl224_WT_sgAB_R1_branch.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl225_R1_2DSBs.sam -ref ref_seq/2DSB_R1_cmv.fa -o libraries_2/yjl225_WT_sgAB_R1_cmv.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl226_R1_2DSBs.sam -ref ref_seq/2DSB_R1_cmv.fa -o libraries_2/yjl226_WT_sgAB_R1_cmv.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl227_R1_2DSBs.sam -ref ref_seq/2DSB_R1_cmv.fa -o libraries_2/yjl227_WT_sgAB_R1_cmv.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl228_R1_2DSBs.sam -ref ref_seq/2DSB_R1_cmv.fa -o libraries_2/yjl228_WT_sgAB_R1_cmv.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl229_R1_2DSBs.sam -ref ref_seq/2DSB_R1_sense.fa -o libraries_2/yjl229_KO_sgAB_R1_sense.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl230_R1_2DSBs.sam -ref ref_seq/2DSB_R1_sense.fa -o libraries_2/yjl230_KO_sgAB_R1_sense.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl231_R1_2DSBs.sam -ref ref_seq/2DSB_R1_sense.fa -o libraries_2/yjl231_KO_sgAB_R1_sense.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl232_R1_2DSBs.sam -ref ref_seq/2DSB_R1_sense.fa -o libraries_2/yjl232_KO_sgAB_R1_sense.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl233_R1_2DSBs.sam -ref ref_seq/2DSB_R1_branch.fa -o libraries_2/yjl233_KO_sgAB_R1_branch.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl234_R1_2DSBs.sam -ref ref_seq/2DSB_R1_branch.fa -o libraries_2/yjl234_KO_sgAB_R1_branch.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl235_R1_2DSBs.sam -ref ref_seq/2DSB_R1_branch.fa -o libraries_2/yjl235_KO_sgAB_R1_branch.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl236_R1_2DSBs.sam -ref ref_seq/2DSB_R1_branch.fa -o libraries_2/yjl236_KO_sgAB_R1_branch.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl237_R1_2DSBs.sam -ref ref_seq/2DSB_R1_cmv.fa -o libraries_2/yjl237_KO_sgAB_R1_cmv.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl238_R1_2DSBs.sam -ref ref_seq/2DSB_R1_cmv.fa -o libraries_2/yjl238_KO_sgAB_R1_cmv.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl239_R1_2DSBs.sam -ref ref_seq/2DSB_R1_cmv.fa -o libraries_2/yjl239_KO_sgAB_R1_cmv.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl240_R1_2DSBs.sam -ref ref_seq/2DSB_R1_cmv.fa -o libraries_2/yjl240_KO_sgAB_R1_cmv.tsv --min_length 50 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl217_R2_2DSBs.sam -ref ref_seq/2DSB_R2_sense.fa -o libraries_2/yjl217_WT_sgAB_R2_sense.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl218_R2_2DSBs.sam -ref ref_seq/2DSB_R2_sense.fa -o libraries_2/yjl218_WT_sgAB_R2_sense.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl219_R2_2DSBs.sam -ref ref_seq/2DSB_R2_sense.fa -o libraries_2/yjl219_WT_sgAB_R2_sense.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl220_R2_2DSBs.sam -ref ref_seq/2DSB_R2_sense.fa -o libraries_2/yjl220_WT_sgAB_R2_sense.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl221_R2_2DSBs.sam -ref ref_seq/2DSB_R2_branch.fa -o libraries_2/yjl221_WT_sgAB_R2_branch.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl222_R2_2DSBs.sam -ref ref_seq/2DSB_R2_branch.fa -o libraries_2/yjl222_WT_sgAB_R2_branch.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl223_R2_2DSBs.sam -ref ref_seq/2DSB_R2_branch.fa -o libraries_2/yjl223_WT_sgAB_R2_branch.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl224_R2_2DSBs.sam -ref ref_seq/2DSB_R2_branch.fa -o libraries_2/yjl224_WT_sgAB_R2_branch.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl225_R2_2DSBs.sam -ref ref_seq/2DSB_R2_cmv.fa -o libraries_2/yjl225_WT_sgAB_R2_cmv.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl226_R2_2DSBs.sam -ref ref_seq/2DSB_R2_cmv.fa -o libraries_2/yjl226_WT_sgAB_R2_cmv.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl227_R2_2DSBs.sam -ref ref_seq/2DSB_R2_cmv.fa -o libraries_2/yjl227_WT_sgAB_R2_cmv.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl228_R2_2DSBs.sam -ref ref_seq/2DSB_R2_cmv.fa -o libraries_2/yjl228_WT_sgAB_R2_cmv.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl229_R2_2DSBs.sam -ref ref_seq/2DSB_R2_sense.fa -o libraries_2/yjl229_KO_sgAB_R2_sense.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl230_R2_2DSBs.sam -ref ref_seq/2DSB_R2_sense.fa -o libraries_2/yjl230_KO_sgAB_R2_sense.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl231_R2_2DSBs.sam -ref ref_seq/2DSB_R2_sense.fa -o libraries_2/yjl231_KO_sgAB_R2_sense.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl232_R2_2DSBs.sam -ref ref_seq/2DSB_R2_sense.fa -o libraries_2/yjl232_KO_sgAB_R2_sense.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl233_R2_2DSBs.sam -ref ref_seq/2DSB_R2_branch.fa -o libraries_2/yjl233_KO_sgAB_R2_branch.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl234_R2_2DSBs.sam -ref ref_seq/2DSB_R2_branch.fa -o libraries_2/yjl234_KO_sgAB_R2_branch.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl235_R2_2DSBs.sam -ref ref_seq/2DSB_R2_branch.fa -o libraries_2/yjl235_KO_sgAB_R2_branch.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl236_R2_2DSBs.sam -ref ref_seq/2DSB_R2_branch.fa -o libraries_2/yjl236_KO_sgAB_R2_branch.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl237_R2_2DSBs.sam -ref ref_seq/2DSB_R2_cmv.fa -o libraries_2/yjl237_KO_sgAB_R2_cmv.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl238_R2_2DSBs.sam -ref ref_seq/2DSB_R2_cmv.fa -o libraries_2/yjl238_KO_sgAB_R2_cmv.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl239_R2_2DSBs.sam -ref ref_seq/2DSB_R2_cmv.fa -o libraries_2/yjl239_KO_sgAB_R2_cmv.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl240_R2_2DSBs.sam -ref ref_seq/2DSB_R2_cmv.fa -o libraries_2/yjl240_KO_sgAB_R2_cmv.tsv --min_length 50 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl255_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl255_WT_sgA_R1_sense.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl256_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl256_WT_sgA_R1_sense.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl257_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl257_WT_sgA_R1_sense.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl258_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl258_WT_sgA_R1_sense.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl259_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl259_WT_sgA_R1_branch.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl260_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl260_WT_sgA_R1_branch.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl261_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl261_WT_sgA_R1_branch.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl262_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl262_WT_sgA_R1_branch.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl263_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl263_WT_sgA_R1_cmv.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl264_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl264_WT_sgA_R1_cmv.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl265_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl265_WT_sgA_R1_cmv.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl266_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl266_WT_sgA_R1_cmv.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl292_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl292_KO_sgA_R1_sense.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl293_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl293_KO_sgA_R1_sense.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl294_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl294_KO_sgA_R1_sense.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl295_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl295_KO_sgA_R1_sense.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl296_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl296_KO_sgA_R1_branch.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl297_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl297_KO_sgA_R1_branch.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl298_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl298_KO_sgA_R1_branch.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl299_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl299_KO_sgA_R1_branch.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl300_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl300_KO_sgA_R1_cmv.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl301_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl301_KO_sgA_R1_cmv.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl302_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl302_KO_sgA_R1_cmv.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl303_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl303_KO_sgA_R1_cmv.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl267_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl267_WT_sgB_R2_sense.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl268_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl268_WT_sgB_R2_sense.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl269_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl269_WT_sgB_R2_sense.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl270_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl270_WT_sgB_R2_sense.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl271_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl271_WT_sgB_R2_branch.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl272_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl272_WT_sgB_R2_branch.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl273_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl273_WT_sgB_R2_branch.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl274_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl274_WT_sgB_R2_branch.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl275_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl275_WT_sgB_R2_cmv.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl276_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl276_WT_sgB_R2_cmv.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl277_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl277_WT_sgB_R2_cmv.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl278_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl278_WT_sgB_R2_cmv.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl304_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl304_KO_sgB_R2_sense.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl305_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl305_KO_sgB_R2_sense.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl306_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl306_KO_sgB_R2_sense.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl307_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl307_KO_sgB_R2_sense.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl308_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl308_KO_sgB_R2_branch.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl309_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl309_KO_sgB_R2_branch.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl310_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl310_KO_sgB_R2_branch.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl311_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl311_KO_sgB_R2_branch.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl312_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl312_KO_sgB_R2_cmv.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl313_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl313_KO_sgB_R2_cmv.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl314_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl314_KO_sgB_R2_cmv.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl315_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl315_KO_sgB_R2_cmv.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl255_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl255_WT_sgA_R1_sense_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl256_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl256_WT_sgA_R1_sense_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl257_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl257_WT_sgA_R1_sense_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl258_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl258_WT_sgA_R1_sense_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl259_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl259_WT_sgA_R1_branch_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl260_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl260_WT_sgA_R1_branch_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl261_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl261_WT_sgA_R1_branch_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl262_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl262_WT_sgA_R1_branch_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl263_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl263_WT_sgA_R1_cmv_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl264_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl264_WT_sgA_R1_cmv_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl265_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl265_WT_sgA_R1_cmv_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl266_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl266_WT_sgA_R1_cmv_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl292_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl292_KO_sgA_R1_sense_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl293_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl293_KO_sgA_R1_sense_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl294_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl294_KO_sgA_R1_sense_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl295_R1_sgA.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl295_KO_sgA_R1_sense_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl296_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl296_KO_sgA_R1_branch_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl297_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl297_KO_sgA_R1_branch_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl298_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl298_KO_sgA_R1_branch_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl299_R1_sgA.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl299_KO_sgA_R1_branch_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl300_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl300_KO_sgA_R1_cmv_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl301_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl301_KO_sgA_R1_cmv_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl302_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl302_KO_sgA_R1_cmv_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl303_R1_sgA.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl303_KO_sgA_R1_cmv_30bpDown.tsv --min_length 130 -dsb 97 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl267_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl267_WT_sgB_R2_sense_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl268_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl268_WT_sgB_R2_sense_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl269_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl269_WT_sgB_R2_sense_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl270_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl270_WT_sgB_R2_sense_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl271_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl271_WT_sgB_R2_branch_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl272_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl272_WT_sgB_R2_branch_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl273_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl273_WT_sgB_R2_branch_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl274_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl274_WT_sgB_R2_branch_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl275_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl275_WT_sgB_R2_cmv_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl276_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl276_WT_sgB_R2_cmv_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl277_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl277_WT_sgB_R2_cmv_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl278_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl278_WT_sgB_R2_cmv_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl304_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl304_KO_sgB_R2_sense_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl305_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl305_KO_sgB_R2_sense_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl306_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl306_KO_sgB_R2_sense_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl307_R2_sgB.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl307_KO_sgB_R2_sense_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl308_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl308_KO_sgB_R2_branch_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl309_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl309_KO_sgB_R2_branch_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl310_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl310_KO_sgB_R2_branch_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl311_R2_sgB.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl311_KO_sgB_R2_branch_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl312_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl312_KO_sgB_R2_cmv_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl313_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl313_KO_sgB_R2_cmv_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl314_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl314_KO_sgB_R2_cmv_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl315_R2_sgB.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl315_KO_sgB_R2_cmv_30bpDown.tsv --min_length 130 -dsb 76 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl89_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl89_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 50 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl90_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl90_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 50 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl91_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl91_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 50 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl92_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_antisense.fa -o libraries_2/yjl92_WT_sgCD_R1_antisense.tsv --min_length 50 -dsb 50 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl93_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl93_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 50 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl94_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl94_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 50 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl95_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl95_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 50 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl96_anti_R1_2DSBs.sam -ref ref_seq/2DSBanti_R1_splicing.fa -o libraries_2/yjl96_WT_sgCD_R1_splicing.tsv --min_length 50 -dsb 50 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl89_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_antisense.fa -o libraries_2/yjl89_WT_sgCD_R2_antisense.tsv --min_length 50 -dsb 47 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl90_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_antisense.fa -o libraries_2/yjl90_WT_sgCD_R2_antisense.tsv --min_length 50 -dsb 47 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl91_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_antisense.fa -o libraries_2/yjl91_WT_sgCD_R2_antisense.tsv --min_length 50 -dsb 47 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl92_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_antisense.fa -o libraries_2/yjl92_WT_sgCD_R2_antisense.tsv --min_length 50 -dsb 47 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl93_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_splicing.fa -o libraries_2/yjl93_WT_sgCD_R2_splicing.tsv --min_length 50 -dsb 47 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl94_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_splicing.fa -o libraries_2/yjl94_WT_sgCD_R2_splicing.tsv --min_length 50 -dsb 47 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl95_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_splicing.fa -o libraries_2/yjl95_WT_sgCD_R2_splicing.tsv --min_length 50 -dsb 47 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl96_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_splicing.fa -o libraries_2/yjl96_WT_sgCD_R2_splicing.tsv --min_length 50 -dsb 47 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl244_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl244_WT_sgA_R1_sense_nodsb.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl245_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl245_WT_sgA_R1_branch_nodsb.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl246_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl246_WT_sgA_R1_cmv_nodsb.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl281_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl281_KO_sgA_R1_sense_nodsb.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl282_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl282_KO_sgA_R1_branch_nodsb.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl283_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl283_KO_sgA_R1_cmv_nodsb.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl244_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl244_WT_sgB_R2_sense_nodsb.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl245_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl245_WT_sgB_R2_branch_nodsb.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl246_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl246_WT_sgB_R2_cmv_nodsb.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl281_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl281_KO_sgB_R2_sense_nodsb.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl282_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl282_KO_sgB_R2_branch_nodsb.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl283_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl283_KO_sgB_R2_cmv_nodsb.tsv --min_length 130 -dsb 46 --quiet</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14076,10 +14264,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D704B5-D01A-4D17-9252-416EA08BC871}">
-  <dimension ref="A1:S56"/>
+  <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2"/>
+    <sheetView topLeftCell="H43" workbookViewId="0">
+      <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17922,6 +18110,68 @@
         <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl283_KO_sgB_R2_cmv_nodsb.tsv  --total_reads 7622513 -o libraries_3/KO_sgB_R2_cmv_nodsb.tsv --quiet </v>
       </c>
     </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H58" s="1" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H59" t="str">
+        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, S2:S41,M45:M56)</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl217_WT_sgAB_R1_sense.tsv libraries_2/yjl218_WT_sgAB_R1_sense.tsv libraries_2/yjl219_WT_sgAB_R1_sense.tsv libraries_4/yjl220_WT_sgAB_R1_sense.tsv --total_reads 6630053 7246619 8069391 7513691 -o libraries_3/WT_sgAB_R1_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl221_WT_sgAB_R1_branch.tsv libraries_2/yjl222_WT_sgAB_R1_branch.tsv libraries_2/yjl223_WT_sgAB_R1_branch.tsv libraries_4/yjl224_WT_sgAB_R1_branch.tsv --total_reads 9021462 9430938 9051278 9192054 -o libraries_3/WT_sgAB_R1_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl225_WT_sgAB_R1_cmv.tsv libraries_2/yjl226_WT_sgAB_R1_cmv.tsv libraries_2/yjl227_WT_sgAB_R1_cmv.tsv libraries_4/yjl228_WT_sgAB_R1_cmv.tsv --total_reads 7604379 8885716 8150455 7694818 -o libraries_3/WT_sgAB_R1_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl229_KO_sgAB_R1_sense.tsv libraries_2/yjl230_KO_sgAB_R1_sense.tsv libraries_2/yjl231_KO_sgAB_R1_sense.tsv libraries_4/yjl232_KO_sgAB_R1_sense.tsv --total_reads 11320509 12480734 12500966 12479012 -o libraries_3/KO_sgAB_R1_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl233_KO_sgAB_R1_branch.tsv libraries_2/yjl234_KO_sgAB_R1_branch.tsv libraries_2/yjl235_KO_sgAB_R1_branch.tsv libraries_4/yjl236_KO_sgAB_R1_branch.tsv --total_reads 13912975 15839537 13872702 13493608 -o libraries_3/KO_sgAB_R1_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl237_KO_sgAB_R1_cmv.tsv libraries_2/yjl238_KO_sgAB_R1_cmv.tsv libraries_2/yjl239_KO_sgAB_R1_cmv.tsv libraries_4/yjl240_KO_sgAB_R1_cmv.tsv --total_reads 11307677 11757615 10272339 9412394 -o libraries_3/KO_sgAB_R1_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl217_WT_sgAB_R2_sense.tsv libraries_2/yjl218_WT_sgAB_R2_sense.tsv libraries_2/yjl219_WT_sgAB_R2_sense.tsv libraries_4/yjl220_WT_sgAB_R2_sense.tsv --total_reads 6177083 6744517 7507107 7001340 -o libraries_3/WT_sgAB_R2_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl221_WT_sgAB_R2_branch.tsv libraries_2/yjl222_WT_sgAB_R2_branch.tsv libraries_2/yjl223_WT_sgAB_R2_branch.tsv libraries_4/yjl224_WT_sgAB_R2_branch.tsv --total_reads 8525251 8875435 8522228 8656502 -o libraries_3/WT_sgAB_R2_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl225_WT_sgAB_R2_cmv.tsv libraries_2/yjl226_WT_sgAB_R2_cmv.tsv libraries_2/yjl227_WT_sgAB_R2_cmv.tsv libraries_4/yjl228_WT_sgAB_R2_cmv.tsv --total_reads 6898791 7986453 7354088 6940576 -o libraries_3/WT_sgAB_R2_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl229_KO_sgAB_R2_sense.tsv libraries_2/yjl230_KO_sgAB_R2_sense.tsv libraries_2/yjl231_KO_sgAB_R2_sense.tsv libraries_4/yjl232_KO_sgAB_R2_sense.tsv --total_reads 10142826 11211467 11130391 11080481 -o libraries_3/KO_sgAB_R2_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl233_KO_sgAB_R2_branch.tsv libraries_2/yjl234_KO_sgAB_R2_branch.tsv libraries_2/yjl235_KO_sgAB_R2_branch.tsv libraries_4/yjl236_KO_sgAB_R2_branch.tsv --total_reads 12987477 14745821 12946604 12582077 -o libraries_3/KO_sgAB_R2_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl237_KO_sgAB_R2_cmv.tsv libraries_2/yjl238_KO_sgAB_R2_cmv.tsv libraries_2/yjl239_KO_sgAB_R2_cmv.tsv libraries_4/yjl240_KO_sgAB_R2_cmv.tsv --total_reads 10562895 10985096 9559721 8729797 -o libraries_3/KO_sgAB_R2_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl255_WT_sgA_R1_sense.tsv libraries_2/yjl256_WT_sgA_R1_sense.tsv libraries_2/yjl257_WT_sgA_R1_sense.tsv libraries_4/yjl258_WT_sgA_R1_sense.tsv --total_reads 7579965 7982725 7854740 7534924 -o libraries_3/WT_sgA_R1_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl259_WT_sgA_R1_branch.tsv libraries_2/yjl260_WT_sgA_R1_branch.tsv libraries_2/yjl261_WT_sgA_R1_branch.tsv libraries_4/yjl262_WT_sgA_R1_branch.tsv --total_reads 8808358 9297647 9399483 8799841 -o libraries_3/WT_sgA_R1_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl263_WT_sgA_R1_cmv.tsv libraries_2/yjl264_WT_sgA_R1_cmv.tsv libraries_2/yjl265_WT_sgA_R1_cmv.tsv libraries_4/yjl266_WT_sgA_R1_cmv.tsv --total_reads 8171224 8180897 8314116 8096639 -o libraries_3/WT_sgA_R1_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl292_KO_sgA_R1_sense.tsv libraries_2/yjl293_KO_sgA_R1_sense.tsv libraries_2/yjl294_KO_sgA_R1_sense.tsv libraries_4/yjl295_KO_sgA_R1_sense.tsv --total_reads 8597510 10116623 8703707 9021103 -o libraries_3/KO_sgA_R1_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl296_KO_sgA_R1_branch.tsv libraries_2/yjl297_KO_sgA_R1_branch.tsv libraries_2/yjl298_KO_sgA_R1_branch.tsv libraries_4/yjl299_KO_sgA_R1_branch.tsv --total_reads 11021111 11280773 12426852 11659042 -o libraries_3/KO_sgA_R1_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl300_KO_sgA_R1_cmv.tsv libraries_2/yjl301_KO_sgA_R1_cmv.tsv libraries_2/yjl302_KO_sgA_R1_cmv.tsv libraries_4/yjl303_KO_sgA_R1_cmv.tsv --total_reads 9933546 10351309 9388188 8668198 -o libraries_3/KO_sgA_R1_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl267_WT_sgB_R2_sense.tsv libraries_2/yjl268_WT_sgB_R2_sense.tsv libraries_2/yjl269_WT_sgB_R2_sense.tsv libraries_4/yjl270_WT_sgB_R2_sense.tsv --total_reads 7137355 6618133 8227882 7238408 -o libraries_3/WT_sgB_R2_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl271_WT_sgB_R2_branch.tsv libraries_2/yjl272_WT_sgB_R2_branch.tsv libraries_2/yjl273_WT_sgB_R2_branch.tsv libraries_4/yjl274_WT_sgB_R2_branch.tsv --total_reads 9524548 10125834 10173904 9525100 -o libraries_3/WT_sgB_R2_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl275_WT_sgB_R2_cmv.tsv libraries_2/yjl276_WT_sgB_R2_cmv.tsv libraries_2/yjl277_WT_sgB_R2_cmv.tsv libraries_4/yjl278_WT_sgB_R2_cmv.tsv --total_reads 7280860 6872217 6847531 7081713 -o libraries_3/WT_sgB_R2_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl304_KO_sgB_R2_sense.tsv libraries_2/yjl305_KO_sgB_R2_sense.tsv libraries_2/yjl306_KO_sgB_R2_sense.tsv libraries_4/yjl307_KO_sgB_R2_sense.tsv --total_reads 6494964 7011524 7131423 6545416 -o libraries_3/KO_sgB_R2_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl308_KO_sgB_R2_branch.tsv libraries_2/yjl309_KO_sgB_R2_branch.tsv libraries_2/yjl310_KO_sgB_R2_branch.tsv libraries_4/yjl311_KO_sgB_R2_branch.tsv --total_reads 9730255 10430885 9770845 10249893 -o libraries_3/KO_sgB_R2_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl312_KO_sgB_R2_cmv.tsv libraries_2/yjl313_KO_sgB_R2_cmv.tsv libraries_2/yjl314_KO_sgB_R2_cmv.tsv libraries_4/yjl315_KO_sgB_R2_cmv.tsv --total_reads 6718301 6435913 7285831 6372479 -o libraries_3/KO_sgB_R2_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl255_WT_sgA_R1_sense_30bpDown.tsv libraries_2/yjl256_WT_sgA_R1_sense_30bpDown.tsv libraries_2/yjl257_WT_sgA_R1_sense_30bpDown.tsv libraries_4/yjl258_WT_sgA_R1_sense_30bpDown.tsv --total_reads 7579965 7982725 7854740 7534924 -o libraries_3/WT_sgA_R1_sense_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl259_WT_sgA_R1_branch_30bpDown.tsv libraries_2/yjl260_WT_sgA_R1_branch_30bpDown.tsv libraries_2/yjl261_WT_sgA_R1_branch_30bpDown.tsv libraries_4/yjl262_WT_sgA_R1_branch_30bpDown.tsv --total_reads 8808358 9297647 9399483 8799841 -o libraries_3/WT_sgA_R1_branch_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl263_WT_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl264_WT_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl265_WT_sgA_R1_cmv_30bpDown.tsv libraries_4/yjl266_WT_sgA_R1_cmv_30bpDown.tsv --total_reads 8171224 8180897 8314116 8096639 -o libraries_3/WT_sgA_R1_cmv_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl292_KO_sgA_R1_sense_30bpDown.tsv libraries_2/yjl293_KO_sgA_R1_sense_30bpDown.tsv libraries_2/yjl294_KO_sgA_R1_sense_30bpDown.tsv libraries_4/yjl295_KO_sgA_R1_sense_30bpDown.tsv --total_reads 8597510 10116623 8703707 9021103 -o libraries_3/KO_sgA_R1_sense_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl296_KO_sgA_R1_branch_30bpDown.tsv libraries_2/yjl297_KO_sgA_R1_branch_30bpDown.tsv libraries_2/yjl298_KO_sgA_R1_branch_30bpDown.tsv libraries_4/yjl299_KO_sgA_R1_branch_30bpDown.tsv --total_reads 11021111 11280773 12426852 11659042 -o libraries_3/KO_sgA_R1_branch_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl300_KO_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl301_KO_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl302_KO_sgA_R1_cmv_30bpDown.tsv libraries_4/yjl303_KO_sgA_R1_cmv_30bpDown.tsv --total_reads 9933546 10351309 9388188 8668198 -o libraries_3/KO_sgA_R1_cmv_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl267_WT_sgB_R2_sense_30bpDown.tsv libraries_2/yjl268_WT_sgB_R2_sense_30bpDown.tsv libraries_2/yjl269_WT_sgB_R2_sense_30bpDown.tsv libraries_4/yjl270_WT_sgB_R2_sense_30bpDown.tsv --total_reads 7137355 6618133 8227882 7238408 -o libraries_3/WT_sgB_R2_sense_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl271_WT_sgB_R2_branch_30bpDown.tsv libraries_2/yjl272_WT_sgB_R2_branch_30bpDown.tsv libraries_2/yjl273_WT_sgB_R2_branch_30bpDown.tsv libraries_4/yjl274_WT_sgB_R2_branch_30bpDown.tsv --total_reads 9524548 10125834 10173904 9525100 -o libraries_3/WT_sgB_R2_branch_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl275_WT_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl276_WT_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl277_WT_sgB_R2_cmv_30bpDown.tsv libraries_4/yjl278_WT_sgB_R2_cmv_30bpDown.tsv --total_reads 7280860 6872217 6847531 7081713 -o libraries_3/WT_sgB_R2_cmv_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl304_KO_sgB_R2_sense_30bpDown.tsv libraries_2/yjl305_KO_sgB_R2_sense_30bpDown.tsv libraries_2/yjl306_KO_sgB_R2_sense_30bpDown.tsv libraries_4/yjl307_KO_sgB_R2_sense_30bpDown.tsv --total_reads 6494964 7011524 7131423 6545416 -o libraries_3/KO_sgB_R2_sense_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl308_KO_sgB_R2_branch_30bpDown.tsv libraries_2/yjl309_KO_sgB_R2_branch_30bpDown.tsv libraries_2/yjl310_KO_sgB_R2_branch_30bpDown.tsv libraries_4/yjl311_KO_sgB_R2_branch_30bpDown.tsv --total_reads 9730255 10430885 9770845 10249893 -o libraries_3/KO_sgB_R2_branch_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl312_KO_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl313_KO_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl314_KO_sgB_R2_cmv_30bpDown.tsv libraries_4/yjl315_KO_sgB_R2_cmv_30bpDown.tsv --total_reads 6718301 6435913 7285831 6372479 -o libraries_3/KO_sgB_R2_cmv_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl89_WT_sgCD_R1_antisense.tsv libraries_2/yjl90_WT_sgCD_R1_antisense.tsv libraries_2/yjl91_WT_sgCD_R1_antisense.tsv libraries_4/yjl92_WT_sgCD_R1_antisense.tsv --total_reads 7813781 7486736 8114856 6586577 -o libraries_3/WT_sgCD_R1_antisense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl93_WT_sgCD_R1_splicing.tsv libraries_2/yjl94_WT_sgCD_R1_splicing.tsv libraries_2/yjl95_WT_sgCD_R1_splicing.tsv libraries_4/yjl96_WT_sgCD_R1_splicing.tsv --total_reads 9334492 9142001 8497185 8346242 -o libraries_3/WT_sgCD_R1_splicing.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl89_WT_sgCD_R2_antisense.tsv libraries_2/yjl90_WT_sgCD_R2_antisense.tsv libraries_2/yjl91_WT_sgCD_R2_antisense.tsv libraries_4/yjl92_WT_sgCD_R2_antisense.tsv --total_reads 7813781 7486736 8114856 6586577 -o libraries_3/WT_sgCD_R2_antisense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl93_WT_sgCD_R2_splicing.tsv libraries_2/yjl94_WT_sgCD_R2_splicing.tsv libraries_2/yjl95_WT_sgCD_R2_splicing.tsv libraries_4/yjl96_WT_sgCD_R2_splicing.tsv --total_reads 9334492 9142001 8497185 8346242 -o libraries_3/WT_sgCD_R2_splicing.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl244_WT_sgA_R1_sense_nodsb.tsv  --total_reads 10005232 -o libraries_3/WT_sgA_R1_sense_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl245_WT_sgA_R1_branch_nodsb.tsv  --total_reads 12898941 -o libraries_3/WT_sgA_R1_branch_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl246_WT_sgA_R1_cmv_nodsb.tsv  --total_reads 10217401 -o libraries_3/WT_sgA_R1_cmv_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl281_KO_sgA_R1_sense_nodsb.tsv  --total_reads 7424148 -o libraries_3/KO_sgA_R1_sense_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl282_KO_sgA_R1_branch_nodsb.tsv  --total_reads 10190833 -o libraries_3/KO_sgA_R1_branch_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl283_KO_sgA_R1_cmv_nodsb.tsv  --total_reads 7763439 -o libraries_3/KO_sgA_R1_cmv_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl244_WT_sgB_R2_sense_nodsb.tsv  --total_reads 9354510 -o libraries_3/WT_sgB_R2_sense_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl245_WT_sgB_R2_branch_nodsb.tsv  --total_reads 12461219 -o libraries_3/WT_sgB_R2_branch_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl246_WT_sgB_R2_cmv_nodsb.tsv  --total_reads 9853052 -o libraries_3/WT_sgB_R2_cmv_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl281_KO_sgB_R2_sense_nodsb.tsv  --total_reads 7181166 -o libraries_3/KO_sgB_R2_sense_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl282_KO_sgB_R2_branch_nodsb.tsv  --total_reads 10027116 -o libraries_3/KO_sgB_R2_branch_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl283_KO_sgB_R2_cmv_nodsb.tsv  --total_reads 7622513 -o libraries_3/KO_sgB_R2_cmv_nodsb.tsv --quiet </v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17935,10 +18185,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FB6E33-93C4-4971-BF44-23A0F65AADA0}">
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="A61" sqref="A61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21008,6 +21258,130 @@
         <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_cmv_nodsb</v>
       </c>
     </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" t="str">
+        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, M2:M41,M44:M55)</f>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgAB_R1_sense.tsv -o libraries_4/WT_sgAB_R1_sense -ref ref_seq/2DSB_R1_sense.fa -dsb 67 --dsb_type 2 --strand R1 --hguide AB --cell WT --treatment sense --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgAB_R1_branch.tsv -o libraries_4/WT_sgAB_R1_branch -ref ref_seq/2DSB_R1_branch.fa -dsb 67 --dsb_type 2 --strand R1 --hguide AB --cell WT --treatment branch --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgAB_R1_cmv.tsv -o libraries_4/WT_sgAB_R1_cmv -ref ref_seq/2DSB_R1_cmv.fa -dsb 67 --dsb_type 2 --strand R1 --hguide AB --cell WT --treatment cmv --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgAB_R1_sense.tsv -o libraries_4/KO_sgAB_R1_sense -ref ref_seq/2DSB_R1_sense.fa -dsb 67 --dsb_type 2 --strand R1 --hguide AB --cell KO --treatment sense --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgAB_R1_branch.tsv -o libraries_4/KO_sgAB_R1_branch -ref ref_seq/2DSB_R1_branch.fa -dsb 67 --dsb_type 2 --strand R1 --hguide AB --cell KO --treatment branch --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgAB_R1_cmv.tsv -o libraries_4/KO_sgAB_R1_cmv -ref ref_seq/2DSB_R1_cmv.fa -dsb 67 --dsb_type 2 --strand R1 --hguide AB --cell KO --treatment cmv --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgAB_R2_sense.tsv -o libraries_4/WT_sgAB_R2_sense -ref ref_seq/2DSB_R2_sense.fa -dsb 46 --dsb_type 2 --strand R2 --hguide AB --cell WT --treatment sense --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgAB_R2_branch.tsv -o libraries_4/WT_sgAB_R2_branch -ref ref_seq/2DSB_R2_branch.fa -dsb 46 --dsb_type 2 --strand R2 --hguide AB --cell WT --treatment branch --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgAB_R2_cmv.tsv -o libraries_4/WT_sgAB_R2_cmv -ref ref_seq/2DSB_R2_cmv.fa -dsb 46 --dsb_type 2 --strand R2 --hguide AB --cell WT --treatment cmv --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgAB_R2_sense.tsv -o libraries_4/KO_sgAB_R2_sense -ref ref_seq/2DSB_R2_sense.fa -dsb 46 --dsb_type 2 --strand R2 --hguide AB --cell KO --treatment sense --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgAB_R2_branch.tsv -o libraries_4/KO_sgAB_R2_branch -ref ref_seq/2DSB_R2_branch.fa -dsb 46 --dsb_type 2 --strand R2 --hguide AB --cell KO --treatment branch --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgAB_R2_cmv.tsv -o libraries_4/KO_sgAB_R2_cmv -ref ref_seq/2DSB_R2_cmv.fa -dsb 46 --dsb_type 2 --strand R2 --hguide AB --cell KO --treatment cmv --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_sense.tsv -o libraries_4/WT_sgA_R1_sense -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment sense --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_branch.tsv -o libraries_4/WT_sgA_R1_branch -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment branch --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_cmv.tsv -o libraries_4/WT_sgA_R1_cmv -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment cmv --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_sense.tsv -o libraries_4/KO_sgA_R1_sense -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment sense --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_branch.tsv -o libraries_4/KO_sgA_R1_branch -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment branch --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_cmv.tsv -o libraries_4/KO_sgA_R1_cmv -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment cmv --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_sense.tsv -o libraries_4/WT_sgB_R2_sense -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment sense --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_branch.tsv -o libraries_4/WT_sgB_R2_branch -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment branch --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_cmv.tsv -o libraries_4/WT_sgB_R2_cmv -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment cmv --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_sense.tsv -o libraries_4/KO_sgB_R2_sense -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment sense --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_branch.tsv -o libraries_4/KO_sgB_R2_branch -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment branch --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_cmv.tsv -o libraries_4/KO_sgB_R2_cmv -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment cmv --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_sense_30bpDown.tsv -o libraries_4/WT_sgA_R1_sense_30bpDown -ref ref_seq/1DSB_R1_sense.fa -dsb 97 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment sense --subst_type without --control 30bpDown
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_branch_30bpDown.tsv -o libraries_4/WT_sgA_R1_branch_30bpDown -ref ref_seq/1DSB_R1_branch.fa -dsb 97 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment branch --subst_type without --control 30bpDown
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_cmv_30bpDown.tsv -o libraries_4/WT_sgA_R1_cmv_30bpDown -ref ref_seq/1DSB_R1_cmv.fa -dsb 97 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment cmv --subst_type without --control 30bpDown
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_sense_30bpDown.tsv -o libraries_4/KO_sgA_R1_sense_30bpDown -ref ref_seq/1DSB_R1_sense.fa -dsb 97 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment sense --subst_type without --control 30bpDown
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_branch_30bpDown.tsv -o libraries_4/KO_sgA_R1_branch_30bpDown -ref ref_seq/1DSB_R1_branch.fa -dsb 97 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment branch --subst_type without --control 30bpDown
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_cmv_30bpDown.tsv -o libraries_4/KO_sgA_R1_cmv_30bpDown -ref ref_seq/1DSB_R1_cmv.fa -dsb 97 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment cmv --subst_type without --control 30bpDown
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_sense_30bpDown.tsv -o libraries_4/WT_sgB_R2_sense_30bpDown -ref ref_seq/1DSB_R2_sense.fa -dsb 76 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment sense --subst_type without --control 30bpDown
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_branch_30bpDown.tsv -o libraries_4/WT_sgB_R2_branch_30bpDown -ref ref_seq/1DSB_R2_branch.fa -dsb 76 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment branch --subst_type without --control 30bpDown
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_cmv_30bpDown.tsv -o libraries_4/WT_sgB_R2_cmv_30bpDown -ref ref_seq/1DSB_R2_cmv.fa -dsb 76 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment cmv --subst_type without --control 30bpDown
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_sense_30bpDown.tsv -o libraries_4/KO_sgB_R2_sense_30bpDown -ref ref_seq/1DSB_R2_sense.fa -dsb 76 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment sense --subst_type without --control 30bpDown
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_branch_30bpDown.tsv -o libraries_4/KO_sgB_R2_branch_30bpDown -ref ref_seq/1DSB_R2_branch.fa -dsb 76 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment branch --subst_type without --control 30bpDown
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_cmv_30bpDown.tsv -o libraries_4/KO_sgB_R2_cmv_30bpDown -ref ref_seq/1DSB_R2_cmv.fa -dsb 76 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment cmv --subst_type without --control 30bpDown
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R1_antisense.tsv -o libraries_4/WT_sgCD_R1_antisense -ref ref_seq/2DSBanti_R1_antisense.fa -dsb 50 --dsb_type 2a --strand R1 --hguide CD --cell WT --treatment antisense --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R1_splicing.tsv -o libraries_4/WT_sgCD_R1_splicing -ref ref_seq/2DSBanti_R1_splicing.fa -dsb 50 --dsb_type 2a --strand R1 --hguide CD --cell WT --treatment splicing --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R2_antisense.tsv -o libraries_4/WT_sgCD_R2_antisense -ref ref_seq/2DSBanti_R2_antisense.fa -dsb 47 --dsb_type 2a --strand R2 --hguide CD --cell WT --treatment antisense --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R2_splicing.tsv -o libraries_4/WT_sgCD_R2_splicing -ref ref_seq/2DSBanti_R2_splicing.fa -dsb 47 --dsb_type 2a --strand R2 --hguide CD --cell WT --treatment splicing --subst_type without --control none
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_sense_nodsb.tsv -o libraries_4/WT_sgA_R1_sense_nodsb -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment sense --subst_type without --control nodsb
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_branch_nodsb.tsv -o libraries_4/WT_sgA_R1_branch_nodsb -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment branch --subst_type without --control nodsb
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_cmv_nodsb.tsv -o libraries_4/WT_sgA_R1_cmv_nodsb -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment cmv --subst_type without --control nodsb
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_sense_nodsb.tsv -o libraries_4/KO_sgA_R1_sense_nodsb -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment sense --subst_type without --control nodsb
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_branch_nodsb.tsv -o libraries_4/KO_sgA_R1_branch_nodsb -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment branch --subst_type without --control nodsb
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_cmv_nodsb.tsv -o libraries_4/KO_sgA_R1_cmv_nodsb -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment cmv --subst_type without --control nodsb
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_sense_nodsb.tsv -o libraries_4/WT_sgB_R2_sense_nodsb -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment sense --subst_type without --control nodsb
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_branch_nodsb.tsv -o libraries_4/WT_sgB_R2_branch_nodsb -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment branch --subst_type without --control nodsb
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_cmv_nodsb.tsv -o libraries_4/WT_sgB_R2_cmv_nodsb -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment cmv --subst_type without --control nodsb
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_sense_nodsb.tsv -o libraries_4/KO_sgB_R2_sense_nodsb -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment sense --subst_type without --control nodsb
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_branch_nodsb.tsv -o libraries_4/KO_sgB_R2_branch_nodsb -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment branch --subst_type without --control nodsb
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_cmv_nodsb.tsv -o libraries_4/KO_sgB_R2_cmv_nodsb -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment cmv --subst_type without --control nodsb</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" t="str">
+        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, N2:N41,N44:N55)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgAB_R1_sense
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgAB_R1_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgAB_R1_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R1_sense
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R1_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R1_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgAB_R2_sense
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgAB_R2_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgAB_R2_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R2_sense
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R2_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R2_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_sense
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_sense
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_sense
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_sense
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_sense_30bpDown
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_branch_30bpDown
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_cmv_30bpDown
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_sense_30bpDown
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_branch_30bpDown
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_cmv_30bpDown
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_sense_30bpDown
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_branch_30bpDown
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_cmv_30bpDown
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_sense_30bpDown
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_branch_30bpDown
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_cmv_30bpDown
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgCD_R1_antisense
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgCD_R1_splicing
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgCD_R2_antisense
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgCD_R2_splicing
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_sense_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_branch_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_cmv_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_sense_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_branch_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_cmv_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_sense_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_branch_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_cmv_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_sense_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_branch_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_cmv_nodsb</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -21021,10 +21395,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AFDA2BA-58B9-4C12-83E9-7C389A51814A}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K33" sqref="K26:K33"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22327,6 +22701,78 @@
         <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_sense_cmv_nodsb</v>
       </c>
     </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="str">
+        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, J2:J17,J21:J22,J26:J33)</f>
+        <v>python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_branch -o libraries_4/WT_sgAB_R1_sense_branch --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R1_sense libraries_4/WT_sgAB_R1_cmv -o libraries_4/WT_sgAB_R1_sense_cmv --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_branch -o libraries_4/KO_sgAB_R1_sense_branch --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R1_sense libraries_4/KO_sgAB_R1_cmv -o libraries_4/KO_sgAB_R1_sense_cmv --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_branch -o libraries_4/WT_sgAB_R2_sense_branch --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgAB_R2_sense libraries_4/WT_sgAB_R2_cmv -o libraries_4/WT_sgAB_R2_sense_cmv --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_branch -o libraries_4/KO_sgAB_R2_sense_branch --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgAB_R2_sense libraries_4/KO_sgAB_R2_cmv -o libraries_4/KO_sgAB_R2_sense_cmv --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_branch -o libraries_4/WT_sgA_R1_sense_branch --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_R1_sense libraries_4/WT_sgA_R1_cmv -o libraries_4/WT_sgA_R1_sense_cmv --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_branch -o libraries_4/KO_sgA_R1_sense_branch --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_R1_sense libraries_4/KO_sgA_R1_cmv -o libraries_4/KO_sgA_R1_sense_cmv --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_branch -o libraries_4/WT_sgB_R2_sense_branch --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_R2_sense libraries_4/WT_sgB_R2_cmv -o libraries_4/WT_sgB_R2_sense_cmv --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_branch -o libraries_4/KO_sgB_R2_sense_branch --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_R2_sense libraries_4/KO_sgB_R2_cmv -o libraries_4/KO_sgB_R2_sense_cmv --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_R1_antisense libraries_4/WT_sgCD_R1_splicing -o libraries_4/WT_sgCD_R1_antisense_splicing --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgCD_R2_antisense libraries_4/WT_sgCD_R2_splicing -o libraries_4/WT_sgCD_R2_antisense_splicing --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_R1_sense_nodsb libraries_4/WT_sgA_R1_branch_nodsb -o libraries_4/WT_sgA_R1_sense_branch_nodsb --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgA_R1_sense_nodsb libraries_4/WT_sgA_R1_cmv_nodsb -o libraries_4/WT_sgA_R1_sense_cmv_nodsb --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_R1_sense_nodsb libraries_4/KO_sgA_R1_branch_nodsb -o libraries_4/KO_sgA_R1_sense_branch_nodsb --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgA_R1_sense_nodsb libraries_4/KO_sgA_R1_cmv_nodsb -o libraries_4/KO_sgA_R1_sense_cmv_nodsb --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_R2_sense_nodsb libraries_4/WT_sgB_R2_branch_nodsb -o libraries_4/WT_sgB_R2_sense_branch_nodsb --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/WT_sgB_R2_sense_nodsb libraries_4/WT_sgB_R2_cmv_nodsb -o libraries_4/WT_sgB_R2_sense_cmv_nodsb --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_R2_sense_nodsb libraries_4/KO_sgB_R2_branch_nodsb -o libraries_4/KO_sgB_R2_sense_branch_nodsb --subst_type without
+python 2_graph_processing/make_main_data_combined.py -i libraries_4/KO_sgB_R2_sense_nodsb libraries_4/KO_sgB_R2_cmv_nodsb -o libraries_4/KO_sgB_R2_sense_cmv_nodsb --subst_type without</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="str">
+        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, K2:K17,K21:K22,K26:K33)</f>
+        <v>python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgAB_R1_sense_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgAB_R1_sense_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R1_sense_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R1_sense_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgAB_R2_sense_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgAB_R2_sense_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R2_sense_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgAB_R2_sense_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_sense_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_sense_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_sense_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_sense_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_sense_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_sense_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_sense_branch
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_sense_cmv
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgCD_R1_antisense_splicing
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgCD_R2_antisense_splicing
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_sense_branch_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgA_R1_sense_cmv_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_sense_branch_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgA_R1_sense_cmv_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_sense_branch_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/WT_sgB_R2_sense_cmv_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_sense_branch_nodsb
+python 2_graph_processing/make_graph_data.py --subst_type without -dir libraries_4/KO_sgB_R2_sense_cmv_nodsb</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -22343,7 +22789,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCC207B-A9CD-4866-A17E-A3EE763F139F}">
   <dimension ref="A1:M58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A43" workbookViewId="0">
       <selection activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
@@ -25276,7 +25722,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1417E7-0E2A-4E67-94B4-4030BF5F7C23}">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -25653,7 +26099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix wrong directory in script.
</commit_message>
<xml_diff>
--- a/analyze_nhej/libinfo.xlsx
+++ b/analyze_nhej/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\analyze_nhej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AE94EBC-C2E5-44BA-964F-B18EB30A3E65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41892E74-79E0-4C6E-AD90-EE2CA8DD30C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="3" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -811,9 +811,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1500,6 +1497,12 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1875,9 +1878,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1990,44 +1990,44 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="98">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="97">
   <autoFilter ref="A1:M41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="13">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="97"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="96">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="96"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="95">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="95">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="94">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="94">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="93">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="93">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="92">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="92">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="91">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="91">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="90">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="90">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="89">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="89">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="88">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="88">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="87">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="87">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="86">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="86">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="85">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="85">
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="84">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2040,40 +2040,40 @@
   <autoFilter ref="A43:M55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
-    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="84">
+    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="83">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="83">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="82">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="82">
+    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="81">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="81">
+    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="80">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="80">
+    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="79">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="79">
+    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="78">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="78">
+    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="77">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="77">
+    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="76">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="76">
+    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="75">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="75">
+    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="74">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="74">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="73">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="73">
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="72">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2082,36 +2082,36 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="72">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="71">
   <autoFilter ref="A3:I4" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="71"/>
-    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="70">
+    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="70"/>
+    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="69">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="69">
+    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="68">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="68">
+    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="67">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="67">
+    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="66">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 12 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="33" xr3:uid="{8FF7E83A-9135-4A64-965C-48368A6C0367}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="66">
+    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="65">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="65">
+    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="64">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="64">
+    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="63">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2120,32 +2120,32 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="62">
   <autoFilter ref="A7:I9" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="62"/>
-    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="61">
+    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="61"/>
+    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="60">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="60">
+    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="59">
       <calculatedColumnFormula>IF(table_6_4[[#This Row],[hguide]]="A",NA(), IF(var_6_layout = "universal", "1 1 1 1 1 1", NA()))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="59">
+    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="58">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="58">
+    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="57">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" xr3:uid="{5BD83012-469D-4202-9584-AA182CDF11F9}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="57">
+    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="56">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="56">
+    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="55">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="55">
+    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="54">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2154,36 +2154,36 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="54" headerRowBorderDxfId="53" tableBorderDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="53" headerRowBorderDxfId="52" tableBorderDxfId="51">
   <autoFilter ref="A12:I13" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0F421990-E775-4F35-92AF-6BA19E0E8AEE}" name="index"/>
-    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="51">
+    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="50">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="50">
+    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="49">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0,4, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="49">
+    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="48">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="48">
+    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="47">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{E0783723-9246-4BF6-A5DA-E000EA1E5E87}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="47">
+    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="46">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="46">
+    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="45">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="45">
+    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="44">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2192,44 +2192,44 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:R42" totalsRowShown="0" headerRowDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:R42" totalsRowShown="0" headerRowDxfId="43">
   <autoFilter ref="A2:R42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="18">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="43"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="42">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="42"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="41">
       <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="41">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="40">
       <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="40">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="39">
       <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="39">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="38">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="38">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="37">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="37">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="36">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="36">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="35">
       <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="35">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="34">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="34">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="33">
       <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="33">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="32">
       <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="32">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="31">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="31">
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="30">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
       OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
       IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
@@ -2241,19 +2241,19 @@
       )
   )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="30">
+    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="29">
       <calculatedColumnFormula>AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="29">
+    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="28">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 13 --range_y -22 22 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 13 --range_y -18 25 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 13 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 13 --range_y -20 16 ", NA())))), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{891739FF-B093-4EE5-A0A2-20948C58CB96}" name="universal_layout_legend_pos_x" dataDxfId="28">
+    <tableColumn id="17" xr3:uid="{891739FF-B093-4EE5-A0A2-20948C58CB96}" name="universal_layout_legend_pos_x" dataDxfId="27">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 12, IF(table_7_1[[#This Row],[hguide]]="A", 12, IF(table_7_1[[#This Row],[hguide]]="B", 12, IF(table_7_1[[#This Row],[hguide]]="CD", 12, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="27">
+    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="26">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/individual/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="26">
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="25">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], IF(NOT(ISNA(table_7_1[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_1[[#This Row],[universal_layout_legend_pos_x]], "")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2262,38 +2262,38 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:K60" totalsRowShown="0" headerRowDxfId="25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:K60" totalsRowShown="0" headerRowDxfId="24">
   <autoFilter ref="A44:K60" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="23">
+    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="22">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="22">
+    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="21">
+    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="20">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="20">
+    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="19">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="19">
+    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="18">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="18">
+    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="17">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="17">
+    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="16">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_legend_pos_x" dataDxfId="16">
+    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_legend_pos_x" dataDxfId="15">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_legend_pos_x]:[universal_layout_legend_pos_x]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="15">
+    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="14">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="14">
+    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="13">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], IF(NOT(ISNA(table_7_2[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_2[[#This Row],[universal_layout_legend_pos_x]], "")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2302,38 +2302,38 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:K64" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:K64" totalsRowShown="0" headerRowDxfId="12">
   <autoFilter ref="A62:K64" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="10">
       <calculatedColumnFormula>OFFSET(table_4_2[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="10">
+    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="9">
+    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="8">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="8">
+    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="7">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="7">
+    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="6">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="6">
+    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="5">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="5">
+    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="4">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_legend_pos_x" dataDxfId="4">
+    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_legend_pos_x" dataDxfId="3">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_legend_pos_x]:[universal_layout_legend_pos_x]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="3">
+    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="2">
+    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], IF(NOT(ISNA(table_7_3[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_3[[#This Row],[universal_layout_legend_pos_x]], "")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2435,8 +2435,8 @@
     <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="174">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="173">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
+    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2447,41 +2447,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}" name="table_2_2" displayName="table_2_2" ref="A44:M56" totalsRowShown="0">
   <autoFilter ref="A44:M56" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="172"/>
-    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="171">
+    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="173"/>
+    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="172">
       <calculatedColumnFormula>OFFSET(table_1[ref], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="170">
+    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="171">
       <calculatedColumnFormula>OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="169">
+    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="170">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="168">
+    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="169">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="167">
+    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="168">
       <calculatedColumnFormula>OFFSET(table_1[cell], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="166">
+    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="167">
       <calculatedColumnFormula>OFFSET(table_1[strand], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="165">
+    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="166">
       <calculatedColumnFormula>OFFSET(table_1[treatment], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="164">
+    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="165">
       <calculatedColumnFormula>OFFSET(table_1[hguide], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="163">
+    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="164">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_2[[#This Row],[cell]], "_", table_2_2[[#This Row],[hguide]], "_", table_2_2[[#This Row],[strand]], "_", table_2_2[[#This Row],[treatment]], "_nodsb")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="162">
+    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="163">
       <calculatedColumnFormula>OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="161">
+    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="162">
       <calculatedColumnFormula>OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="160">
+    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="161">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2490,47 +2490,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="159">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="160">
   <autoFilter ref="A1:N41" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="158"/>
-    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="157">
+    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="159"/>
+    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="158">
       <calculatedColumnFormula>OFFSET(table_2_1[output_dir], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="156">
+    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="157">
       <calculatedColumnFormula>OFFSET(table_2_1[control], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="155">
+    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="156">
       <calculatedColumnFormula>OFFSET(table_2_1[ref], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="154">
+    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="155">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="153">
+    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="154">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="152">
+    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="153">
       <calculatedColumnFormula array="1">IF(table_3_1[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_1[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_1[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="151">
+    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="152">
       <calculatedColumnFormula>OFFSET(table_2_1[strand], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="150">
+    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="151">
       <calculatedColumnFormula>MID(OFFSET(table_2_1[hguide], table_3_1[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="149">
+    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="150">
       <calculatedColumnFormula>OFFSET(table_2_1[cell], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="148">
+    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="149">
       <calculatedColumnFormula>OFFSET(table_2_1[treatment], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DB6998A3-1431-4DDD-8DA0-525B805BF436}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="147">
+    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="148">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="146">
+    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="147">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2539,47 +2539,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="145">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="146">
   <autoFilter ref="A43:N55" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="144"/>
-    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="143">
+    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="145"/>
+    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="144">
       <calculatedColumnFormula>OFFSET(table_2_2[output_dir], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="142">
+    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="143">
       <calculatedColumnFormula>OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="141">
+    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="142">
       <calculatedColumnFormula>OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="140">
+    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="141">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_pos], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="139">
+    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="140">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_type], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="138">
+    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="139">
       <calculatedColumnFormula array="1">IF(table_3_2[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_2[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_2[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="137">
+    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="138">
       <calculatedColumnFormula>OFFSET(table_2_2[strand], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="136">
+    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="137">
       <calculatedColumnFormula>MID(OFFSET(table_2_2[hguide], table_3_2[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="135">
+    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="136">
       <calculatedColumnFormula>OFFSET(table_2_2[cell], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="134">
+    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="135">
       <calculatedColumnFormula>OFFSET(table_2_2[treatment], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{142C480D-E258-4979-A008-3940A3FE78E4}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="133">
+    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="134">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="132">
+    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="133">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2588,38 +2588,38 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="131">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="132">
   <autoFilter ref="A1:K17" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="130"/>
-    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="129">
+    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="131"/>
+    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="130">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="128">
+    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="129">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="127">
+    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="128">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="126">
+    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="127">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="125">
+    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="126">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="124">
+    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="125">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_1[[#This Row],[treatment_1]], "_", table_4_1[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="123">
+    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="124">
       <calculatedColumnFormula>SUBSTITUTE(table_4_1[[#This Row],[dir_1]], table_4_1[[#This Row],[treatment_1]], table_4_1[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="122">
+    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="123">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="121">
+    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="122">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_1[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_1[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_1[[#This Row],[dir_out]], " --subst_type ", table_4_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="120">
+    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="121">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_1[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2628,38 +2628,38 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="120">
   <autoFilter ref="A20:K22" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="118"/>
-    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="117">
+    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="119"/>
+    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="118">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_4_anti_offset + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="116">
+    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="117">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="1">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="116">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="115">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="0">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="114">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="114">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="113">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_2[[#This Row],[treatment_1]], "_", table_4_2[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="113">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="112">
       <calculatedColumnFormula>SUBSTITUTE(table_4_2[[#This Row],[dir_1]], table_4_2[[#This Row],[treatment_1]], table_4_2[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="112">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="111">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_2[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_2[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_2[[#This Row],[dir_out]], " --subst_type ", table_4_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="111">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="110">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_2[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2668,38 +2668,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="109">
   <autoFilter ref="A25:K33" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="109"/>
-    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="108">
+    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="108"/>
+    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="107">
       <calculatedColumnFormula>OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="107">
+    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="106">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="106">
+    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="105">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="105">
+    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="104">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="104">
+    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="103">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="103">
+    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="102">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_3[[#This Row],[treatment_1]], "_", table_4_3[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="102">
+    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="101">
       <calculatedColumnFormula>SUBSTITUTE(table_4_3[[#This Row],[dir_1]], table_4_3[[#This Row],[treatment_1]], table_4_3[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="101">
+    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="100">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="100">
+    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="99">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_3[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_3[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_3[[#This Row],[dir_out]], " --subst_type ", table_4_3[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="99">
+    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="98">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_3[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_3[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -14266,7 +14266,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D704B5-D01A-4D17-9252-416EA08BC871}">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView topLeftCell="H43" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H46" workbookViewId="0">
       <selection activeCell="H59" sqref="H59"/>
     </sheetView>
   </sheetViews>
@@ -14418,8 +14418,8 @@
         <v>7513691</v>
       </c>
       <c r="S2" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl217_WT_sgAB_R1_sense.tsv libraries_2/yjl218_WT_sgAB_R1_sense.tsv libraries_2/yjl219_WT_sgAB_R1_sense.tsv libraries_4/yjl220_WT_sgAB_R1_sense.tsv --total_reads 6630053 7246619 8069391 7513691 -o libraries_3/WT_sgAB_R1_sense.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl217_WT_sgAB_R1_sense.tsv libraries_2/yjl218_WT_sgAB_R1_sense.tsv libraries_2/yjl219_WT_sgAB_R1_sense.tsv libraries_2/yjl220_WT_sgAB_R1_sense.tsv --total_reads 6630053 7246619 8069391 7513691 -o libraries_3/WT_sgAB_R1_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -14495,8 +14495,8 @@
         <v>9192054</v>
       </c>
       <c r="S3" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl221_WT_sgAB_R1_branch.tsv libraries_2/yjl222_WT_sgAB_R1_branch.tsv libraries_2/yjl223_WT_sgAB_R1_branch.tsv libraries_4/yjl224_WT_sgAB_R1_branch.tsv --total_reads 9021462 9430938 9051278 9192054 -o libraries_3/WT_sgAB_R1_branch.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl221_WT_sgAB_R1_branch.tsv libraries_2/yjl222_WT_sgAB_R1_branch.tsv libraries_2/yjl223_WT_sgAB_R1_branch.tsv libraries_2/yjl224_WT_sgAB_R1_branch.tsv --total_reads 9021462 9430938 9051278 9192054 -o libraries_3/WT_sgAB_R1_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
@@ -14572,8 +14572,8 @@
         <v>7694818</v>
       </c>
       <c r="S4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl225_WT_sgAB_R1_cmv.tsv libraries_2/yjl226_WT_sgAB_R1_cmv.tsv libraries_2/yjl227_WT_sgAB_R1_cmv.tsv libraries_4/yjl228_WT_sgAB_R1_cmv.tsv --total_reads 7604379 8885716 8150455 7694818 -o libraries_3/WT_sgAB_R1_cmv.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl225_WT_sgAB_R1_cmv.tsv libraries_2/yjl226_WT_sgAB_R1_cmv.tsv libraries_2/yjl227_WT_sgAB_R1_cmv.tsv libraries_2/yjl228_WT_sgAB_R1_cmv.tsv --total_reads 7604379 8885716 8150455 7694818 -o libraries_3/WT_sgAB_R1_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
@@ -14649,8 +14649,8 @@
         <v>12479012</v>
       </c>
       <c r="S5" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl229_KO_sgAB_R1_sense.tsv libraries_2/yjl230_KO_sgAB_R1_sense.tsv libraries_2/yjl231_KO_sgAB_R1_sense.tsv libraries_4/yjl232_KO_sgAB_R1_sense.tsv --total_reads 11320509 12480734 12500966 12479012 -o libraries_3/KO_sgAB_R1_sense.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl229_KO_sgAB_R1_sense.tsv libraries_2/yjl230_KO_sgAB_R1_sense.tsv libraries_2/yjl231_KO_sgAB_R1_sense.tsv libraries_2/yjl232_KO_sgAB_R1_sense.tsv --total_reads 11320509 12480734 12500966 12479012 -o libraries_3/KO_sgAB_R1_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
@@ -14726,8 +14726,8 @@
         <v>13493608</v>
       </c>
       <c r="S6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl233_KO_sgAB_R1_branch.tsv libraries_2/yjl234_KO_sgAB_R1_branch.tsv libraries_2/yjl235_KO_sgAB_R1_branch.tsv libraries_4/yjl236_KO_sgAB_R1_branch.tsv --total_reads 13912975 15839537 13872702 13493608 -o libraries_3/KO_sgAB_R1_branch.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl233_KO_sgAB_R1_branch.tsv libraries_2/yjl234_KO_sgAB_R1_branch.tsv libraries_2/yjl235_KO_sgAB_R1_branch.tsv libraries_2/yjl236_KO_sgAB_R1_branch.tsv --total_reads 13912975 15839537 13872702 13493608 -o libraries_3/KO_sgAB_R1_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
@@ -14803,8 +14803,8 @@
         <v>9412394</v>
       </c>
       <c r="S7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl237_KO_sgAB_R1_cmv.tsv libraries_2/yjl238_KO_sgAB_R1_cmv.tsv libraries_2/yjl239_KO_sgAB_R1_cmv.tsv libraries_4/yjl240_KO_sgAB_R1_cmv.tsv --total_reads 11307677 11757615 10272339 9412394 -o libraries_3/KO_sgAB_R1_cmv.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl237_KO_sgAB_R1_cmv.tsv libraries_2/yjl238_KO_sgAB_R1_cmv.tsv libraries_2/yjl239_KO_sgAB_R1_cmv.tsv libraries_2/yjl240_KO_sgAB_R1_cmv.tsv --total_reads 11307677 11757615 10272339 9412394 -o libraries_3/KO_sgAB_R1_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
@@ -14880,8 +14880,8 @@
         <v>7001340</v>
       </c>
       <c r="S8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl217_WT_sgAB_R2_sense.tsv libraries_2/yjl218_WT_sgAB_R2_sense.tsv libraries_2/yjl219_WT_sgAB_R2_sense.tsv libraries_4/yjl220_WT_sgAB_R2_sense.tsv --total_reads 6177083 6744517 7507107 7001340 -o libraries_3/WT_sgAB_R2_sense.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl217_WT_sgAB_R2_sense.tsv libraries_2/yjl218_WT_sgAB_R2_sense.tsv libraries_2/yjl219_WT_sgAB_R2_sense.tsv libraries_2/yjl220_WT_sgAB_R2_sense.tsv --total_reads 6177083 6744517 7507107 7001340 -o libraries_3/WT_sgAB_R2_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
@@ -14957,8 +14957,8 @@
         <v>8656502</v>
       </c>
       <c r="S9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl221_WT_sgAB_R2_branch.tsv libraries_2/yjl222_WT_sgAB_R2_branch.tsv libraries_2/yjl223_WT_sgAB_R2_branch.tsv libraries_4/yjl224_WT_sgAB_R2_branch.tsv --total_reads 8525251 8875435 8522228 8656502 -o libraries_3/WT_sgAB_R2_branch.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl221_WT_sgAB_R2_branch.tsv libraries_2/yjl222_WT_sgAB_R2_branch.tsv libraries_2/yjl223_WT_sgAB_R2_branch.tsv libraries_2/yjl224_WT_sgAB_R2_branch.tsv --total_reads 8525251 8875435 8522228 8656502 -o libraries_3/WT_sgAB_R2_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
@@ -15034,8 +15034,8 @@
         <v>6940576</v>
       </c>
       <c r="S10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl225_WT_sgAB_R2_cmv.tsv libraries_2/yjl226_WT_sgAB_R2_cmv.tsv libraries_2/yjl227_WT_sgAB_R2_cmv.tsv libraries_4/yjl228_WT_sgAB_R2_cmv.tsv --total_reads 6898791 7986453 7354088 6940576 -o libraries_3/WT_sgAB_R2_cmv.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl225_WT_sgAB_R2_cmv.tsv libraries_2/yjl226_WT_sgAB_R2_cmv.tsv libraries_2/yjl227_WT_sgAB_R2_cmv.tsv libraries_2/yjl228_WT_sgAB_R2_cmv.tsv --total_reads 6898791 7986453 7354088 6940576 -o libraries_3/WT_sgAB_R2_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
@@ -15111,8 +15111,8 @@
         <v>11080481</v>
       </c>
       <c r="S11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl229_KO_sgAB_R2_sense.tsv libraries_2/yjl230_KO_sgAB_R2_sense.tsv libraries_2/yjl231_KO_sgAB_R2_sense.tsv libraries_4/yjl232_KO_sgAB_R2_sense.tsv --total_reads 10142826 11211467 11130391 11080481 -o libraries_3/KO_sgAB_R2_sense.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl229_KO_sgAB_R2_sense.tsv libraries_2/yjl230_KO_sgAB_R2_sense.tsv libraries_2/yjl231_KO_sgAB_R2_sense.tsv libraries_2/yjl232_KO_sgAB_R2_sense.tsv --total_reads 10142826 11211467 11130391 11080481 -o libraries_3/KO_sgAB_R2_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
@@ -15188,8 +15188,8 @@
         <v>12582077</v>
       </c>
       <c r="S12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl233_KO_sgAB_R2_branch.tsv libraries_2/yjl234_KO_sgAB_R2_branch.tsv libraries_2/yjl235_KO_sgAB_R2_branch.tsv libraries_4/yjl236_KO_sgAB_R2_branch.tsv --total_reads 12987477 14745821 12946604 12582077 -o libraries_3/KO_sgAB_R2_branch.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl233_KO_sgAB_R2_branch.tsv libraries_2/yjl234_KO_sgAB_R2_branch.tsv libraries_2/yjl235_KO_sgAB_R2_branch.tsv libraries_2/yjl236_KO_sgAB_R2_branch.tsv --total_reads 12987477 14745821 12946604 12582077 -o libraries_3/KO_sgAB_R2_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
@@ -15265,8 +15265,8 @@
         <v>8729797</v>
       </c>
       <c r="S13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl237_KO_sgAB_R2_cmv.tsv libraries_2/yjl238_KO_sgAB_R2_cmv.tsv libraries_2/yjl239_KO_sgAB_R2_cmv.tsv libraries_4/yjl240_KO_sgAB_R2_cmv.tsv --total_reads 10562895 10985096 9559721 8729797 -o libraries_3/KO_sgAB_R2_cmv.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl237_KO_sgAB_R2_cmv.tsv libraries_2/yjl238_KO_sgAB_R2_cmv.tsv libraries_2/yjl239_KO_sgAB_R2_cmv.tsv libraries_2/yjl240_KO_sgAB_R2_cmv.tsv --total_reads 10562895 10985096 9559721 8729797 -o libraries_3/KO_sgAB_R2_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
@@ -15342,8 +15342,8 @@
         <v>7534924</v>
       </c>
       <c r="S14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl255_WT_sgA_R1_sense.tsv libraries_2/yjl256_WT_sgA_R1_sense.tsv libraries_2/yjl257_WT_sgA_R1_sense.tsv libraries_4/yjl258_WT_sgA_R1_sense.tsv --total_reads 7579965 7982725 7854740 7534924 -o libraries_3/WT_sgA_R1_sense.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl255_WT_sgA_R1_sense.tsv libraries_2/yjl256_WT_sgA_R1_sense.tsv libraries_2/yjl257_WT_sgA_R1_sense.tsv libraries_2/yjl258_WT_sgA_R1_sense.tsv --total_reads 7579965 7982725 7854740 7534924 -o libraries_3/WT_sgA_R1_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
@@ -15419,8 +15419,8 @@
         <v>8799841</v>
       </c>
       <c r="S15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl259_WT_sgA_R1_branch.tsv libraries_2/yjl260_WT_sgA_R1_branch.tsv libraries_2/yjl261_WT_sgA_R1_branch.tsv libraries_4/yjl262_WT_sgA_R1_branch.tsv --total_reads 8808358 9297647 9399483 8799841 -o libraries_3/WT_sgA_R1_branch.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl259_WT_sgA_R1_branch.tsv libraries_2/yjl260_WT_sgA_R1_branch.tsv libraries_2/yjl261_WT_sgA_R1_branch.tsv libraries_2/yjl262_WT_sgA_R1_branch.tsv --total_reads 8808358 9297647 9399483 8799841 -o libraries_3/WT_sgA_R1_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
@@ -15496,8 +15496,8 @@
         <v>8096639</v>
       </c>
       <c r="S16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl263_WT_sgA_R1_cmv.tsv libraries_2/yjl264_WT_sgA_R1_cmv.tsv libraries_2/yjl265_WT_sgA_R1_cmv.tsv libraries_4/yjl266_WT_sgA_R1_cmv.tsv --total_reads 8171224 8180897 8314116 8096639 -o libraries_3/WT_sgA_R1_cmv.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl263_WT_sgA_R1_cmv.tsv libraries_2/yjl264_WT_sgA_R1_cmv.tsv libraries_2/yjl265_WT_sgA_R1_cmv.tsv libraries_2/yjl266_WT_sgA_R1_cmv.tsv --total_reads 8171224 8180897 8314116 8096639 -o libraries_3/WT_sgA_R1_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
@@ -15573,8 +15573,8 @@
         <v>9021103</v>
       </c>
       <c r="S17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl292_KO_sgA_R1_sense.tsv libraries_2/yjl293_KO_sgA_R1_sense.tsv libraries_2/yjl294_KO_sgA_R1_sense.tsv libraries_4/yjl295_KO_sgA_R1_sense.tsv --total_reads 8597510 10116623 8703707 9021103 -o libraries_3/KO_sgA_R1_sense.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl292_KO_sgA_R1_sense.tsv libraries_2/yjl293_KO_sgA_R1_sense.tsv libraries_2/yjl294_KO_sgA_R1_sense.tsv libraries_2/yjl295_KO_sgA_R1_sense.tsv --total_reads 8597510 10116623 8703707 9021103 -o libraries_3/KO_sgA_R1_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
@@ -15650,8 +15650,8 @@
         <v>11659042</v>
       </c>
       <c r="S18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl296_KO_sgA_R1_branch.tsv libraries_2/yjl297_KO_sgA_R1_branch.tsv libraries_2/yjl298_KO_sgA_R1_branch.tsv libraries_4/yjl299_KO_sgA_R1_branch.tsv --total_reads 11021111 11280773 12426852 11659042 -o libraries_3/KO_sgA_R1_branch.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl296_KO_sgA_R1_branch.tsv libraries_2/yjl297_KO_sgA_R1_branch.tsv libraries_2/yjl298_KO_sgA_R1_branch.tsv libraries_2/yjl299_KO_sgA_R1_branch.tsv --total_reads 11021111 11280773 12426852 11659042 -o libraries_3/KO_sgA_R1_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
@@ -15727,8 +15727,8 @@
         <v>8668198</v>
       </c>
       <c r="S19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl300_KO_sgA_R1_cmv.tsv libraries_2/yjl301_KO_sgA_R1_cmv.tsv libraries_2/yjl302_KO_sgA_R1_cmv.tsv libraries_4/yjl303_KO_sgA_R1_cmv.tsv --total_reads 9933546 10351309 9388188 8668198 -o libraries_3/KO_sgA_R1_cmv.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl300_KO_sgA_R1_cmv.tsv libraries_2/yjl301_KO_sgA_R1_cmv.tsv libraries_2/yjl302_KO_sgA_R1_cmv.tsv libraries_2/yjl303_KO_sgA_R1_cmv.tsv --total_reads 9933546 10351309 9388188 8668198 -o libraries_3/KO_sgA_R1_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
@@ -15804,8 +15804,8 @@
         <v>7238408</v>
       </c>
       <c r="S20" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl267_WT_sgB_R2_sense.tsv libraries_2/yjl268_WT_sgB_R2_sense.tsv libraries_2/yjl269_WT_sgB_R2_sense.tsv libraries_4/yjl270_WT_sgB_R2_sense.tsv --total_reads 7137355 6618133 8227882 7238408 -o libraries_3/WT_sgB_R2_sense.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl267_WT_sgB_R2_sense.tsv libraries_2/yjl268_WT_sgB_R2_sense.tsv libraries_2/yjl269_WT_sgB_R2_sense.tsv libraries_2/yjl270_WT_sgB_R2_sense.tsv --total_reads 7137355 6618133 8227882 7238408 -o libraries_3/WT_sgB_R2_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
@@ -15881,8 +15881,8 @@
         <v>9525100</v>
       </c>
       <c r="S21" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl271_WT_sgB_R2_branch.tsv libraries_2/yjl272_WT_sgB_R2_branch.tsv libraries_2/yjl273_WT_sgB_R2_branch.tsv libraries_4/yjl274_WT_sgB_R2_branch.tsv --total_reads 9524548 10125834 10173904 9525100 -o libraries_3/WT_sgB_R2_branch.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl271_WT_sgB_R2_branch.tsv libraries_2/yjl272_WT_sgB_R2_branch.tsv libraries_2/yjl273_WT_sgB_R2_branch.tsv libraries_2/yjl274_WT_sgB_R2_branch.tsv --total_reads 9524548 10125834 10173904 9525100 -o libraries_3/WT_sgB_R2_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
@@ -15958,8 +15958,8 @@
         <v>7081713</v>
       </c>
       <c r="S22" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl275_WT_sgB_R2_cmv.tsv libraries_2/yjl276_WT_sgB_R2_cmv.tsv libraries_2/yjl277_WT_sgB_R2_cmv.tsv libraries_4/yjl278_WT_sgB_R2_cmv.tsv --total_reads 7280860 6872217 6847531 7081713 -o libraries_3/WT_sgB_R2_cmv.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl275_WT_sgB_R2_cmv.tsv libraries_2/yjl276_WT_sgB_R2_cmv.tsv libraries_2/yjl277_WT_sgB_R2_cmv.tsv libraries_2/yjl278_WT_sgB_R2_cmv.tsv --total_reads 7280860 6872217 6847531 7081713 -o libraries_3/WT_sgB_R2_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
@@ -16035,8 +16035,8 @@
         <v>6545416</v>
       </c>
       <c r="S23" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl304_KO_sgB_R2_sense.tsv libraries_2/yjl305_KO_sgB_R2_sense.tsv libraries_2/yjl306_KO_sgB_R2_sense.tsv libraries_4/yjl307_KO_sgB_R2_sense.tsv --total_reads 6494964 7011524 7131423 6545416 -o libraries_3/KO_sgB_R2_sense.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl304_KO_sgB_R2_sense.tsv libraries_2/yjl305_KO_sgB_R2_sense.tsv libraries_2/yjl306_KO_sgB_R2_sense.tsv libraries_2/yjl307_KO_sgB_R2_sense.tsv --total_reads 6494964 7011524 7131423 6545416 -o libraries_3/KO_sgB_R2_sense.tsv --quiet </v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
@@ -16112,8 +16112,8 @@
         <v>10249893</v>
       </c>
       <c r="S24" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl308_KO_sgB_R2_branch.tsv libraries_2/yjl309_KO_sgB_R2_branch.tsv libraries_2/yjl310_KO_sgB_R2_branch.tsv libraries_4/yjl311_KO_sgB_R2_branch.tsv --total_reads 9730255 10430885 9770845 10249893 -o libraries_3/KO_sgB_R2_branch.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl308_KO_sgB_R2_branch.tsv libraries_2/yjl309_KO_sgB_R2_branch.tsv libraries_2/yjl310_KO_sgB_R2_branch.tsv libraries_2/yjl311_KO_sgB_R2_branch.tsv --total_reads 9730255 10430885 9770845 10249893 -o libraries_3/KO_sgB_R2_branch.tsv --quiet </v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
@@ -16189,8 +16189,8 @@
         <v>6372479</v>
       </c>
       <c r="S25" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl312_KO_sgB_R2_cmv.tsv libraries_2/yjl313_KO_sgB_R2_cmv.tsv libraries_2/yjl314_KO_sgB_R2_cmv.tsv libraries_4/yjl315_KO_sgB_R2_cmv.tsv --total_reads 6718301 6435913 7285831 6372479 -o libraries_3/KO_sgB_R2_cmv.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl312_KO_sgB_R2_cmv.tsv libraries_2/yjl313_KO_sgB_R2_cmv.tsv libraries_2/yjl314_KO_sgB_R2_cmv.tsv libraries_2/yjl315_KO_sgB_R2_cmv.tsv --total_reads 6718301 6435913 7285831 6372479 -o libraries_3/KO_sgB_R2_cmv.tsv --quiet </v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
@@ -16266,8 +16266,8 @@
         <v>7534924</v>
       </c>
       <c r="S26" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl255_WT_sgA_R1_sense_30bpDown.tsv libraries_2/yjl256_WT_sgA_R1_sense_30bpDown.tsv libraries_2/yjl257_WT_sgA_R1_sense_30bpDown.tsv libraries_4/yjl258_WT_sgA_R1_sense_30bpDown.tsv --total_reads 7579965 7982725 7854740 7534924 -o libraries_3/WT_sgA_R1_sense_30bpDown.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl255_WT_sgA_R1_sense_30bpDown.tsv libraries_2/yjl256_WT_sgA_R1_sense_30bpDown.tsv libraries_2/yjl257_WT_sgA_R1_sense_30bpDown.tsv libraries_2/yjl258_WT_sgA_R1_sense_30bpDown.tsv --total_reads 7579965 7982725 7854740 7534924 -o libraries_3/WT_sgA_R1_sense_30bpDown.tsv --quiet </v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
@@ -16343,8 +16343,8 @@
         <v>8799841</v>
       </c>
       <c r="S27" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl259_WT_sgA_R1_branch_30bpDown.tsv libraries_2/yjl260_WT_sgA_R1_branch_30bpDown.tsv libraries_2/yjl261_WT_sgA_R1_branch_30bpDown.tsv libraries_4/yjl262_WT_sgA_R1_branch_30bpDown.tsv --total_reads 8808358 9297647 9399483 8799841 -o libraries_3/WT_sgA_R1_branch_30bpDown.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl259_WT_sgA_R1_branch_30bpDown.tsv libraries_2/yjl260_WT_sgA_R1_branch_30bpDown.tsv libraries_2/yjl261_WT_sgA_R1_branch_30bpDown.tsv libraries_2/yjl262_WT_sgA_R1_branch_30bpDown.tsv --total_reads 8808358 9297647 9399483 8799841 -o libraries_3/WT_sgA_R1_branch_30bpDown.tsv --quiet </v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
@@ -16420,8 +16420,8 @@
         <v>8096639</v>
       </c>
       <c r="S28" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl263_WT_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl264_WT_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl265_WT_sgA_R1_cmv_30bpDown.tsv libraries_4/yjl266_WT_sgA_R1_cmv_30bpDown.tsv --total_reads 8171224 8180897 8314116 8096639 -o libraries_3/WT_sgA_R1_cmv_30bpDown.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl263_WT_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl264_WT_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl265_WT_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl266_WT_sgA_R1_cmv_30bpDown.tsv --total_reads 8171224 8180897 8314116 8096639 -o libraries_3/WT_sgA_R1_cmv_30bpDown.tsv --quiet </v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
@@ -16497,8 +16497,8 @@
         <v>9021103</v>
       </c>
       <c r="S29" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl292_KO_sgA_R1_sense_30bpDown.tsv libraries_2/yjl293_KO_sgA_R1_sense_30bpDown.tsv libraries_2/yjl294_KO_sgA_R1_sense_30bpDown.tsv libraries_4/yjl295_KO_sgA_R1_sense_30bpDown.tsv --total_reads 8597510 10116623 8703707 9021103 -o libraries_3/KO_sgA_R1_sense_30bpDown.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl292_KO_sgA_R1_sense_30bpDown.tsv libraries_2/yjl293_KO_sgA_R1_sense_30bpDown.tsv libraries_2/yjl294_KO_sgA_R1_sense_30bpDown.tsv libraries_2/yjl295_KO_sgA_R1_sense_30bpDown.tsv --total_reads 8597510 10116623 8703707 9021103 -o libraries_3/KO_sgA_R1_sense_30bpDown.tsv --quiet </v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
@@ -16574,8 +16574,8 @@
         <v>11659042</v>
       </c>
       <c r="S30" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl296_KO_sgA_R1_branch_30bpDown.tsv libraries_2/yjl297_KO_sgA_R1_branch_30bpDown.tsv libraries_2/yjl298_KO_sgA_R1_branch_30bpDown.tsv libraries_4/yjl299_KO_sgA_R1_branch_30bpDown.tsv --total_reads 11021111 11280773 12426852 11659042 -o libraries_3/KO_sgA_R1_branch_30bpDown.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl296_KO_sgA_R1_branch_30bpDown.tsv libraries_2/yjl297_KO_sgA_R1_branch_30bpDown.tsv libraries_2/yjl298_KO_sgA_R1_branch_30bpDown.tsv libraries_2/yjl299_KO_sgA_R1_branch_30bpDown.tsv --total_reads 11021111 11280773 12426852 11659042 -o libraries_3/KO_sgA_R1_branch_30bpDown.tsv --quiet </v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
@@ -16651,8 +16651,8 @@
         <v>8668198</v>
       </c>
       <c r="S31" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl300_KO_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl301_KO_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl302_KO_sgA_R1_cmv_30bpDown.tsv libraries_4/yjl303_KO_sgA_R1_cmv_30bpDown.tsv --total_reads 9933546 10351309 9388188 8668198 -o libraries_3/KO_sgA_R1_cmv_30bpDown.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl300_KO_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl301_KO_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl302_KO_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl303_KO_sgA_R1_cmv_30bpDown.tsv --total_reads 9933546 10351309 9388188 8668198 -o libraries_3/KO_sgA_R1_cmv_30bpDown.tsv --quiet </v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
@@ -16728,8 +16728,8 @@
         <v>7238408</v>
       </c>
       <c r="S32" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl267_WT_sgB_R2_sense_30bpDown.tsv libraries_2/yjl268_WT_sgB_R2_sense_30bpDown.tsv libraries_2/yjl269_WT_sgB_R2_sense_30bpDown.tsv libraries_4/yjl270_WT_sgB_R2_sense_30bpDown.tsv --total_reads 7137355 6618133 8227882 7238408 -o libraries_3/WT_sgB_R2_sense_30bpDown.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl267_WT_sgB_R2_sense_30bpDown.tsv libraries_2/yjl268_WT_sgB_R2_sense_30bpDown.tsv libraries_2/yjl269_WT_sgB_R2_sense_30bpDown.tsv libraries_2/yjl270_WT_sgB_R2_sense_30bpDown.tsv --total_reads 7137355 6618133 8227882 7238408 -o libraries_3/WT_sgB_R2_sense_30bpDown.tsv --quiet </v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
@@ -16805,8 +16805,8 @@
         <v>9525100</v>
       </c>
       <c r="S33" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl271_WT_sgB_R2_branch_30bpDown.tsv libraries_2/yjl272_WT_sgB_R2_branch_30bpDown.tsv libraries_2/yjl273_WT_sgB_R2_branch_30bpDown.tsv libraries_4/yjl274_WT_sgB_R2_branch_30bpDown.tsv --total_reads 9524548 10125834 10173904 9525100 -o libraries_3/WT_sgB_R2_branch_30bpDown.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl271_WT_sgB_R2_branch_30bpDown.tsv libraries_2/yjl272_WT_sgB_R2_branch_30bpDown.tsv libraries_2/yjl273_WT_sgB_R2_branch_30bpDown.tsv libraries_2/yjl274_WT_sgB_R2_branch_30bpDown.tsv --total_reads 9524548 10125834 10173904 9525100 -o libraries_3/WT_sgB_R2_branch_30bpDown.tsv --quiet </v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
@@ -16882,8 +16882,8 @@
         <v>7081713</v>
       </c>
       <c r="S34" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl275_WT_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl276_WT_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl277_WT_sgB_R2_cmv_30bpDown.tsv libraries_4/yjl278_WT_sgB_R2_cmv_30bpDown.tsv --total_reads 7280860 6872217 6847531 7081713 -o libraries_3/WT_sgB_R2_cmv_30bpDown.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl275_WT_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl276_WT_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl277_WT_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl278_WT_sgB_R2_cmv_30bpDown.tsv --total_reads 7280860 6872217 6847531 7081713 -o libraries_3/WT_sgB_R2_cmv_30bpDown.tsv --quiet </v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -16959,8 +16959,8 @@
         <v>6545416</v>
       </c>
       <c r="S35" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl304_KO_sgB_R2_sense_30bpDown.tsv libraries_2/yjl305_KO_sgB_R2_sense_30bpDown.tsv libraries_2/yjl306_KO_sgB_R2_sense_30bpDown.tsv libraries_4/yjl307_KO_sgB_R2_sense_30bpDown.tsv --total_reads 6494964 7011524 7131423 6545416 -o libraries_3/KO_sgB_R2_sense_30bpDown.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl304_KO_sgB_R2_sense_30bpDown.tsv libraries_2/yjl305_KO_sgB_R2_sense_30bpDown.tsv libraries_2/yjl306_KO_sgB_R2_sense_30bpDown.tsv libraries_2/yjl307_KO_sgB_R2_sense_30bpDown.tsv --total_reads 6494964 7011524 7131423 6545416 -o libraries_3/KO_sgB_R2_sense_30bpDown.tsv --quiet </v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
@@ -17036,8 +17036,8 @@
         <v>10249893</v>
       </c>
       <c r="S36" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl308_KO_sgB_R2_branch_30bpDown.tsv libraries_2/yjl309_KO_sgB_R2_branch_30bpDown.tsv libraries_2/yjl310_KO_sgB_R2_branch_30bpDown.tsv libraries_4/yjl311_KO_sgB_R2_branch_30bpDown.tsv --total_reads 9730255 10430885 9770845 10249893 -o libraries_3/KO_sgB_R2_branch_30bpDown.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl308_KO_sgB_R2_branch_30bpDown.tsv libraries_2/yjl309_KO_sgB_R2_branch_30bpDown.tsv libraries_2/yjl310_KO_sgB_R2_branch_30bpDown.tsv libraries_2/yjl311_KO_sgB_R2_branch_30bpDown.tsv --total_reads 9730255 10430885 9770845 10249893 -o libraries_3/KO_sgB_R2_branch_30bpDown.tsv --quiet </v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
@@ -17113,8 +17113,8 @@
         <v>6372479</v>
       </c>
       <c r="S37" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl312_KO_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl313_KO_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl314_KO_sgB_R2_cmv_30bpDown.tsv libraries_4/yjl315_KO_sgB_R2_cmv_30bpDown.tsv --total_reads 6718301 6435913 7285831 6372479 -o libraries_3/KO_sgB_R2_cmv_30bpDown.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl312_KO_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl313_KO_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl314_KO_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl315_KO_sgB_R2_cmv_30bpDown.tsv --total_reads 6718301 6435913 7285831 6372479 -o libraries_3/KO_sgB_R2_cmv_30bpDown.tsv --quiet </v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
@@ -17190,8 +17190,8 @@
         <v>6586577</v>
       </c>
       <c r="S38" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl89_WT_sgCD_R1_antisense.tsv libraries_2/yjl90_WT_sgCD_R1_antisense.tsv libraries_2/yjl91_WT_sgCD_R1_antisense.tsv libraries_4/yjl92_WT_sgCD_R1_antisense.tsv --total_reads 7813781 7486736 8114856 6586577 -o libraries_3/WT_sgCD_R1_antisense.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl89_WT_sgCD_R1_antisense.tsv libraries_2/yjl90_WT_sgCD_R1_antisense.tsv libraries_2/yjl91_WT_sgCD_R1_antisense.tsv libraries_2/yjl92_WT_sgCD_R1_antisense.tsv --total_reads 7813781 7486736 8114856 6586577 -o libraries_3/WT_sgCD_R1_antisense.tsv --quiet </v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -17267,8 +17267,8 @@
         <v>8346242</v>
       </c>
       <c r="S39" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl93_WT_sgCD_R1_splicing.tsv libraries_2/yjl94_WT_sgCD_R1_splicing.tsv libraries_2/yjl95_WT_sgCD_R1_splicing.tsv libraries_4/yjl96_WT_sgCD_R1_splicing.tsv --total_reads 9334492 9142001 8497185 8346242 -o libraries_3/WT_sgCD_R1_splicing.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl93_WT_sgCD_R1_splicing.tsv libraries_2/yjl94_WT_sgCD_R1_splicing.tsv libraries_2/yjl95_WT_sgCD_R1_splicing.tsv libraries_2/yjl96_WT_sgCD_R1_splicing.tsv --total_reads 9334492 9142001 8497185 8346242 -o libraries_3/WT_sgCD_R1_splicing.tsv --quiet </v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
@@ -17344,8 +17344,8 @@
         <v>6586577</v>
       </c>
       <c r="S40" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl89_WT_sgCD_R2_antisense.tsv libraries_2/yjl90_WT_sgCD_R2_antisense.tsv libraries_2/yjl91_WT_sgCD_R2_antisense.tsv libraries_4/yjl92_WT_sgCD_R2_antisense.tsv --total_reads 7813781 7486736 8114856 6586577 -o libraries_3/WT_sgCD_R2_antisense.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl89_WT_sgCD_R2_antisense.tsv libraries_2/yjl90_WT_sgCD_R2_antisense.tsv libraries_2/yjl91_WT_sgCD_R2_antisense.tsv libraries_2/yjl92_WT_sgCD_R2_antisense.tsv --total_reads 7813781 7486736 8114856 6586577 -o libraries_3/WT_sgCD_R2_antisense.tsv --quiet </v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
@@ -17421,8 +17421,8 @@
         <v>8346242</v>
       </c>
       <c r="S41" t="str">
-        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_4, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl93_WT_sgCD_R2_splicing.tsv libraries_2/yjl94_WT_sgCD_R2_splicing.tsv libraries_2/yjl95_WT_sgCD_R2_splicing.tsv libraries_4/yjl96_WT_sgCD_R2_splicing.tsv --total_reads 9334492 9142001 8497185 8346242 -o libraries_3/WT_sgCD_R2_splicing.tsv --quiet </v>
+        <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl93_WT_sgCD_R2_splicing.tsv libraries_2/yjl94_WT_sgCD_R2_splicing.tsv libraries_2/yjl95_WT_sgCD_R2_splicing.tsv libraries_2/yjl96_WT_sgCD_R2_splicing.tsv --total_reads 9334492 9142001 8497185 8346242 -o libraries_3/WT_sgCD_R2_splicing.tsv --quiet </v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
@@ -18118,46 +18118,46 @@
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H59" t="str">
         <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, S2:S41,M45:M56)</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl217_WT_sgAB_R1_sense.tsv libraries_2/yjl218_WT_sgAB_R1_sense.tsv libraries_2/yjl219_WT_sgAB_R1_sense.tsv libraries_4/yjl220_WT_sgAB_R1_sense.tsv --total_reads 6630053 7246619 8069391 7513691 -o libraries_3/WT_sgAB_R1_sense.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl221_WT_sgAB_R1_branch.tsv libraries_2/yjl222_WT_sgAB_R1_branch.tsv libraries_2/yjl223_WT_sgAB_R1_branch.tsv libraries_4/yjl224_WT_sgAB_R1_branch.tsv --total_reads 9021462 9430938 9051278 9192054 -o libraries_3/WT_sgAB_R1_branch.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl225_WT_sgAB_R1_cmv.tsv libraries_2/yjl226_WT_sgAB_R1_cmv.tsv libraries_2/yjl227_WT_sgAB_R1_cmv.tsv libraries_4/yjl228_WT_sgAB_R1_cmv.tsv --total_reads 7604379 8885716 8150455 7694818 -o libraries_3/WT_sgAB_R1_cmv.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl229_KO_sgAB_R1_sense.tsv libraries_2/yjl230_KO_sgAB_R1_sense.tsv libraries_2/yjl231_KO_sgAB_R1_sense.tsv libraries_4/yjl232_KO_sgAB_R1_sense.tsv --total_reads 11320509 12480734 12500966 12479012 -o libraries_3/KO_sgAB_R1_sense.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl233_KO_sgAB_R1_branch.tsv libraries_2/yjl234_KO_sgAB_R1_branch.tsv libraries_2/yjl235_KO_sgAB_R1_branch.tsv libraries_4/yjl236_KO_sgAB_R1_branch.tsv --total_reads 13912975 15839537 13872702 13493608 -o libraries_3/KO_sgAB_R1_branch.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl237_KO_sgAB_R1_cmv.tsv libraries_2/yjl238_KO_sgAB_R1_cmv.tsv libraries_2/yjl239_KO_sgAB_R1_cmv.tsv libraries_4/yjl240_KO_sgAB_R1_cmv.tsv --total_reads 11307677 11757615 10272339 9412394 -o libraries_3/KO_sgAB_R1_cmv.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl217_WT_sgAB_R2_sense.tsv libraries_2/yjl218_WT_sgAB_R2_sense.tsv libraries_2/yjl219_WT_sgAB_R2_sense.tsv libraries_4/yjl220_WT_sgAB_R2_sense.tsv --total_reads 6177083 6744517 7507107 7001340 -o libraries_3/WT_sgAB_R2_sense.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl221_WT_sgAB_R2_branch.tsv libraries_2/yjl222_WT_sgAB_R2_branch.tsv libraries_2/yjl223_WT_sgAB_R2_branch.tsv libraries_4/yjl224_WT_sgAB_R2_branch.tsv --total_reads 8525251 8875435 8522228 8656502 -o libraries_3/WT_sgAB_R2_branch.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl225_WT_sgAB_R2_cmv.tsv libraries_2/yjl226_WT_sgAB_R2_cmv.tsv libraries_2/yjl227_WT_sgAB_R2_cmv.tsv libraries_4/yjl228_WT_sgAB_R2_cmv.tsv --total_reads 6898791 7986453 7354088 6940576 -o libraries_3/WT_sgAB_R2_cmv.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl229_KO_sgAB_R2_sense.tsv libraries_2/yjl230_KO_sgAB_R2_sense.tsv libraries_2/yjl231_KO_sgAB_R2_sense.tsv libraries_4/yjl232_KO_sgAB_R2_sense.tsv --total_reads 10142826 11211467 11130391 11080481 -o libraries_3/KO_sgAB_R2_sense.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl233_KO_sgAB_R2_branch.tsv libraries_2/yjl234_KO_sgAB_R2_branch.tsv libraries_2/yjl235_KO_sgAB_R2_branch.tsv libraries_4/yjl236_KO_sgAB_R2_branch.tsv --total_reads 12987477 14745821 12946604 12582077 -o libraries_3/KO_sgAB_R2_branch.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl237_KO_sgAB_R2_cmv.tsv libraries_2/yjl238_KO_sgAB_R2_cmv.tsv libraries_2/yjl239_KO_sgAB_R2_cmv.tsv libraries_4/yjl240_KO_sgAB_R2_cmv.tsv --total_reads 10562895 10985096 9559721 8729797 -o libraries_3/KO_sgAB_R2_cmv.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl255_WT_sgA_R1_sense.tsv libraries_2/yjl256_WT_sgA_R1_sense.tsv libraries_2/yjl257_WT_sgA_R1_sense.tsv libraries_4/yjl258_WT_sgA_R1_sense.tsv --total_reads 7579965 7982725 7854740 7534924 -o libraries_3/WT_sgA_R1_sense.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl259_WT_sgA_R1_branch.tsv libraries_2/yjl260_WT_sgA_R1_branch.tsv libraries_2/yjl261_WT_sgA_R1_branch.tsv libraries_4/yjl262_WT_sgA_R1_branch.tsv --total_reads 8808358 9297647 9399483 8799841 -o libraries_3/WT_sgA_R1_branch.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl263_WT_sgA_R1_cmv.tsv libraries_2/yjl264_WT_sgA_R1_cmv.tsv libraries_2/yjl265_WT_sgA_R1_cmv.tsv libraries_4/yjl266_WT_sgA_R1_cmv.tsv --total_reads 8171224 8180897 8314116 8096639 -o libraries_3/WT_sgA_R1_cmv.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl292_KO_sgA_R1_sense.tsv libraries_2/yjl293_KO_sgA_R1_sense.tsv libraries_2/yjl294_KO_sgA_R1_sense.tsv libraries_4/yjl295_KO_sgA_R1_sense.tsv --total_reads 8597510 10116623 8703707 9021103 -o libraries_3/KO_sgA_R1_sense.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl296_KO_sgA_R1_branch.tsv libraries_2/yjl297_KO_sgA_R1_branch.tsv libraries_2/yjl298_KO_sgA_R1_branch.tsv libraries_4/yjl299_KO_sgA_R1_branch.tsv --total_reads 11021111 11280773 12426852 11659042 -o libraries_3/KO_sgA_R1_branch.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl300_KO_sgA_R1_cmv.tsv libraries_2/yjl301_KO_sgA_R1_cmv.tsv libraries_2/yjl302_KO_sgA_R1_cmv.tsv libraries_4/yjl303_KO_sgA_R1_cmv.tsv --total_reads 9933546 10351309 9388188 8668198 -o libraries_3/KO_sgA_R1_cmv.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl267_WT_sgB_R2_sense.tsv libraries_2/yjl268_WT_sgB_R2_sense.tsv libraries_2/yjl269_WT_sgB_R2_sense.tsv libraries_4/yjl270_WT_sgB_R2_sense.tsv --total_reads 7137355 6618133 8227882 7238408 -o libraries_3/WT_sgB_R2_sense.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl271_WT_sgB_R2_branch.tsv libraries_2/yjl272_WT_sgB_R2_branch.tsv libraries_2/yjl273_WT_sgB_R2_branch.tsv libraries_4/yjl274_WT_sgB_R2_branch.tsv --total_reads 9524548 10125834 10173904 9525100 -o libraries_3/WT_sgB_R2_branch.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl275_WT_sgB_R2_cmv.tsv libraries_2/yjl276_WT_sgB_R2_cmv.tsv libraries_2/yjl277_WT_sgB_R2_cmv.tsv libraries_4/yjl278_WT_sgB_R2_cmv.tsv --total_reads 7280860 6872217 6847531 7081713 -o libraries_3/WT_sgB_R2_cmv.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl304_KO_sgB_R2_sense.tsv libraries_2/yjl305_KO_sgB_R2_sense.tsv libraries_2/yjl306_KO_sgB_R2_sense.tsv libraries_4/yjl307_KO_sgB_R2_sense.tsv --total_reads 6494964 7011524 7131423 6545416 -o libraries_3/KO_sgB_R2_sense.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl308_KO_sgB_R2_branch.tsv libraries_2/yjl309_KO_sgB_R2_branch.tsv libraries_2/yjl310_KO_sgB_R2_branch.tsv libraries_4/yjl311_KO_sgB_R2_branch.tsv --total_reads 9730255 10430885 9770845 10249893 -o libraries_3/KO_sgB_R2_branch.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl312_KO_sgB_R2_cmv.tsv libraries_2/yjl313_KO_sgB_R2_cmv.tsv libraries_2/yjl314_KO_sgB_R2_cmv.tsv libraries_4/yjl315_KO_sgB_R2_cmv.tsv --total_reads 6718301 6435913 7285831 6372479 -o libraries_3/KO_sgB_R2_cmv.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl255_WT_sgA_R1_sense_30bpDown.tsv libraries_2/yjl256_WT_sgA_R1_sense_30bpDown.tsv libraries_2/yjl257_WT_sgA_R1_sense_30bpDown.tsv libraries_4/yjl258_WT_sgA_R1_sense_30bpDown.tsv --total_reads 7579965 7982725 7854740 7534924 -o libraries_3/WT_sgA_R1_sense_30bpDown.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl259_WT_sgA_R1_branch_30bpDown.tsv libraries_2/yjl260_WT_sgA_R1_branch_30bpDown.tsv libraries_2/yjl261_WT_sgA_R1_branch_30bpDown.tsv libraries_4/yjl262_WT_sgA_R1_branch_30bpDown.tsv --total_reads 8808358 9297647 9399483 8799841 -o libraries_3/WT_sgA_R1_branch_30bpDown.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl263_WT_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl264_WT_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl265_WT_sgA_R1_cmv_30bpDown.tsv libraries_4/yjl266_WT_sgA_R1_cmv_30bpDown.tsv --total_reads 8171224 8180897 8314116 8096639 -o libraries_3/WT_sgA_R1_cmv_30bpDown.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl292_KO_sgA_R1_sense_30bpDown.tsv libraries_2/yjl293_KO_sgA_R1_sense_30bpDown.tsv libraries_2/yjl294_KO_sgA_R1_sense_30bpDown.tsv libraries_4/yjl295_KO_sgA_R1_sense_30bpDown.tsv --total_reads 8597510 10116623 8703707 9021103 -o libraries_3/KO_sgA_R1_sense_30bpDown.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl296_KO_sgA_R1_branch_30bpDown.tsv libraries_2/yjl297_KO_sgA_R1_branch_30bpDown.tsv libraries_2/yjl298_KO_sgA_R1_branch_30bpDown.tsv libraries_4/yjl299_KO_sgA_R1_branch_30bpDown.tsv --total_reads 11021111 11280773 12426852 11659042 -o libraries_3/KO_sgA_R1_branch_30bpDown.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl300_KO_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl301_KO_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl302_KO_sgA_R1_cmv_30bpDown.tsv libraries_4/yjl303_KO_sgA_R1_cmv_30bpDown.tsv --total_reads 9933546 10351309 9388188 8668198 -o libraries_3/KO_sgA_R1_cmv_30bpDown.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl267_WT_sgB_R2_sense_30bpDown.tsv libraries_2/yjl268_WT_sgB_R2_sense_30bpDown.tsv libraries_2/yjl269_WT_sgB_R2_sense_30bpDown.tsv libraries_4/yjl270_WT_sgB_R2_sense_30bpDown.tsv --total_reads 7137355 6618133 8227882 7238408 -o libraries_3/WT_sgB_R2_sense_30bpDown.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl271_WT_sgB_R2_branch_30bpDown.tsv libraries_2/yjl272_WT_sgB_R2_branch_30bpDown.tsv libraries_2/yjl273_WT_sgB_R2_branch_30bpDown.tsv libraries_4/yjl274_WT_sgB_R2_branch_30bpDown.tsv --total_reads 9524548 10125834 10173904 9525100 -o libraries_3/WT_sgB_R2_branch_30bpDown.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl275_WT_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl276_WT_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl277_WT_sgB_R2_cmv_30bpDown.tsv libraries_4/yjl278_WT_sgB_R2_cmv_30bpDown.tsv --total_reads 7280860 6872217 6847531 7081713 -o libraries_3/WT_sgB_R2_cmv_30bpDown.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl304_KO_sgB_R2_sense_30bpDown.tsv libraries_2/yjl305_KO_sgB_R2_sense_30bpDown.tsv libraries_2/yjl306_KO_sgB_R2_sense_30bpDown.tsv libraries_4/yjl307_KO_sgB_R2_sense_30bpDown.tsv --total_reads 6494964 7011524 7131423 6545416 -o libraries_3/KO_sgB_R2_sense_30bpDown.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl308_KO_sgB_R2_branch_30bpDown.tsv libraries_2/yjl309_KO_sgB_R2_branch_30bpDown.tsv libraries_2/yjl310_KO_sgB_R2_branch_30bpDown.tsv libraries_4/yjl311_KO_sgB_R2_branch_30bpDown.tsv --total_reads 9730255 10430885 9770845 10249893 -o libraries_3/KO_sgB_R2_branch_30bpDown.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl312_KO_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl313_KO_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl314_KO_sgB_R2_cmv_30bpDown.tsv libraries_4/yjl315_KO_sgB_R2_cmv_30bpDown.tsv --total_reads 6718301 6435913 7285831 6372479 -o libraries_3/KO_sgB_R2_cmv_30bpDown.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl89_WT_sgCD_R1_antisense.tsv libraries_2/yjl90_WT_sgCD_R1_antisense.tsv libraries_2/yjl91_WT_sgCD_R1_antisense.tsv libraries_4/yjl92_WT_sgCD_R1_antisense.tsv --total_reads 7813781 7486736 8114856 6586577 -o libraries_3/WT_sgCD_R1_antisense.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl93_WT_sgCD_R1_splicing.tsv libraries_2/yjl94_WT_sgCD_R1_splicing.tsv libraries_2/yjl95_WT_sgCD_R1_splicing.tsv libraries_4/yjl96_WT_sgCD_R1_splicing.tsv --total_reads 9334492 9142001 8497185 8346242 -o libraries_3/WT_sgCD_R1_splicing.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl89_WT_sgCD_R2_antisense.tsv libraries_2/yjl90_WT_sgCD_R2_antisense.tsv libraries_2/yjl91_WT_sgCD_R2_antisense.tsv libraries_4/yjl92_WT_sgCD_R2_antisense.tsv --total_reads 7813781 7486736 8114856 6586577 -o libraries_3/WT_sgCD_R2_antisense.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl93_WT_sgCD_R2_splicing.tsv libraries_2/yjl94_WT_sgCD_R2_splicing.tsv libraries_2/yjl95_WT_sgCD_R2_splicing.tsv libraries_4/yjl96_WT_sgCD_R2_splicing.tsv --total_reads 9334492 9142001 8497185 8346242 -o libraries_3/WT_sgCD_R2_splicing.tsv --quiet 
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl217_WT_sgAB_R1_sense.tsv libraries_2/yjl218_WT_sgAB_R1_sense.tsv libraries_2/yjl219_WT_sgAB_R1_sense.tsv libraries_2/yjl220_WT_sgAB_R1_sense.tsv --total_reads 6630053 7246619 8069391 7513691 -o libraries_3/WT_sgAB_R1_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl221_WT_sgAB_R1_branch.tsv libraries_2/yjl222_WT_sgAB_R1_branch.tsv libraries_2/yjl223_WT_sgAB_R1_branch.tsv libraries_2/yjl224_WT_sgAB_R1_branch.tsv --total_reads 9021462 9430938 9051278 9192054 -o libraries_3/WT_sgAB_R1_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl225_WT_sgAB_R1_cmv.tsv libraries_2/yjl226_WT_sgAB_R1_cmv.tsv libraries_2/yjl227_WT_sgAB_R1_cmv.tsv libraries_2/yjl228_WT_sgAB_R1_cmv.tsv --total_reads 7604379 8885716 8150455 7694818 -o libraries_3/WT_sgAB_R1_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl229_KO_sgAB_R1_sense.tsv libraries_2/yjl230_KO_sgAB_R1_sense.tsv libraries_2/yjl231_KO_sgAB_R1_sense.tsv libraries_2/yjl232_KO_sgAB_R1_sense.tsv --total_reads 11320509 12480734 12500966 12479012 -o libraries_3/KO_sgAB_R1_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl233_KO_sgAB_R1_branch.tsv libraries_2/yjl234_KO_sgAB_R1_branch.tsv libraries_2/yjl235_KO_sgAB_R1_branch.tsv libraries_2/yjl236_KO_sgAB_R1_branch.tsv --total_reads 13912975 15839537 13872702 13493608 -o libraries_3/KO_sgAB_R1_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl237_KO_sgAB_R1_cmv.tsv libraries_2/yjl238_KO_sgAB_R1_cmv.tsv libraries_2/yjl239_KO_sgAB_R1_cmv.tsv libraries_2/yjl240_KO_sgAB_R1_cmv.tsv --total_reads 11307677 11757615 10272339 9412394 -o libraries_3/KO_sgAB_R1_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl217_WT_sgAB_R2_sense.tsv libraries_2/yjl218_WT_sgAB_R2_sense.tsv libraries_2/yjl219_WT_sgAB_R2_sense.tsv libraries_2/yjl220_WT_sgAB_R2_sense.tsv --total_reads 6177083 6744517 7507107 7001340 -o libraries_3/WT_sgAB_R2_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl221_WT_sgAB_R2_branch.tsv libraries_2/yjl222_WT_sgAB_R2_branch.tsv libraries_2/yjl223_WT_sgAB_R2_branch.tsv libraries_2/yjl224_WT_sgAB_R2_branch.tsv --total_reads 8525251 8875435 8522228 8656502 -o libraries_3/WT_sgAB_R2_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl225_WT_sgAB_R2_cmv.tsv libraries_2/yjl226_WT_sgAB_R2_cmv.tsv libraries_2/yjl227_WT_sgAB_R2_cmv.tsv libraries_2/yjl228_WT_sgAB_R2_cmv.tsv --total_reads 6898791 7986453 7354088 6940576 -o libraries_3/WT_sgAB_R2_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl229_KO_sgAB_R2_sense.tsv libraries_2/yjl230_KO_sgAB_R2_sense.tsv libraries_2/yjl231_KO_sgAB_R2_sense.tsv libraries_2/yjl232_KO_sgAB_R2_sense.tsv --total_reads 10142826 11211467 11130391 11080481 -o libraries_3/KO_sgAB_R2_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl233_KO_sgAB_R2_branch.tsv libraries_2/yjl234_KO_sgAB_R2_branch.tsv libraries_2/yjl235_KO_sgAB_R2_branch.tsv libraries_2/yjl236_KO_sgAB_R2_branch.tsv --total_reads 12987477 14745821 12946604 12582077 -o libraries_3/KO_sgAB_R2_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl237_KO_sgAB_R2_cmv.tsv libraries_2/yjl238_KO_sgAB_R2_cmv.tsv libraries_2/yjl239_KO_sgAB_R2_cmv.tsv libraries_2/yjl240_KO_sgAB_R2_cmv.tsv --total_reads 10562895 10985096 9559721 8729797 -o libraries_3/KO_sgAB_R2_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl255_WT_sgA_R1_sense.tsv libraries_2/yjl256_WT_sgA_R1_sense.tsv libraries_2/yjl257_WT_sgA_R1_sense.tsv libraries_2/yjl258_WT_sgA_R1_sense.tsv --total_reads 7579965 7982725 7854740 7534924 -o libraries_3/WT_sgA_R1_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl259_WT_sgA_R1_branch.tsv libraries_2/yjl260_WT_sgA_R1_branch.tsv libraries_2/yjl261_WT_sgA_R1_branch.tsv libraries_2/yjl262_WT_sgA_R1_branch.tsv --total_reads 8808358 9297647 9399483 8799841 -o libraries_3/WT_sgA_R1_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl263_WT_sgA_R1_cmv.tsv libraries_2/yjl264_WT_sgA_R1_cmv.tsv libraries_2/yjl265_WT_sgA_R1_cmv.tsv libraries_2/yjl266_WT_sgA_R1_cmv.tsv --total_reads 8171224 8180897 8314116 8096639 -o libraries_3/WT_sgA_R1_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl292_KO_sgA_R1_sense.tsv libraries_2/yjl293_KO_sgA_R1_sense.tsv libraries_2/yjl294_KO_sgA_R1_sense.tsv libraries_2/yjl295_KO_sgA_R1_sense.tsv --total_reads 8597510 10116623 8703707 9021103 -o libraries_3/KO_sgA_R1_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl296_KO_sgA_R1_branch.tsv libraries_2/yjl297_KO_sgA_R1_branch.tsv libraries_2/yjl298_KO_sgA_R1_branch.tsv libraries_2/yjl299_KO_sgA_R1_branch.tsv --total_reads 11021111 11280773 12426852 11659042 -o libraries_3/KO_sgA_R1_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl300_KO_sgA_R1_cmv.tsv libraries_2/yjl301_KO_sgA_R1_cmv.tsv libraries_2/yjl302_KO_sgA_R1_cmv.tsv libraries_2/yjl303_KO_sgA_R1_cmv.tsv --total_reads 9933546 10351309 9388188 8668198 -o libraries_3/KO_sgA_R1_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl267_WT_sgB_R2_sense.tsv libraries_2/yjl268_WT_sgB_R2_sense.tsv libraries_2/yjl269_WT_sgB_R2_sense.tsv libraries_2/yjl270_WT_sgB_R2_sense.tsv --total_reads 7137355 6618133 8227882 7238408 -o libraries_3/WT_sgB_R2_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl271_WT_sgB_R2_branch.tsv libraries_2/yjl272_WT_sgB_R2_branch.tsv libraries_2/yjl273_WT_sgB_R2_branch.tsv libraries_2/yjl274_WT_sgB_R2_branch.tsv --total_reads 9524548 10125834 10173904 9525100 -o libraries_3/WT_sgB_R2_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl275_WT_sgB_R2_cmv.tsv libraries_2/yjl276_WT_sgB_R2_cmv.tsv libraries_2/yjl277_WT_sgB_R2_cmv.tsv libraries_2/yjl278_WT_sgB_R2_cmv.tsv --total_reads 7280860 6872217 6847531 7081713 -o libraries_3/WT_sgB_R2_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl304_KO_sgB_R2_sense.tsv libraries_2/yjl305_KO_sgB_R2_sense.tsv libraries_2/yjl306_KO_sgB_R2_sense.tsv libraries_2/yjl307_KO_sgB_R2_sense.tsv --total_reads 6494964 7011524 7131423 6545416 -o libraries_3/KO_sgB_R2_sense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl308_KO_sgB_R2_branch.tsv libraries_2/yjl309_KO_sgB_R2_branch.tsv libraries_2/yjl310_KO_sgB_R2_branch.tsv libraries_2/yjl311_KO_sgB_R2_branch.tsv --total_reads 9730255 10430885 9770845 10249893 -o libraries_3/KO_sgB_R2_branch.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl312_KO_sgB_R2_cmv.tsv libraries_2/yjl313_KO_sgB_R2_cmv.tsv libraries_2/yjl314_KO_sgB_R2_cmv.tsv libraries_2/yjl315_KO_sgB_R2_cmv.tsv --total_reads 6718301 6435913 7285831 6372479 -o libraries_3/KO_sgB_R2_cmv.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl255_WT_sgA_R1_sense_30bpDown.tsv libraries_2/yjl256_WT_sgA_R1_sense_30bpDown.tsv libraries_2/yjl257_WT_sgA_R1_sense_30bpDown.tsv libraries_2/yjl258_WT_sgA_R1_sense_30bpDown.tsv --total_reads 7579965 7982725 7854740 7534924 -o libraries_3/WT_sgA_R1_sense_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl259_WT_sgA_R1_branch_30bpDown.tsv libraries_2/yjl260_WT_sgA_R1_branch_30bpDown.tsv libraries_2/yjl261_WT_sgA_R1_branch_30bpDown.tsv libraries_2/yjl262_WT_sgA_R1_branch_30bpDown.tsv --total_reads 8808358 9297647 9399483 8799841 -o libraries_3/WT_sgA_R1_branch_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl263_WT_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl264_WT_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl265_WT_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl266_WT_sgA_R1_cmv_30bpDown.tsv --total_reads 8171224 8180897 8314116 8096639 -o libraries_3/WT_sgA_R1_cmv_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl292_KO_sgA_R1_sense_30bpDown.tsv libraries_2/yjl293_KO_sgA_R1_sense_30bpDown.tsv libraries_2/yjl294_KO_sgA_R1_sense_30bpDown.tsv libraries_2/yjl295_KO_sgA_R1_sense_30bpDown.tsv --total_reads 8597510 10116623 8703707 9021103 -o libraries_3/KO_sgA_R1_sense_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl296_KO_sgA_R1_branch_30bpDown.tsv libraries_2/yjl297_KO_sgA_R1_branch_30bpDown.tsv libraries_2/yjl298_KO_sgA_R1_branch_30bpDown.tsv libraries_2/yjl299_KO_sgA_R1_branch_30bpDown.tsv --total_reads 11021111 11280773 12426852 11659042 -o libraries_3/KO_sgA_R1_branch_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl300_KO_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl301_KO_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl302_KO_sgA_R1_cmv_30bpDown.tsv libraries_2/yjl303_KO_sgA_R1_cmv_30bpDown.tsv --total_reads 9933546 10351309 9388188 8668198 -o libraries_3/KO_sgA_R1_cmv_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl267_WT_sgB_R2_sense_30bpDown.tsv libraries_2/yjl268_WT_sgB_R2_sense_30bpDown.tsv libraries_2/yjl269_WT_sgB_R2_sense_30bpDown.tsv libraries_2/yjl270_WT_sgB_R2_sense_30bpDown.tsv --total_reads 7137355 6618133 8227882 7238408 -o libraries_3/WT_sgB_R2_sense_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl271_WT_sgB_R2_branch_30bpDown.tsv libraries_2/yjl272_WT_sgB_R2_branch_30bpDown.tsv libraries_2/yjl273_WT_sgB_R2_branch_30bpDown.tsv libraries_2/yjl274_WT_sgB_R2_branch_30bpDown.tsv --total_reads 9524548 10125834 10173904 9525100 -o libraries_3/WT_sgB_R2_branch_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl275_WT_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl276_WT_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl277_WT_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl278_WT_sgB_R2_cmv_30bpDown.tsv --total_reads 7280860 6872217 6847531 7081713 -o libraries_3/WT_sgB_R2_cmv_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl304_KO_sgB_R2_sense_30bpDown.tsv libraries_2/yjl305_KO_sgB_R2_sense_30bpDown.tsv libraries_2/yjl306_KO_sgB_R2_sense_30bpDown.tsv libraries_2/yjl307_KO_sgB_R2_sense_30bpDown.tsv --total_reads 6494964 7011524 7131423 6545416 -o libraries_3/KO_sgB_R2_sense_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl308_KO_sgB_R2_branch_30bpDown.tsv libraries_2/yjl309_KO_sgB_R2_branch_30bpDown.tsv libraries_2/yjl310_KO_sgB_R2_branch_30bpDown.tsv libraries_2/yjl311_KO_sgB_R2_branch_30bpDown.tsv --total_reads 9730255 10430885 9770845 10249893 -o libraries_3/KO_sgB_R2_branch_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl312_KO_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl313_KO_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl314_KO_sgB_R2_cmv_30bpDown.tsv libraries_2/yjl315_KO_sgB_R2_cmv_30bpDown.tsv --total_reads 6718301 6435913 7285831 6372479 -o libraries_3/KO_sgB_R2_cmv_30bpDown.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl89_WT_sgCD_R1_antisense.tsv libraries_2/yjl90_WT_sgCD_R1_antisense.tsv libraries_2/yjl91_WT_sgCD_R1_antisense.tsv libraries_2/yjl92_WT_sgCD_R1_antisense.tsv --total_reads 7813781 7486736 8114856 6586577 -o libraries_3/WT_sgCD_R1_antisense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl93_WT_sgCD_R1_splicing.tsv libraries_2/yjl94_WT_sgCD_R1_splicing.tsv libraries_2/yjl95_WT_sgCD_R1_splicing.tsv libraries_2/yjl96_WT_sgCD_R1_splicing.tsv --total_reads 9334492 9142001 8497185 8346242 -o libraries_3/WT_sgCD_R1_splicing.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl89_WT_sgCD_R2_antisense.tsv libraries_2/yjl90_WT_sgCD_R2_antisense.tsv libraries_2/yjl91_WT_sgCD_R2_antisense.tsv libraries_2/yjl92_WT_sgCD_R2_antisense.tsv --total_reads 7813781 7486736 8114856 6586577 -o libraries_3/WT_sgCD_R2_antisense.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl93_WT_sgCD_R2_splicing.tsv libraries_2/yjl94_WT_sgCD_R2_splicing.tsv libraries_2/yjl95_WT_sgCD_R2_splicing.tsv libraries_2/yjl96_WT_sgCD_R2_splicing.tsv --total_reads 9334492 9142001 8497185 8346242 -o libraries_3/WT_sgCD_R2_splicing.tsv --quiet 
 python 1_process_nhej/combine_repeats.py -i libraries_2/yjl244_WT_sgA_R1_sense_nodsb.tsv  --total_reads 10005232 -o libraries_3/WT_sgA_R1_sense_nodsb.tsv --quiet 
 python 1_process_nhej/combine_repeats.py -i libraries_2/yjl245_WT_sgA_R1_branch_nodsb.tsv  --total_reads 12898941 -o libraries_3/WT_sgA_R1_branch_nodsb.tsv --quiet 
 python 1_process_nhej/combine_repeats.py -i libraries_2/yjl246_WT_sgA_R1_cmv_nodsb.tsv  --total_reads 10217401 -o libraries_3/WT_sgA_R1_cmv_nodsb.tsv --quiet 
@@ -26099,8 +26099,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:R67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="K45" sqref="K45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fix typo nodsb => noDSB. Add run_all scripts.
</commit_message>
<xml_diff>
--- a/analyze_nhej/libinfo.xlsx
+++ b/analyze_nhej/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\analyze_nhej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41892E74-79E0-4C6E-AD90-EE2CA8DD30C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD9E6BC-FAC3-48E6-8E0E-D2E56755B08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="3" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="2" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -515,9 +515,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>nodsb</t>
-  </si>
-  <si>
     <t>30bpDown</t>
   </si>
   <si>
@@ -658,6 +655,9 @@
   <si>
     <t>full_command_graph</t>
   </si>
+  <si>
+    <t>noDSB</t>
+  </si>
 </sst>
 </file>
 
@@ -777,9 +777,6 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FFD19645-61C4-4244-A560-0232B787F38C}"/>
   </cellStyles>
   <dxfs count="200">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1878,6 +1875,9 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1990,44 +1990,44 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="97">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="96">
   <autoFilter ref="A1:M41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="13">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="96"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="95">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="95"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="94">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="94">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="93">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="93">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="92">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="92">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="91">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="91">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="90">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="90">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="89">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="89">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="88">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="88">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="87">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="87">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="86">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="86">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="85">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="85">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="84">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="84">
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="83">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2040,40 +2040,40 @@
   <autoFilter ref="A43:M55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
-    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="83">
+    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="82">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="82">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="81">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="81">
+    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="80">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="80">
+    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="79">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="79">
+    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="78">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="78">
+    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="77">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="77">
+    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="76">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="76">
+    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="75">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="75">
+    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="74">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="74">
+    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="73">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="73">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="72">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="72">
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="71">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2082,36 +2082,36 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="71">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="70">
   <autoFilter ref="A3:I4" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="70"/>
-    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="69">
+    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="69"/>
+    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="68">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="68">
+    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="67">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="67">
+    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="66">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="66">
+    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="65">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 12 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="33" xr3:uid="{8FF7E83A-9135-4A64-965C-48368A6C0367}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="65">
+    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="64">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="64">
+    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="63">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="63">
+    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="62">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2120,32 +2120,32 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="61">
   <autoFilter ref="A7:I9" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="61"/>
-    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="60">
+    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="60"/>
+    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="59">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="59">
+    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="58">
       <calculatedColumnFormula>IF(table_6_4[[#This Row],[hguide]]="A",NA(), IF(var_6_layout = "universal", "1 1 1 1 1 1", NA()))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="58">
+    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="57">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="57">
+    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="56">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" xr3:uid="{5BD83012-469D-4202-9584-AA182CDF11F9}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="56">
+    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="55">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="55">
+    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="54">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="54">
+    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="53">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2154,36 +2154,36 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="53" headerRowBorderDxfId="52" tableBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50">
   <autoFilter ref="A12:I13" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0F421990-E775-4F35-92AF-6BA19E0E8AEE}" name="index"/>
-    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="50">
+    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="49">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="49">
+    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="48">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0,4, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="48">
+    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="47">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="47">
+    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="46">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{E0783723-9246-4BF6-A5DA-E000EA1E5E87}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="46">
+    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="45">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="45">
+    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="44">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="44">
+    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="43">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2192,44 +2192,44 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:R42" totalsRowShown="0" headerRowDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:R42" totalsRowShown="0" headerRowDxfId="42">
   <autoFilter ref="A2:R42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="18">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="42"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="41">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="40">
       <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="40">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="39">
       <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="39">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="38">
       <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="38">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="37">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="37">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="36">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="36">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="35">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="35">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="34">
       <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="34">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="33">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="33">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="32">
       <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="32">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="31">
       <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="31">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="30">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="30">
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="29">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
       OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
       IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
@@ -2241,19 +2241,19 @@
       )
   )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="29">
+    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="28">
       <calculatedColumnFormula>AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="28">
+    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="27">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 13 --range_y -22 22 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 13 --range_y -18 25 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 13 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 13 --range_y -20 16 ", NA())))), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{891739FF-B093-4EE5-A0A2-20948C58CB96}" name="universal_layout_legend_pos_x" dataDxfId="27">
+    <tableColumn id="17" xr3:uid="{891739FF-B093-4EE5-A0A2-20948C58CB96}" name="universal_layout_legend_pos_x" dataDxfId="26">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 12, IF(table_7_1[[#This Row],[hguide]]="A", 12, IF(table_7_1[[#This Row],[hguide]]="B", 12, IF(table_7_1[[#This Row],[hguide]]="CD", 12, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="26">
+    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="25">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/individual/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="25">
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="24">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], IF(NOT(ISNA(table_7_1[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_1[[#This Row],[universal_layout_legend_pos_x]], "")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2262,38 +2262,38 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:K60" totalsRowShown="0" headerRowDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:K60" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="A44:K60" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="22">
+    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="21">
+    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="20">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="20">
+    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="19">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="19">
+    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="18">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="18">
+    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="17">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="17">
+    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="16">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="16">
+    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="15">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_legend_pos_x" dataDxfId="15">
+    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_legend_pos_x" dataDxfId="14">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_legend_pos_x]:[universal_layout_legend_pos_x]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="14">
+    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="13">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="13">
+    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="12">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], IF(NOT(ISNA(table_7_2[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_2[[#This Row],[universal_layout_legend_pos_x]], "")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2302,38 +2302,38 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:K64" totalsRowShown="0" headerRowDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:K64" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A62:K64" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_4_2[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="9">
+    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="8">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="8">
+    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="7">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="7">
+    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="6">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="6">
+    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="5">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="5">
+    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="4">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="4">
+    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="3">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_legend_pos_x" dataDxfId="3">
+    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_legend_pos_x" dataDxfId="2">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_legend_pos_x]:[universal_layout_legend_pos_x]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="1">
+    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], IF(NOT(ISNA(table_7_3[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_3[[#This Row],[universal_layout_legend_pos_x]], "")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2435,7 +2435,7 @@
     <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="174">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="0">
+    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="173">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2447,41 +2447,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}" name="table_2_2" displayName="table_2_2" ref="A44:M56" totalsRowShown="0">
   <autoFilter ref="A44:M56" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="173"/>
-    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="172">
+    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="172"/>
+    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="171">
       <calculatedColumnFormula>OFFSET(table_1[ref], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="171">
+    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="170">
       <calculatedColumnFormula>OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="170">
+    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="169">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="169">
+    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="168">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="168">
+    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="167">
       <calculatedColumnFormula>OFFSET(table_1[cell], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="167">
+    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="166">
       <calculatedColumnFormula>OFFSET(table_1[strand], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="166">
+    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="165">
       <calculatedColumnFormula>OFFSET(table_1[treatment], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="165">
+    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="164">
       <calculatedColumnFormula>OFFSET(table_1[hguide], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="164">
+    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="163">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_2[[#This Row],[cell]], "_", table_2_2[[#This Row],[hguide]], "_", table_2_2[[#This Row],[strand]], "_", table_2_2[[#This Row],[treatment]], "_nodsb")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="163">
+    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="162">
       <calculatedColumnFormula>OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="162">
+    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="161">
       <calculatedColumnFormula>OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="161">
+    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="160">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2490,47 +2490,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="160">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="159">
   <autoFilter ref="A1:N41" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="159"/>
-    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="158">
+    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="158"/>
+    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="157">
       <calculatedColumnFormula>OFFSET(table_2_1[output_dir], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="157">
+    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="156">
       <calculatedColumnFormula>OFFSET(table_2_1[control], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="156">
+    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="155">
       <calculatedColumnFormula>OFFSET(table_2_1[ref], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="155">
+    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="154">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="154">
+    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="153">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="153">
+    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="152">
       <calculatedColumnFormula array="1">IF(table_3_1[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_1[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_1[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="152">
+    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="151">
       <calculatedColumnFormula>OFFSET(table_2_1[strand], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="151">
+    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="150">
       <calculatedColumnFormula>MID(OFFSET(table_2_1[hguide], table_3_1[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="150">
+    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="149">
       <calculatedColumnFormula>OFFSET(table_2_1[cell], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="149">
+    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="148">
       <calculatedColumnFormula>OFFSET(table_2_1[treatment], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DB6998A3-1431-4DDD-8DA0-525B805BF436}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="148">
+    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="147">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="147">
+    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="146">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2539,47 +2539,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="146">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="145">
   <autoFilter ref="A43:N55" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="145"/>
-    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="144">
+    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="144"/>
+    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="143">
       <calculatedColumnFormula>OFFSET(table_2_2[output_dir], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="143">
+    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="142">
       <calculatedColumnFormula>OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="142">
+    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="141">
       <calculatedColumnFormula>OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="141">
+    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="140">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_pos], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="140">
+    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="139">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_type], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="139">
+    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="138">
       <calculatedColumnFormula array="1">IF(table_3_2[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_2[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_2[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="138">
+    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="137">
       <calculatedColumnFormula>OFFSET(table_2_2[strand], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="137">
+    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="136">
       <calculatedColumnFormula>MID(OFFSET(table_2_2[hguide], table_3_2[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="136">
+    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="135">
       <calculatedColumnFormula>OFFSET(table_2_2[cell], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="135">
+    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="134">
       <calculatedColumnFormula>OFFSET(table_2_2[treatment], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{142C480D-E258-4979-A008-3940A3FE78E4}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="134">
+    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="133">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="133">
+    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="132">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2588,38 +2588,38 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="132">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="131">
   <autoFilter ref="A1:K17" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="131"/>
-    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="130">
+    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="130"/>
+    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="129">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="129">
+    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="128">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="128">
+    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="127">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="127">
+    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="126">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="126">
+    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="125">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="125">
+    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="124">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_1[[#This Row],[treatment_1]], "_", table_4_1[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="124">
+    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="123">
       <calculatedColumnFormula>SUBSTITUTE(table_4_1[[#This Row],[dir_1]], table_4_1[[#This Row],[treatment_1]], table_4_1[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="123">
+    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="122">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="122">
+    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="121">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_1[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_1[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_1[[#This Row],[dir_out]], " --subst_type ", table_4_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="121">
+    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="120">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_1[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2628,38 +2628,38 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="119">
   <autoFilter ref="A20:K22" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="119"/>
-    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="118">
+    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="118"/>
+    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="117">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_4_anti_offset + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="117">
+    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="116">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="116">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="115">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="115">
+    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="114">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="114">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="113">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="113">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="112">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_2[[#This Row],[treatment_1]], "_", table_4_2[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="112">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="111">
       <calculatedColumnFormula>SUBSTITUTE(table_4_2[[#This Row],[dir_1]], table_4_2[[#This Row],[treatment_1]], table_4_2[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="111">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="110">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_2[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_2[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_2[[#This Row],[dir_out]], " --subst_type ", table_4_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="110">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="109">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_2[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2668,38 +2668,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="109">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="108">
   <autoFilter ref="A25:K33" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="108"/>
-    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="107">
+    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="107"/>
+    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="106">
       <calculatedColumnFormula>OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="106">
+    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="105">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="105">
+    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="104">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="104">
+    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="103">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="103">
+    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="102">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="102">
+    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="101">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_3[[#This Row],[treatment_1]], "_", table_4_3[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="101">
+    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="100">
       <calculatedColumnFormula>SUBSTITUTE(table_4_3[[#This Row],[dir_1]], table_4_3[[#This Row],[treatment_1]], table_4_3[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="100">
+    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="99">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="99">
+    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="98">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_3[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_3[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_3[[#This Row],[dir_out]], " --subst_type ", table_4_3[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="98">
+    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="97">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_3[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_3[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3041,27 +3041,27 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3084,7 +3084,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B1" t="s">
         <v>80</v>
@@ -3582,7 +3582,7 @@
         <v>241</v>
       </c>
       <c r="B34" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C34">
         <v>12353899</v>
@@ -3597,7 +3597,7 @@
         <v>242</v>
       </c>
       <c r="B35" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C35">
         <v>8729055</v>
@@ -3612,7 +3612,7 @@
         <v>243</v>
       </c>
       <c r="B36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C36">
         <v>9194763</v>
@@ -3672,7 +3672,7 @@
         <v>247</v>
       </c>
       <c r="B40" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C40">
         <v>8496668</v>
@@ -3687,7 +3687,7 @@
         <v>248</v>
       </c>
       <c r="B41" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C41">
         <v>8842556</v>
@@ -3702,7 +3702,7 @@
         <v>249</v>
       </c>
       <c r="B42" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C42">
         <v>8994367</v>
@@ -3717,7 +3717,7 @@
         <v>250</v>
       </c>
       <c r="B43" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C43">
         <v>7898524</v>
@@ -3732,7 +3732,7 @@
         <v>251</v>
       </c>
       <c r="B44" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C44">
         <v>8711046</v>
@@ -3747,7 +3747,7 @@
         <v>252</v>
       </c>
       <c r="B45" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C45">
         <v>8055418</v>
@@ -3762,7 +3762,7 @@
         <v>253</v>
       </c>
       <c r="B46" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C46">
         <v>8697160</v>
@@ -3777,7 +3777,7 @@
         <v>254</v>
       </c>
       <c r="B47" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C47">
         <v>8748510</v>
@@ -4152,7 +4152,7 @@
         <v>279</v>
       </c>
       <c r="B72" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C72">
         <v>7179482</v>
@@ -4167,7 +4167,7 @@
         <v>280</v>
       </c>
       <c r="B73" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C73">
         <v>8143045</v>
@@ -4227,7 +4227,7 @@
         <v>284</v>
       </c>
       <c r="B77" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C77">
         <v>6747088</v>
@@ -4242,7 +4242,7 @@
         <v>285</v>
       </c>
       <c r="B78" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C78">
         <v>7603110</v>
@@ -4257,7 +4257,7 @@
         <v>286</v>
       </c>
       <c r="B79" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C79">
         <v>6540897</v>
@@ -4272,7 +4272,7 @@
         <v>287</v>
       </c>
       <c r="B80" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C80">
         <v>6213540</v>
@@ -4287,7 +4287,7 @@
         <v>288</v>
       </c>
       <c r="B81" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C81">
         <v>6775774</v>
@@ -4302,7 +4302,7 @@
         <v>289</v>
       </c>
       <c r="B82" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C82">
         <v>6586903</v>
@@ -4317,7 +4317,7 @@
         <v>290</v>
       </c>
       <c r="B83" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C83">
         <v>6492202</v>
@@ -4332,7 +4332,7 @@
         <v>291</v>
       </c>
       <c r="B84" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C84">
         <v>6473393</v>
@@ -4713,8 +4713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F1EACD-27DC-4973-8E3A-9162F610D9C4}">
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView topLeftCell="B169" workbookViewId="0">
-      <selection activeCell="B176" sqref="B176"/>
+    <sheetView tabSelected="1" topLeftCell="B157" workbookViewId="0">
+      <selection activeCell="O173" sqref="O173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4729,7 +4729,7 @@
     <col min="8" max="8" width="10.42578125" customWidth="1"/>
     <col min="9" max="9" width="25.140625" customWidth="1"/>
     <col min="10" max="10" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="31.42578125" customWidth="1"/>
     <col min="12" max="12" width="13.140625" customWidth="1"/>
     <col min="13" max="13" width="13.28515625" customWidth="1"/>
     <col min="14" max="14" width="22.28515625" customWidth="1"/>
@@ -9977,7 +9977,7 @@
         <v>1</v>
       </c>
       <c r="D98" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E98" t="s">
         <v>124</v>
@@ -10031,7 +10031,7 @@
         <v>1</v>
       </c>
       <c r="D99" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E99" t="s">
         <v>124</v>
@@ -10085,7 +10085,7 @@
         <v>1</v>
       </c>
       <c r="D100" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E100" t="s">
         <v>124</v>
@@ -10139,7 +10139,7 @@
         <v>1</v>
       </c>
       <c r="D101" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E101" t="s">
         <v>124</v>
@@ -10193,7 +10193,7 @@
         <v>1</v>
       </c>
       <c r="D102" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E102" t="s">
         <v>124</v>
@@ -10247,7 +10247,7 @@
         <v>1</v>
       </c>
       <c r="D103" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E103" t="s">
         <v>124</v>
@@ -10301,7 +10301,7 @@
         <v>1</v>
       </c>
       <c r="D104" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E104" t="s">
         <v>124</v>
@@ -10355,7 +10355,7 @@
         <v>1</v>
       </c>
       <c r="D105" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E105" t="s">
         <v>124</v>
@@ -10409,7 +10409,7 @@
         <v>1</v>
       </c>
       <c r="D106" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E106" t="s">
         <v>124</v>
@@ -10463,7 +10463,7 @@
         <v>1</v>
       </c>
       <c r="D107" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E107" t="s">
         <v>124</v>
@@ -10517,7 +10517,7 @@
         <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E108" t="s">
         <v>124</v>
@@ -10571,7 +10571,7 @@
         <v>1</v>
       </c>
       <c r="D109" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E109" t="s">
         <v>124</v>
@@ -10625,7 +10625,7 @@
         <v>14</v>
       </c>
       <c r="D110" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E110" t="s">
         <v>124</v>
@@ -10679,7 +10679,7 @@
         <v>14</v>
       </c>
       <c r="D111" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E111" t="s">
         <v>124</v>
@@ -10733,7 +10733,7 @@
         <v>14</v>
       </c>
       <c r="D112" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E112" t="s">
         <v>124</v>
@@ -10787,7 +10787,7 @@
         <v>14</v>
       </c>
       <c r="D113" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E113" t="s">
         <v>124</v>
@@ -10841,7 +10841,7 @@
         <v>14</v>
       </c>
       <c r="D114" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E114" t="s">
         <v>124</v>
@@ -10895,7 +10895,7 @@
         <v>14</v>
       </c>
       <c r="D115" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E115" t="s">
         <v>124</v>
@@ -10949,7 +10949,7 @@
         <v>14</v>
       </c>
       <c r="D116" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E116" t="s">
         <v>124</v>
@@ -11003,7 +11003,7 @@
         <v>14</v>
       </c>
       <c r="D117" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E117" t="s">
         <v>124</v>
@@ -11057,7 +11057,7 @@
         <v>14</v>
       </c>
       <c r="D118" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E118" t="s">
         <v>124</v>
@@ -11111,7 +11111,7 @@
         <v>14</v>
       </c>
       <c r="D119" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E119" t="s">
         <v>124</v>
@@ -11165,7 +11165,7 @@
         <v>14</v>
       </c>
       <c r="D120" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E120" t="s">
         <v>124</v>
@@ -11219,7 +11219,7 @@
         <v>14</v>
       </c>
       <c r="D121" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E121" t="s">
         <v>124</v>
@@ -11273,7 +11273,7 @@
         <v>1</v>
       </c>
       <c r="D122" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E122" t="s">
         <v>124</v>
@@ -11327,7 +11327,7 @@
         <v>1</v>
       </c>
       <c r="D123" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E123" t="s">
         <v>124</v>
@@ -11381,7 +11381,7 @@
         <v>1</v>
       </c>
       <c r="D124" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E124" t="s">
         <v>124</v>
@@ -11435,7 +11435,7 @@
         <v>1</v>
       </c>
       <c r="D125" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E125" t="s">
         <v>124</v>
@@ -11489,7 +11489,7 @@
         <v>1</v>
       </c>
       <c r="D126" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E126" t="s">
         <v>124</v>
@@ -11543,7 +11543,7 @@
         <v>1</v>
       </c>
       <c r="D127" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E127" t="s">
         <v>124</v>
@@ -11597,7 +11597,7 @@
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E128" t="s">
         <v>124</v>
@@ -11651,7 +11651,7 @@
         <v>1</v>
       </c>
       <c r="D129" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E129" t="s">
         <v>124</v>
@@ -11705,7 +11705,7 @@
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E130" t="s">
         <v>124</v>
@@ -11759,7 +11759,7 @@
         <v>1</v>
       </c>
       <c r="D131" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E131" t="s">
         <v>124</v>
@@ -11813,7 +11813,7 @@
         <v>1</v>
       </c>
       <c r="D132" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E132" t="s">
         <v>124</v>
@@ -11867,7 +11867,7 @@
         <v>1</v>
       </c>
       <c r="D133" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E133" t="s">
         <v>124</v>
@@ -11921,7 +11921,7 @@
         <v>14</v>
       </c>
       <c r="D134" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E134" t="s">
         <v>124</v>
@@ -11975,7 +11975,7 @@
         <v>14</v>
       </c>
       <c r="D135" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E135" t="s">
         <v>124</v>
@@ -12029,7 +12029,7 @@
         <v>14</v>
       </c>
       <c r="D136" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E136" t="s">
         <v>124</v>
@@ -12083,7 +12083,7 @@
         <v>14</v>
       </c>
       <c r="D137" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E137" t="s">
         <v>124</v>
@@ -12137,7 +12137,7 @@
         <v>14</v>
       </c>
       <c r="D138" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E138" t="s">
         <v>124</v>
@@ -12191,7 +12191,7 @@
         <v>14</v>
       </c>
       <c r="D139" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E139" t="s">
         <v>124</v>
@@ -12245,7 +12245,7 @@
         <v>14</v>
       </c>
       <c r="D140" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E140" t="s">
         <v>124</v>
@@ -12299,7 +12299,7 @@
         <v>14</v>
       </c>
       <c r="D141" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E141" t="s">
         <v>124</v>
@@ -12353,7 +12353,7 @@
         <v>14</v>
       </c>
       <c r="D142" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E142" t="s">
         <v>124</v>
@@ -12407,7 +12407,7 @@
         <v>14</v>
       </c>
       <c r="D143" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E143" t="s">
         <v>124</v>
@@ -12461,7 +12461,7 @@
         <v>14</v>
       </c>
       <c r="D144" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E144" t="s">
         <v>124</v>
@@ -12515,7 +12515,7 @@
         <v>14</v>
       </c>
       <c r="D145" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E145" t="s">
         <v>124</v>
@@ -13433,7 +13433,7 @@
         <v>1</v>
       </c>
       <c r="D162" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E162" t="s">
         <v>124</v>
@@ -13457,7 +13457,7 @@
       </c>
       <c r="K162" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</f>
-        <v>yjl244_WT_sgA_R1_sense_nodsb</v>
+        <v>yjl244_WT_sgA_R1_sense_noDSB</v>
       </c>
       <c r="L162" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</f>
@@ -13473,7 +13473,7 @@
       </c>
       <c r="O162" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl244_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl244_WT_sgA_R1_sense_nodsb.tsv --min_length 130 -dsb 67 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl244_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl244_WT_sgA_R1_sense_noDSB.tsv --min_length 130 -dsb 67 --quiet</v>
       </c>
     </row>
     <row r="163" spans="1:15" x14ac:dyDescent="0.25">
@@ -13487,7 +13487,7 @@
         <v>1</v>
       </c>
       <c r="D163" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E163" t="s">
         <v>124</v>
@@ -13511,7 +13511,7 @@
       </c>
       <c r="K163" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</f>
-        <v>yjl245_WT_sgA_R1_branch_nodsb</v>
+        <v>yjl245_WT_sgA_R1_branch_noDSB</v>
       </c>
       <c r="L163" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</f>
@@ -13527,7 +13527,7 @@
       </c>
       <c r="O163" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl245_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl245_WT_sgA_R1_branch_nodsb.tsv --min_length 130 -dsb 67 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl245_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl245_WT_sgA_R1_branch_noDSB.tsv --min_length 130 -dsb 67 --quiet</v>
       </c>
     </row>
     <row r="164" spans="1:15" x14ac:dyDescent="0.25">
@@ -13541,7 +13541,7 @@
         <v>1</v>
       </c>
       <c r="D164" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E164" t="s">
         <v>124</v>
@@ -13565,7 +13565,7 @@
       </c>
       <c r="K164" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</f>
-        <v>yjl246_WT_sgA_R1_cmv_nodsb</v>
+        <v>yjl246_WT_sgA_R1_cmv_noDSB</v>
       </c>
       <c r="L164" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</f>
@@ -13581,7 +13581,7 @@
       </c>
       <c r="O164" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl246_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl246_WT_sgA_R1_cmv_nodsb.tsv --min_length 130 -dsb 67 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl246_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl246_WT_sgA_R1_cmv_noDSB.tsv --min_length 130 -dsb 67 --quiet</v>
       </c>
     </row>
     <row r="165" spans="1:15" x14ac:dyDescent="0.25">
@@ -13595,7 +13595,7 @@
         <v>14</v>
       </c>
       <c r="D165" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E165" t="s">
         <v>124</v>
@@ -13619,7 +13619,7 @@
       </c>
       <c r="K165" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</f>
-        <v>yjl281_KO_sgA_R1_sense_nodsb</v>
+        <v>yjl281_KO_sgA_R1_sense_noDSB</v>
       </c>
       <c r="L165" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</f>
@@ -13635,7 +13635,7 @@
       </c>
       <c r="O165" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl281_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl281_KO_sgA_R1_sense_nodsb.tsv --min_length 130 -dsb 67 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl281_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl281_KO_sgA_R1_sense_noDSB.tsv --min_length 130 -dsb 67 --quiet</v>
       </c>
     </row>
     <row r="166" spans="1:15" x14ac:dyDescent="0.25">
@@ -13649,7 +13649,7 @@
         <v>14</v>
       </c>
       <c r="D166" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E166" t="s">
         <v>124</v>
@@ -13673,7 +13673,7 @@
       </c>
       <c r="K166" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</f>
-        <v>yjl282_KO_sgA_R1_branch_nodsb</v>
+        <v>yjl282_KO_sgA_R1_branch_noDSB</v>
       </c>
       <c r="L166" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</f>
@@ -13689,7 +13689,7 @@
       </c>
       <c r="O166" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl282_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl282_KO_sgA_R1_branch_nodsb.tsv --min_length 130 -dsb 67 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl282_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl282_KO_sgA_R1_branch_noDSB.tsv --min_length 130 -dsb 67 --quiet</v>
       </c>
     </row>
     <row r="167" spans="1:15" x14ac:dyDescent="0.25">
@@ -13703,7 +13703,7 @@
         <v>14</v>
       </c>
       <c r="D167" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E167" t="s">
         <v>124</v>
@@ -13727,7 +13727,7 @@
       </c>
       <c r="K167" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</f>
-        <v>yjl283_KO_sgA_R1_cmv_nodsb</v>
+        <v>yjl283_KO_sgA_R1_cmv_noDSB</v>
       </c>
       <c r="L167" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</f>
@@ -13743,7 +13743,7 @@
       </c>
       <c r="O167" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl283_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl283_KO_sgA_R1_cmv_nodsb.tsv --min_length 130 -dsb 67 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl283_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl283_KO_sgA_R1_cmv_noDSB.tsv --min_length 130 -dsb 67 --quiet</v>
       </c>
     </row>
     <row r="168" spans="1:15" x14ac:dyDescent="0.25">
@@ -13757,7 +13757,7 @@
         <v>1</v>
       </c>
       <c r="D168" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E168" t="s">
         <v>124</v>
@@ -13781,7 +13781,7 @@
       </c>
       <c r="K168" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</f>
-        <v>yjl244_WT_sgB_R2_sense_nodsb</v>
+        <v>yjl244_WT_sgB_R2_sense_noDSB</v>
       </c>
       <c r="L168" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</f>
@@ -13797,7 +13797,7 @@
       </c>
       <c r="O168" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl244_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl244_WT_sgB_R2_sense_nodsb.tsv --min_length 130 -dsb 46 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl244_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl244_WT_sgB_R2_sense_noDSB.tsv --min_length 130 -dsb 46 --quiet</v>
       </c>
     </row>
     <row r="169" spans="1:15" x14ac:dyDescent="0.25">
@@ -13811,7 +13811,7 @@
         <v>1</v>
       </c>
       <c r="D169" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E169" t="s">
         <v>124</v>
@@ -13835,7 +13835,7 @@
       </c>
       <c r="K169" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</f>
-        <v>yjl245_WT_sgB_R2_branch_nodsb</v>
+        <v>yjl245_WT_sgB_R2_branch_noDSB</v>
       </c>
       <c r="L169" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</f>
@@ -13851,7 +13851,7 @@
       </c>
       <c r="O169" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl245_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl245_WT_sgB_R2_branch_nodsb.tsv --min_length 130 -dsb 46 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl245_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl245_WT_sgB_R2_branch_noDSB.tsv --min_length 130 -dsb 46 --quiet</v>
       </c>
     </row>
     <row r="170" spans="1:15" x14ac:dyDescent="0.25">
@@ -13865,7 +13865,7 @@
         <v>1</v>
       </c>
       <c r="D170" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E170" t="s">
         <v>124</v>
@@ -13889,7 +13889,7 @@
       </c>
       <c r="K170" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</f>
-        <v>yjl246_WT_sgB_R2_cmv_nodsb</v>
+        <v>yjl246_WT_sgB_R2_cmv_noDSB</v>
       </c>
       <c r="L170" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</f>
@@ -13905,7 +13905,7 @@
       </c>
       <c r="O170" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl246_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl246_WT_sgB_R2_cmv_nodsb.tsv --min_length 130 -dsb 46 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl246_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl246_WT_sgB_R2_cmv_noDSB.tsv --min_length 130 -dsb 46 --quiet</v>
       </c>
     </row>
     <row r="171" spans="1:15" x14ac:dyDescent="0.25">
@@ -13919,7 +13919,7 @@
         <v>14</v>
       </c>
       <c r="D171" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E171" t="s">
         <v>124</v>
@@ -13943,7 +13943,7 @@
       </c>
       <c r="K171" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</f>
-        <v>yjl281_KO_sgB_R2_sense_nodsb</v>
+        <v>yjl281_KO_sgB_R2_sense_noDSB</v>
       </c>
       <c r="L171" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</f>
@@ -13959,7 +13959,7 @@
       </c>
       <c r="O171" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl281_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl281_KO_sgB_R2_sense_nodsb.tsv --min_length 130 -dsb 46 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl281_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl281_KO_sgB_R2_sense_noDSB.tsv --min_length 130 -dsb 46 --quiet</v>
       </c>
     </row>
     <row r="172" spans="1:15" x14ac:dyDescent="0.25">
@@ -13973,7 +13973,7 @@
         <v>14</v>
       </c>
       <c r="D172" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E172" t="s">
         <v>124</v>
@@ -13997,7 +13997,7 @@
       </c>
       <c r="K172" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</f>
-        <v>yjl282_KO_sgB_R2_branch_nodsb</v>
+        <v>yjl282_KO_sgB_R2_branch_noDSB</v>
       </c>
       <c r="L172" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</f>
@@ -14013,7 +14013,7 @@
       </c>
       <c r="O172" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl282_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl282_KO_sgB_R2_branch_nodsb.tsv --min_length 130 -dsb 46 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl282_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl282_KO_sgB_R2_branch_noDSB.tsv --min_length 130 -dsb 46 --quiet</v>
       </c>
     </row>
     <row r="173" spans="1:15" x14ac:dyDescent="0.25">
@@ -14027,7 +14027,7 @@
         <v>14</v>
       </c>
       <c r="D173" t="s">
-        <v>141</v>
+        <v>188</v>
       </c>
       <c r="E173" t="s">
         <v>124</v>
@@ -14051,7 +14051,7 @@
       </c>
       <c r="K173" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</f>
-        <v>yjl283_KO_sgB_R2_cmv_nodsb</v>
+        <v>yjl283_KO_sgB_R2_cmv_noDSB</v>
       </c>
       <c r="L173" t="str">
         <f>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</f>
@@ -14067,12 +14067,12 @@
       </c>
       <c r="O173" t="str">
         <f>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</f>
-        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl283_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl283_KO_sgB_R2_cmv_nodsb.tsv --min_length 130 -dsb 46 --quiet</v>
+        <v>python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl283_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl283_KO_sgB_R2_cmv_noDSB.tsv --min_length 130 -dsb 46 --quiet</v>
       </c>
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B175" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.25">
@@ -14238,18 +14238,18 @@
 python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl94_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_splicing.fa -o libraries_2/yjl94_WT_sgCD_R2_splicing.tsv --min_length 50 -dsb 47 --quiet
 python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl95_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_splicing.fa -o libraries_2/yjl95_WT_sgCD_R2_splicing.tsv --min_length 50 -dsb 47 --quiet
 python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl96_anti_R2_2DSBs.sam -ref ref_seq/2DSBanti_R2_splicing.fa -o libraries_2/yjl96_WT_sgCD_R2_splicing.tsv --min_length 50 -dsb 47 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl244_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl244_WT_sgA_R1_sense_nodsb.tsv --min_length 130 -dsb 67 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl245_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl245_WT_sgA_R1_branch_nodsb.tsv --min_length 130 -dsb 67 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl246_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl246_WT_sgA_R1_cmv_nodsb.tsv --min_length 130 -dsb 67 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl281_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl281_KO_sgA_R1_sense_nodsb.tsv --min_length 130 -dsb 67 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl282_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl282_KO_sgA_R1_branch_nodsb.tsv --min_length 130 -dsb 67 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl283_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl283_KO_sgA_R1_cmv_nodsb.tsv --min_length 130 -dsb 67 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl244_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl244_WT_sgB_R2_sense_nodsb.tsv --min_length 130 -dsb 46 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl245_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl245_WT_sgB_R2_branch_nodsb.tsv --min_length 130 -dsb 46 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl246_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl246_WT_sgB_R2_cmv_nodsb.tsv --min_length 130 -dsb 46 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl281_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl281_KO_sgB_R2_sense_nodsb.tsv --min_length 130 -dsb 46 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl282_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl282_KO_sgB_R2_branch_nodsb.tsv --min_length 130 -dsb 46 --quiet
-python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl283_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl283_KO_sgB_R2_cmv_nodsb.tsv --min_length 130 -dsb 46 --quiet</v>
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl244_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl244_WT_sgA_R1_sense_noDSB.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl245_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl245_WT_sgA_R1_branch_noDSB.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl246_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl246_WT_sgA_R1_cmv_noDSB.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl281_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_sense.fa -o libraries_2/yjl281_KO_sgA_R1_sense_noDSB.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl282_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_branch.fa -o libraries_2/yjl282_KO_sgA_R1_branch_noDSB.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl283_NHEJ_hg39_R1.sam -ref ref_seq/1DSB_R1_cmv.fa -o libraries_2/yjl283_KO_sgA_R1_cmv_noDSB.tsv --min_length 130 -dsb 67 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl244_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl244_WT_sgB_R2_sense_noDSB.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl245_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl245_WT_sgB_R2_branch_noDSB.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl246_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl246_WT_sgB_R2_cmv_noDSB.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl281_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_sense.fa -o libraries_2/yjl281_KO_sgB_R2_sense_noDSB.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl282_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_branch.fa -o libraries_2/yjl282_KO_sgB_R2_branch_noDSB.tsv --min_length 130 -dsb 46 --quiet
+python 1_process_nhej/filter_nhej.py -sam libraries_1/yjl283_NHEJ_hg42_R2.sam -ref ref_seq/1DSB_R2_cmv.fa -o libraries_2/yjl283_KO_sgB_R2_cmv_noDSB.tsv --min_length 130 -dsb 46 --quiet</v>
       </c>
     </row>
   </sheetData>
@@ -14266,8 +14266,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8D704B5-D01A-4D17-9252-416EA08BC871}">
   <dimension ref="A1:S59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H46" workbookViewId="0">
-      <selection activeCell="H59" sqref="H59"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14342,7 +14342,7 @@
         <v>100</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
@@ -17471,7 +17471,7 @@
         <v>92</v>
       </c>
       <c r="M44" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
@@ -17484,7 +17484,7 @@
       </c>
       <c r="C45" t="str">
         <f ca="1">OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D45" t="str">
         <f ca="1">OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17516,7 +17516,7 @@
       </c>
       <c r="K45" t="str">
         <f ca="1">OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>yjl244_WT_sgA_R1_sense_nodsb</v>
+        <v>yjl244_WT_sgA_R1_sense_noDSB</v>
       </c>
       <c r="L45">
         <f ca="1">OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17524,7 +17524,7 @@
       </c>
       <c r="M45" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl244_WT_sgA_R1_sense_nodsb.tsv  --total_reads 10005232 -o libraries_3/WT_sgA_R1_sense_nodsb.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl244_WT_sgA_R1_sense_noDSB.tsv  --total_reads 10005232 -o libraries_3/WT_sgA_R1_sense_nodsb.tsv --quiet </v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
@@ -17537,7 +17537,7 @@
       </c>
       <c r="C46" t="str">
         <f ca="1">OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D46" t="str">
         <f ca="1">OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17569,7 +17569,7 @@
       </c>
       <c r="K46" t="str">
         <f ca="1">OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>yjl245_WT_sgA_R1_branch_nodsb</v>
+        <v>yjl245_WT_sgA_R1_branch_noDSB</v>
       </c>
       <c r="L46">
         <f ca="1">OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17577,7 +17577,7 @@
       </c>
       <c r="M46" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl245_WT_sgA_R1_branch_nodsb.tsv  --total_reads 12898941 -o libraries_3/WT_sgA_R1_branch_nodsb.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl245_WT_sgA_R1_branch_noDSB.tsv  --total_reads 12898941 -o libraries_3/WT_sgA_R1_branch_nodsb.tsv --quiet </v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
@@ -17590,7 +17590,7 @@
       </c>
       <c r="C47" t="str">
         <f ca="1">OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D47" t="str">
         <f ca="1">OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17622,7 +17622,7 @@
       </c>
       <c r="K47" t="str">
         <f ca="1">OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>yjl246_WT_sgA_R1_cmv_nodsb</v>
+        <v>yjl246_WT_sgA_R1_cmv_noDSB</v>
       </c>
       <c r="L47">
         <f ca="1">OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17630,7 +17630,7 @@
       </c>
       <c r="M47" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl246_WT_sgA_R1_cmv_nodsb.tsv  --total_reads 10217401 -o libraries_3/WT_sgA_R1_cmv_nodsb.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl246_WT_sgA_R1_cmv_noDSB.tsv  --total_reads 10217401 -o libraries_3/WT_sgA_R1_cmv_nodsb.tsv --quiet </v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
@@ -17643,7 +17643,7 @@
       </c>
       <c r="C48" t="str">
         <f ca="1">OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D48" t="str">
         <f ca="1">OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17675,7 +17675,7 @@
       </c>
       <c r="K48" t="str">
         <f ca="1">OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>yjl281_KO_sgA_R1_sense_nodsb</v>
+        <v>yjl281_KO_sgA_R1_sense_noDSB</v>
       </c>
       <c r="L48">
         <f ca="1">OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17683,7 +17683,7 @@
       </c>
       <c r="M48" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl281_KO_sgA_R1_sense_nodsb.tsv  --total_reads 7424148 -o libraries_3/KO_sgA_R1_sense_nodsb.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl281_KO_sgA_R1_sense_noDSB.tsv  --total_reads 7424148 -o libraries_3/KO_sgA_R1_sense_nodsb.tsv --quiet </v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
@@ -17696,7 +17696,7 @@
       </c>
       <c r="C49" t="str">
         <f ca="1">OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D49" t="str">
         <f ca="1">OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17728,7 +17728,7 @@
       </c>
       <c r="K49" t="str">
         <f ca="1">OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>yjl282_KO_sgA_R1_branch_nodsb</v>
+        <v>yjl282_KO_sgA_R1_branch_noDSB</v>
       </c>
       <c r="L49">
         <f ca="1">OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17736,7 +17736,7 @@
       </c>
       <c r="M49" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl282_KO_sgA_R1_branch_nodsb.tsv  --total_reads 10190833 -o libraries_3/KO_sgA_R1_branch_nodsb.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl282_KO_sgA_R1_branch_noDSB.tsv  --total_reads 10190833 -o libraries_3/KO_sgA_R1_branch_nodsb.tsv --quiet </v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
@@ -17749,7 +17749,7 @@
       </c>
       <c r="C50" t="str">
         <f ca="1">OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D50" t="str">
         <f ca="1">OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17781,7 +17781,7 @@
       </c>
       <c r="K50" t="str">
         <f ca="1">OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>yjl283_KO_sgA_R1_cmv_nodsb</v>
+        <v>yjl283_KO_sgA_R1_cmv_noDSB</v>
       </c>
       <c r="L50">
         <f ca="1">OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17789,7 +17789,7 @@
       </c>
       <c r="M50" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl283_KO_sgA_R1_cmv_nodsb.tsv  --total_reads 7763439 -o libraries_3/KO_sgA_R1_cmv_nodsb.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl283_KO_sgA_R1_cmv_noDSB.tsv  --total_reads 7763439 -o libraries_3/KO_sgA_R1_cmv_nodsb.tsv --quiet </v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
@@ -17802,7 +17802,7 @@
       </c>
       <c r="C51" t="str">
         <f ca="1">OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D51" t="str">
         <f ca="1">OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17834,7 +17834,7 @@
       </c>
       <c r="K51" t="str">
         <f ca="1">OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>yjl244_WT_sgB_R2_sense_nodsb</v>
+        <v>yjl244_WT_sgB_R2_sense_noDSB</v>
       </c>
       <c r="L51">
         <f ca="1">OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17842,7 +17842,7 @@
       </c>
       <c r="M51" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl244_WT_sgB_R2_sense_nodsb.tsv  --total_reads 9354510 -o libraries_3/WT_sgB_R2_sense_nodsb.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl244_WT_sgB_R2_sense_noDSB.tsv  --total_reads 9354510 -o libraries_3/WT_sgB_R2_sense_nodsb.tsv --quiet </v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -17855,7 +17855,7 @@
       </c>
       <c r="C52" t="str">
         <f ca="1">OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D52" t="str">
         <f ca="1">OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17887,7 +17887,7 @@
       </c>
       <c r="K52" t="str">
         <f ca="1">OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>yjl245_WT_sgB_R2_branch_nodsb</v>
+        <v>yjl245_WT_sgB_R2_branch_noDSB</v>
       </c>
       <c r="L52">
         <f ca="1">OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17895,7 +17895,7 @@
       </c>
       <c r="M52" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl245_WT_sgB_R2_branch_nodsb.tsv  --total_reads 12461219 -o libraries_3/WT_sgB_R2_branch_nodsb.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl245_WT_sgB_R2_branch_noDSB.tsv  --total_reads 12461219 -o libraries_3/WT_sgB_R2_branch_nodsb.tsv --quiet </v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.25">
@@ -17908,7 +17908,7 @@
       </c>
       <c r="C53" t="str">
         <f ca="1">OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D53" t="str">
         <f ca="1">OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17940,7 +17940,7 @@
       </c>
       <c r="K53" t="str">
         <f ca="1">OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>yjl246_WT_sgB_R2_cmv_nodsb</v>
+        <v>yjl246_WT_sgB_R2_cmv_noDSB</v>
       </c>
       <c r="L53">
         <f ca="1">OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17948,7 +17948,7 @@
       </c>
       <c r="M53" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl246_WT_sgB_R2_cmv_nodsb.tsv  --total_reads 9853052 -o libraries_3/WT_sgB_R2_cmv_nodsb.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl246_WT_sgB_R2_cmv_noDSB.tsv  --total_reads 9853052 -o libraries_3/WT_sgB_R2_cmv_nodsb.tsv --quiet </v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
@@ -17961,7 +17961,7 @@
       </c>
       <c r="C54" t="str">
         <f ca="1">OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D54" t="str">
         <f ca="1">OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -17993,7 +17993,7 @@
       </c>
       <c r="K54" t="str">
         <f ca="1">OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>yjl281_KO_sgB_R2_sense_nodsb</v>
+        <v>yjl281_KO_sgB_R2_sense_noDSB</v>
       </c>
       <c r="L54">
         <f ca="1">OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -18001,7 +18001,7 @@
       </c>
       <c r="M54" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl281_KO_sgB_R2_sense_nodsb.tsv  --total_reads 7181166 -o libraries_3/KO_sgB_R2_sense_nodsb.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl281_KO_sgB_R2_sense_noDSB.tsv  --total_reads 7181166 -o libraries_3/KO_sgB_R2_sense_nodsb.tsv --quiet </v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
@@ -18014,7 +18014,7 @@
       </c>
       <c r="C55" t="str">
         <f ca="1">OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D55" t="str">
         <f ca="1">OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -18046,7 +18046,7 @@
       </c>
       <c r="K55" t="str">
         <f ca="1">OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>yjl282_KO_sgB_R2_branch_nodsb</v>
+        <v>yjl282_KO_sgB_R2_branch_noDSB</v>
       </c>
       <c r="L55">
         <f ca="1">OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -18054,7 +18054,7 @@
       </c>
       <c r="M55" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl282_KO_sgB_R2_branch_nodsb.tsv  --total_reads 10027116 -o libraries_3/KO_sgB_R2_branch_nodsb.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl282_KO_sgB_R2_branch_noDSB.tsv  --total_reads 10027116 -o libraries_3/KO_sgB_R2_branch_nodsb.tsv --quiet </v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.25">
@@ -18067,7 +18067,7 @@
       </c>
       <c r="C56" t="str">
         <f ca="1">OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D56" t="str">
         <f ca="1">OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -18099,7 +18099,7 @@
       </c>
       <c r="K56" t="str">
         <f ca="1">OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
-        <v>yjl283_KO_sgB_R2_cmv_nodsb</v>
+        <v>yjl283_KO_sgB_R2_cmv_noDSB</v>
       </c>
       <c r="L56">
         <f ca="1">OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</f>
@@ -18107,12 +18107,12 @@
       </c>
       <c r="M56" t="str">
         <f ca="1">_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</f>
-        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl283_KO_sgB_R2_cmv_nodsb.tsv  --total_reads 7622513 -o libraries_3/KO_sgB_R2_cmv_nodsb.tsv --quiet </v>
+        <v xml:space="preserve">python 1_process_nhej/combine_repeats.py -i libraries_2/yjl283_KO_sgB_R2_cmv_noDSB.tsv  --total_reads 7622513 -o libraries_3/KO_sgB_R2_cmv_nodsb.tsv --quiet </v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H58" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -18158,18 +18158,18 @@
 python 1_process_nhej/combine_repeats.py -i libraries_2/yjl93_WT_sgCD_R1_splicing.tsv libraries_2/yjl94_WT_sgCD_R1_splicing.tsv libraries_2/yjl95_WT_sgCD_R1_splicing.tsv libraries_2/yjl96_WT_sgCD_R1_splicing.tsv --total_reads 9334492 9142001 8497185 8346242 -o libraries_3/WT_sgCD_R1_splicing.tsv --quiet 
 python 1_process_nhej/combine_repeats.py -i libraries_2/yjl89_WT_sgCD_R2_antisense.tsv libraries_2/yjl90_WT_sgCD_R2_antisense.tsv libraries_2/yjl91_WT_sgCD_R2_antisense.tsv libraries_2/yjl92_WT_sgCD_R2_antisense.tsv --total_reads 7813781 7486736 8114856 6586577 -o libraries_3/WT_sgCD_R2_antisense.tsv --quiet 
 python 1_process_nhej/combine_repeats.py -i libraries_2/yjl93_WT_sgCD_R2_splicing.tsv libraries_2/yjl94_WT_sgCD_R2_splicing.tsv libraries_2/yjl95_WT_sgCD_R2_splicing.tsv libraries_2/yjl96_WT_sgCD_R2_splicing.tsv --total_reads 9334492 9142001 8497185 8346242 -o libraries_3/WT_sgCD_R2_splicing.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl244_WT_sgA_R1_sense_nodsb.tsv  --total_reads 10005232 -o libraries_3/WT_sgA_R1_sense_nodsb.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl245_WT_sgA_R1_branch_nodsb.tsv  --total_reads 12898941 -o libraries_3/WT_sgA_R1_branch_nodsb.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl246_WT_sgA_R1_cmv_nodsb.tsv  --total_reads 10217401 -o libraries_3/WT_sgA_R1_cmv_nodsb.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl281_KO_sgA_R1_sense_nodsb.tsv  --total_reads 7424148 -o libraries_3/KO_sgA_R1_sense_nodsb.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl282_KO_sgA_R1_branch_nodsb.tsv  --total_reads 10190833 -o libraries_3/KO_sgA_R1_branch_nodsb.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl283_KO_sgA_R1_cmv_nodsb.tsv  --total_reads 7763439 -o libraries_3/KO_sgA_R1_cmv_nodsb.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl244_WT_sgB_R2_sense_nodsb.tsv  --total_reads 9354510 -o libraries_3/WT_sgB_R2_sense_nodsb.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl245_WT_sgB_R2_branch_nodsb.tsv  --total_reads 12461219 -o libraries_3/WT_sgB_R2_branch_nodsb.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl246_WT_sgB_R2_cmv_nodsb.tsv  --total_reads 9853052 -o libraries_3/WT_sgB_R2_cmv_nodsb.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl281_KO_sgB_R2_sense_nodsb.tsv  --total_reads 7181166 -o libraries_3/KO_sgB_R2_sense_nodsb.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl282_KO_sgB_R2_branch_nodsb.tsv  --total_reads 10027116 -o libraries_3/KO_sgB_R2_branch_nodsb.tsv --quiet 
-python 1_process_nhej/combine_repeats.py -i libraries_2/yjl283_KO_sgB_R2_cmv_nodsb.tsv  --total_reads 7622513 -o libraries_3/KO_sgB_R2_cmv_nodsb.tsv --quiet </v>
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl244_WT_sgA_R1_sense_noDSB.tsv  --total_reads 10005232 -o libraries_3/WT_sgA_R1_sense_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl245_WT_sgA_R1_branch_noDSB.tsv  --total_reads 12898941 -o libraries_3/WT_sgA_R1_branch_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl246_WT_sgA_R1_cmv_noDSB.tsv  --total_reads 10217401 -o libraries_3/WT_sgA_R1_cmv_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl281_KO_sgA_R1_sense_noDSB.tsv  --total_reads 7424148 -o libraries_3/KO_sgA_R1_sense_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl282_KO_sgA_R1_branch_noDSB.tsv  --total_reads 10190833 -o libraries_3/KO_sgA_R1_branch_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl283_KO_sgA_R1_cmv_noDSB.tsv  --total_reads 7763439 -o libraries_3/KO_sgA_R1_cmv_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl244_WT_sgB_R2_sense_noDSB.tsv  --total_reads 9354510 -o libraries_3/WT_sgB_R2_sense_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl245_WT_sgB_R2_branch_noDSB.tsv  --total_reads 12461219 -o libraries_3/WT_sgB_R2_branch_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl246_WT_sgB_R2_cmv_noDSB.tsv  --total_reads 9853052 -o libraries_3/WT_sgB_R2_cmv_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl281_KO_sgB_R2_sense_noDSB.tsv  --total_reads 7181166 -o libraries_3/KO_sgB_R2_sense_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl282_KO_sgB_R2_branch_noDSB.tsv  --total_reads 10027116 -o libraries_3/KO_sgB_R2_branch_nodsb.tsv --quiet 
+python 1_process_nhej/combine_repeats.py -i libraries_2/yjl283_KO_sgB_R2_cmv_noDSB.tsv  --total_reads 7622513 -o libraries_3/KO_sgB_R2_cmv_nodsb.tsv --quiet </v>
       </c>
     </row>
   </sheetData>
@@ -18187,8 +18187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7FB6E33-93C4-4971-BF44-23A0F65AADA0}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+    <sheetView topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18226,7 +18226,7 @@
         <v>102</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>82</v>
@@ -20550,7 +20550,7 @@
         <v>102</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>82</v>
@@ -20584,7 +20584,7 @@
       </c>
       <c r="C44" t="str">
         <f ca="1">OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D44" t="str">
         <f ca="1">OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -20624,7 +20624,7 @@
       </c>
       <c r="M44" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_sense_nodsb.tsv -o libraries_4/WT_sgA_R1_sense_nodsb -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment sense --subst_type without --control nodsb</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_sense_nodsb.tsv -o libraries_4/WT_sgA_R1_sense_nodsb -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment sense --subst_type without --control noDSB</v>
       </c>
       <c r="N44" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</f>
@@ -20641,7 +20641,7 @@
       </c>
       <c r="C45" t="str">
         <f ca="1">OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D45" t="str">
         <f ca="1">OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -20681,7 +20681,7 @@
       </c>
       <c r="M45" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_branch_nodsb.tsv -o libraries_4/WT_sgA_R1_branch_nodsb -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment branch --subst_type without --control nodsb</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_branch_nodsb.tsv -o libraries_4/WT_sgA_R1_branch_nodsb -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment branch --subst_type without --control noDSB</v>
       </c>
       <c r="N45" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</f>
@@ -20698,7 +20698,7 @@
       </c>
       <c r="C46" t="str">
         <f ca="1">OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D46" t="str">
         <f ca="1">OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -20738,7 +20738,7 @@
       </c>
       <c r="M46" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_cmv_nodsb.tsv -o libraries_4/WT_sgA_R1_cmv_nodsb -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment cmv --subst_type without --control nodsb</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_cmv_nodsb.tsv -o libraries_4/WT_sgA_R1_cmv_nodsb -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment cmv --subst_type without --control noDSB</v>
       </c>
       <c r="N46" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</f>
@@ -20755,7 +20755,7 @@
       </c>
       <c r="C47" t="str">
         <f ca="1">OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D47" t="str">
         <f ca="1">OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -20795,7 +20795,7 @@
       </c>
       <c r="M47" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_sense_nodsb.tsv -o libraries_4/KO_sgA_R1_sense_nodsb -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment sense --subst_type without --control nodsb</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_sense_nodsb.tsv -o libraries_4/KO_sgA_R1_sense_nodsb -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment sense --subst_type without --control noDSB</v>
       </c>
       <c r="N47" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</f>
@@ -20812,7 +20812,7 @@
       </c>
       <c r="C48" t="str">
         <f ca="1">OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D48" t="str">
         <f ca="1">OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -20852,7 +20852,7 @@
       </c>
       <c r="M48" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_branch_nodsb.tsv -o libraries_4/KO_sgA_R1_branch_nodsb -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment branch --subst_type without --control nodsb</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_branch_nodsb.tsv -o libraries_4/KO_sgA_R1_branch_nodsb -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment branch --subst_type without --control noDSB</v>
       </c>
       <c r="N48" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</f>
@@ -20869,7 +20869,7 @@
       </c>
       <c r="C49" t="str">
         <f ca="1">OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D49" t="str">
         <f ca="1">OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -20909,7 +20909,7 @@
       </c>
       <c r="M49" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_cmv_nodsb.tsv -o libraries_4/KO_sgA_R1_cmv_nodsb -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment cmv --subst_type without --control nodsb</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_cmv_nodsb.tsv -o libraries_4/KO_sgA_R1_cmv_nodsb -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment cmv --subst_type without --control noDSB</v>
       </c>
       <c r="N49" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</f>
@@ -20926,7 +20926,7 @@
       </c>
       <c r="C50" t="str">
         <f ca="1">OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D50" t="str">
         <f ca="1">OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -20966,7 +20966,7 @@
       </c>
       <c r="M50" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_sense_nodsb.tsv -o libraries_4/WT_sgB_R2_sense_nodsb -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment sense --subst_type without --control nodsb</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_sense_nodsb.tsv -o libraries_4/WT_sgB_R2_sense_nodsb -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment sense --subst_type without --control noDSB</v>
       </c>
       <c r="N50" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</f>
@@ -20983,7 +20983,7 @@
       </c>
       <c r="C51" t="str">
         <f ca="1">OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D51" t="str">
         <f ca="1">OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -21023,7 +21023,7 @@
       </c>
       <c r="M51" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_branch_nodsb.tsv -o libraries_4/WT_sgB_R2_branch_nodsb -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment branch --subst_type without --control nodsb</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_branch_nodsb.tsv -o libraries_4/WT_sgB_R2_branch_nodsb -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment branch --subst_type without --control noDSB</v>
       </c>
       <c r="N51" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</f>
@@ -21040,7 +21040,7 @@
       </c>
       <c r="C52" t="str">
         <f ca="1">OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D52" t="str">
         <f ca="1">OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -21080,7 +21080,7 @@
       </c>
       <c r="M52" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_cmv_nodsb.tsv -o libraries_4/WT_sgB_R2_cmv_nodsb -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment cmv --subst_type without --control nodsb</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_cmv_nodsb.tsv -o libraries_4/WT_sgB_R2_cmv_nodsb -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment cmv --subst_type without --control noDSB</v>
       </c>
       <c r="N52" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</f>
@@ -21097,7 +21097,7 @@
       </c>
       <c r="C53" t="str">
         <f ca="1">OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D53" t="str">
         <f ca="1">OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -21137,7 +21137,7 @@
       </c>
       <c r="M53" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_sense_nodsb.tsv -o libraries_4/KO_sgB_R2_sense_nodsb -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment sense --subst_type without --control nodsb</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_sense_nodsb.tsv -o libraries_4/KO_sgB_R2_sense_nodsb -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment sense --subst_type without --control noDSB</v>
       </c>
       <c r="N53" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</f>
@@ -21154,7 +21154,7 @@
       </c>
       <c r="C54" t="str">
         <f ca="1">OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D54" t="str">
         <f ca="1">OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -21194,7 +21194,7 @@
       </c>
       <c r="M54" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_branch_nodsb.tsv -o libraries_4/KO_sgB_R2_branch_nodsb -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment branch --subst_type without --control nodsb</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_branch_nodsb.tsv -o libraries_4/KO_sgB_R2_branch_nodsb -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment branch --subst_type without --control noDSB</v>
       </c>
       <c r="N54" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</f>
@@ -21211,7 +21211,7 @@
       </c>
       <c r="C55" t="str">
         <f ca="1">OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D55" t="str">
         <f ca="1">OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</f>
@@ -21251,7 +21251,7 @@
       </c>
       <c r="M55" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</f>
-        <v>python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_cmv_nodsb.tsv -o libraries_4/KO_sgB_R2_cmv_nodsb -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment cmv --subst_type without --control nodsb</v>
+        <v>python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_cmv_nodsb.tsv -o libraries_4/KO_sgB_R2_cmv_nodsb -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment cmv --subst_type without --control noDSB</v>
       </c>
       <c r="N55" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</f>
@@ -21260,7 +21260,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -21306,23 +21306,23 @@
 python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R1_splicing.tsv -o libraries_4/WT_sgCD_R1_splicing -ref ref_seq/2DSBanti_R1_splicing.fa -dsb 50 --dsb_type 2a --strand R1 --hguide CD --cell WT --treatment splicing --subst_type without --control none
 python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R2_antisense.tsv -o libraries_4/WT_sgCD_R2_antisense -ref ref_seq/2DSBanti_R2_antisense.fa -dsb 47 --dsb_type 2a --strand R2 --hguide CD --cell WT --treatment antisense --subst_type without --control none
 python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgCD_R2_splicing.tsv -o libraries_4/WT_sgCD_R2_splicing -ref ref_seq/2DSBanti_R2_splicing.fa -dsb 47 --dsb_type 2a --strand R2 --hguide CD --cell WT --treatment splicing --subst_type without --control none
-python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_sense_nodsb.tsv -o libraries_4/WT_sgA_R1_sense_nodsb -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment sense --subst_type without --control nodsb
-python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_branch_nodsb.tsv -o libraries_4/WT_sgA_R1_branch_nodsb -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment branch --subst_type without --control nodsb
-python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_cmv_nodsb.tsv -o libraries_4/WT_sgA_R1_cmv_nodsb -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment cmv --subst_type without --control nodsb
-python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_sense_nodsb.tsv -o libraries_4/KO_sgA_R1_sense_nodsb -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment sense --subst_type without --control nodsb
-python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_branch_nodsb.tsv -o libraries_4/KO_sgA_R1_branch_nodsb -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment branch --subst_type without --control nodsb
-python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_cmv_nodsb.tsv -o libraries_4/KO_sgA_R1_cmv_nodsb -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment cmv --subst_type without --control nodsb
-python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_sense_nodsb.tsv -o libraries_4/WT_sgB_R2_sense_nodsb -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment sense --subst_type without --control nodsb
-python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_branch_nodsb.tsv -o libraries_4/WT_sgB_R2_branch_nodsb -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment branch --subst_type without --control nodsb
-python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_cmv_nodsb.tsv -o libraries_4/WT_sgB_R2_cmv_nodsb -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment cmv --subst_type without --control nodsb
-python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_sense_nodsb.tsv -o libraries_4/KO_sgB_R2_sense_nodsb -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment sense --subst_type without --control nodsb
-python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_branch_nodsb.tsv -o libraries_4/KO_sgB_R2_branch_nodsb -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment branch --subst_type without --control nodsb
-python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_cmv_nodsb.tsv -o libraries_4/KO_sgB_R2_cmv_nodsb -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment cmv --subst_type without --control nodsb</v>
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_sense_nodsb.tsv -o libraries_4/WT_sgA_R1_sense_nodsb -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment sense --subst_type without --control noDSB
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_branch_nodsb.tsv -o libraries_4/WT_sgA_R1_branch_nodsb -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment branch --subst_type without --control noDSB
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgA_R1_cmv_nodsb.tsv -o libraries_4/WT_sgA_R1_cmv_nodsb -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell WT --treatment cmv --subst_type without --control noDSB
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_sense_nodsb.tsv -o libraries_4/KO_sgA_R1_sense_nodsb -ref ref_seq/1DSB_R1_sense.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment sense --subst_type without --control noDSB
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_branch_nodsb.tsv -o libraries_4/KO_sgA_R1_branch_nodsb -ref ref_seq/1DSB_R1_branch.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment branch --subst_type without --control noDSB
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgA_R1_cmv_nodsb.tsv -o libraries_4/KO_sgA_R1_cmv_nodsb -ref ref_seq/1DSB_R1_cmv.fa -dsb 67 --dsb_type 1 --strand R1 --hguide A --cell KO --treatment cmv --subst_type without --control noDSB
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_sense_nodsb.tsv -o libraries_4/WT_sgB_R2_sense_nodsb -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment sense --subst_type without --control noDSB
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_branch_nodsb.tsv -o libraries_4/WT_sgB_R2_branch_nodsb -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment branch --subst_type without --control noDSB
+python 2_graph_processing/make_main_data.py -i libraries_3/WT_sgB_R2_cmv_nodsb.tsv -o libraries_4/WT_sgB_R2_cmv_nodsb -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell WT --treatment cmv --subst_type without --control noDSB
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_sense_nodsb.tsv -o libraries_4/KO_sgB_R2_sense_nodsb -ref ref_seq/1DSB_R2_sense.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment sense --subst_type without --control noDSB
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_branch_nodsb.tsv -o libraries_4/KO_sgB_R2_branch_nodsb -ref ref_seq/1DSB_R2_branch.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment branch --subst_type without --control noDSB
+python 2_graph_processing/make_main_data.py -i libraries_3/KO_sgB_R2_cmv_nodsb.tsv -o libraries_4/KO_sgB_R2_cmv_nodsb -ref ref_seq/1DSB_R2_cmv.fa -dsb 46 --dsb_type 1 --strand R2 --hguide B --cell KO --treatment cmv --subst_type without --control noDSB</v>
       </c>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
@@ -21423,19 +21423,19 @@
         <v>134</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>109</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>110</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>111</v>
@@ -22183,19 +22183,19 @@
         <v>134</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>109</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>110</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>111</v>
@@ -22314,19 +22314,19 @@
         <v>134</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>109</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>110</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>111</v>
@@ -22347,7 +22347,7 @@
       </c>
       <c r="B26" s="6" t="str">
         <f ca="1">OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="C26" s="6" t="str">
         <f ca="1">OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
@@ -22392,7 +22392,7 @@
       </c>
       <c r="B27" s="6" t="str">
         <f ca="1">OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="C27" s="6" t="str">
         <f ca="1">OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
@@ -22437,7 +22437,7 @@
       </c>
       <c r="B28" s="5" t="str">
         <f ca="1">OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="C28" s="5" t="str">
         <f ca="1">OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
@@ -22482,7 +22482,7 @@
       </c>
       <c r="B29" s="5" t="str">
         <f ca="1">OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="C29" s="5" t="str">
         <f ca="1">OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
@@ -22527,7 +22527,7 @@
       </c>
       <c r="B30" s="5" t="str">
         <f ca="1">OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="C30" s="5" t="str">
         <f ca="1">OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
@@ -22572,7 +22572,7 @@
       </c>
       <c r="B31" s="5" t="str">
         <f ca="1">OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="C31" s="5" t="str">
         <f ca="1">OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
@@ -22617,7 +22617,7 @@
       </c>
       <c r="B32" s="5" t="str">
         <f ca="1">OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="C32" s="5" t="str">
         <f ca="1">OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
@@ -22662,7 +22662,7 @@
       </c>
       <c r="B33" s="5" t="str">
         <f ca="1">OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="C33" s="5" t="str">
         <f ca="1">OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</f>
@@ -22703,7 +22703,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -22739,7 +22739,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -22828,7 +22828,7 @@
         <v>102</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>82</v>
@@ -22846,7 +22846,7 @@
         <v>105</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -24989,7 +24989,7 @@
         <v>102</v>
       </c>
       <c r="G43" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H43" t="s">
         <v>82</v>
@@ -25007,7 +25007,7 @@
         <v>105</v>
       </c>
       <c r="M43" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
@@ -25020,7 +25020,7 @@
       </c>
       <c r="C44" t="str">
         <f ca="1">table_3_2[[#This Row],[control]]</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D44" t="str">
         <f ca="1">table_3_2[[#This Row],[ref]]</f>
@@ -25073,7 +25073,7 @@
       </c>
       <c r="C45" t="str">
         <f ca="1">table_3_2[[#This Row],[control]]</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D45" t="str">
         <f ca="1">table_3_2[[#This Row],[ref]]</f>
@@ -25126,7 +25126,7 @@
       </c>
       <c r="C46" t="str">
         <f ca="1">table_3_2[[#This Row],[control]]</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D46" t="str">
         <f ca="1">table_3_2[[#This Row],[ref]]</f>
@@ -25179,7 +25179,7 @@
       </c>
       <c r="C47" t="str">
         <f ca="1">table_3_2[[#This Row],[control]]</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D47" t="str">
         <f ca="1">table_3_2[[#This Row],[ref]]</f>
@@ -25232,7 +25232,7 @@
       </c>
       <c r="C48" t="str">
         <f ca="1">table_3_2[[#This Row],[control]]</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D48" t="str">
         <f ca="1">table_3_2[[#This Row],[ref]]</f>
@@ -25285,7 +25285,7 @@
       </c>
       <c r="C49" t="str">
         <f ca="1">table_3_2[[#This Row],[control]]</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D49" t="str">
         <f ca="1">table_3_2[[#This Row],[ref]]</f>
@@ -25338,7 +25338,7 @@
       </c>
       <c r="C50" t="str">
         <f ca="1">table_3_2[[#This Row],[control]]</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D50" t="str">
         <f ca="1">table_3_2[[#This Row],[ref]]</f>
@@ -25391,7 +25391,7 @@
       </c>
       <c r="C51" t="str">
         <f ca="1">table_3_2[[#This Row],[control]]</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D51" t="str">
         <f ca="1">table_3_2[[#This Row],[ref]]</f>
@@ -25444,7 +25444,7 @@
       </c>
       <c r="C52" t="str">
         <f ca="1">table_3_2[[#This Row],[control]]</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D52" t="str">
         <f ca="1">table_3_2[[#This Row],[ref]]</f>
@@ -25497,7 +25497,7 @@
       </c>
       <c r="C53" t="str">
         <f ca="1">table_3_2[[#This Row],[control]]</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D53" t="str">
         <f ca="1">table_3_2[[#This Row],[ref]]</f>
@@ -25550,7 +25550,7 @@
       </c>
       <c r="C54" t="str">
         <f ca="1">table_3_2[[#This Row],[control]]</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D54" t="str">
         <f ca="1">table_3_2[[#This Row],[ref]]</f>
@@ -25603,7 +25603,7 @@
       </c>
       <c r="C55" t="str">
         <f ca="1">table_3_2[[#This Row],[control]]</f>
-        <v>nodsb</v>
+        <v>noDSB</v>
       </c>
       <c r="D55" t="str">
         <f ca="1">table_3_2[[#This Row],[ref]]</f>
@@ -25648,7 +25648,7 @@
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
@@ -25746,10 +25746,10 @@
   <sheetData>
     <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -25760,7 +25760,7 @@
         <v>87</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>134</v>
@@ -25778,7 +25778,7 @@
         <v>111</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -25842,7 +25842,7 @@
         <v>87</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>134</v>
@@ -25860,7 +25860,7 @@
         <v>111</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -25992,7 +25992,7 @@
         <v>111</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
@@ -26050,7 +26050,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -26121,32 +26121,32 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" t="b">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="D1" t="s">
-        <v>178</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="F1" t="str">
         <f>IF(var_7_common_layout, var_6_layout, "universal")</f>
         <v>universal</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="H1">
         <v>2400</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="J1">
         <v>1800</v>
@@ -26172,7 +26172,7 @@
         <v>102</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>82</v>
@@ -26190,22 +26190,22 @@
         <v>105</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="Q2" s="1" t="s">
         <v>139</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -29505,22 +29505,22 @@
         <v>102</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>139</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
@@ -30260,22 +30260,22 @@
         <v>102</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J62" s="1" t="s">
         <v>139</v>
       </c>
       <c r="K62" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
@@ -30370,7 +30370,7 @@
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update the 3d histogram bat/sh files.
</commit_message>
<xml_diff>
--- a/analyze_nhej/libinfo.xlsx
+++ b/analyze_nhej/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\analyze_nhej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FD9E6BC-FAC3-48E6-8E0E-D2E56755B08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA15ECC6-9EFF-4D4A-94F9-B0B35624F49A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="2" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="6" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1543" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="191">
   <si>
     <t>yjl217</t>
   </si>
@@ -658,6 +658,12 @@
   <si>
     <t>noDSB</t>
   </si>
+  <si>
+    <t>label_type</t>
+  </si>
+  <si>
+    <t>reverse_pos</t>
+  </si>
 </sst>
 </file>
 
@@ -776,7 +782,25 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FFD19645-61C4-4244-A560-0232B787F38C}"/>
   </cellStyles>
-  <dxfs count="200">
+  <dxfs count="204">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -1283,12 +1307,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1978,7 +1996,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}" name="table_1_2" displayName="table_1_2" ref="A1:D108" totalsRowShown="0">
   <autoFilter ref="A1:D108" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}"/>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="199">
+    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="203">
       <calculatedColumnFormula>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{5F63B290-093A-48A3-9AFC-EB2FE27DE630}" name="library"/>
@@ -1990,45 +2008,51 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:M41" totalsRowShown="0" headerRowDxfId="96">
-  <autoFilter ref="A1:M41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
-  <tableColumns count="13">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="95"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="94">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:O41" totalsRowShown="0" headerRowDxfId="100">
+  <autoFilter ref="A1:O41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
+  <tableColumns count="15">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="99"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="98">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="93">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="97">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="92">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="96">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="91">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="95">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="90">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="94">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="89">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="93">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="88">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="92">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="87">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="91">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="86">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="90">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="85">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="89">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="84">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="88">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="83">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
+    <tableColumn id="11" xr3:uid="{1D971CC2-F378-4E62-9759-F7168770AA64}" name="label_type" dataDxfId="5">
+      <calculatedColumnFormula>IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="14" xr3:uid="{8241431B-CE1C-49A4-B13E-77512D442338}" name="reverse_pos" dataDxfId="4">
+      <calculatedColumnFormula>IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="3">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2036,45 +2060,51 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}" name="table_5_2" displayName="table_5_2" ref="A43:M55" totalsRowShown="0">
-  <autoFilter ref="A43:M55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
-  <tableColumns count="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}" name="table_5_2" displayName="table_5_2" ref="A43:O55" totalsRowShown="0">
+  <autoFilter ref="A43:O55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
+  <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
-    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="82">
+    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="87">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="81">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="86">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="80">
+    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="85">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="79">
+    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="84">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="78">
+    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="83">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="77">
+    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="82">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="76">
+    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="81">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="75">
+    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="80">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="74">
+    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="79">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="73">
+    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="78">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="72">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="77">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="71">
-      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</calculatedColumnFormula>
+    <tableColumn id="14" xr3:uid="{F5E6916D-F1BC-48E0-9E73-728C62F32A69}" name="label_type" dataDxfId="2">
+      <calculatedColumnFormula>IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="15" xr3:uid="{EF50F256-FFB6-49D0-8199-D7AB5C783AD5}" name="reverse_pos" dataDxfId="1">
+      <calculatedColumnFormula>IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -2082,36 +2112,36 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="76">
   <autoFilter ref="A3:I4" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="69"/>
-    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="68">
+    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="75"/>
+    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="74">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="67">
+    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="73">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="66">
+    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="72">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="65">
+    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="71">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 12 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="33" xr3:uid="{8FF7E83A-9135-4A64-965C-48368A6C0367}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="64">
+    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="70">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="63">
+    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="69">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="62">
+    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="68">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2120,32 +2150,32 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="61">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="67">
   <autoFilter ref="A7:I9" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="60"/>
-    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="59">
+    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="66"/>
+    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="65">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="58">
+    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="64">
       <calculatedColumnFormula>IF(table_6_4[[#This Row],[hguide]]="A",NA(), IF(var_6_layout = "universal", "1 1 1 1 1 1", NA()))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="57">
+    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="63">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="56">
+    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="62">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" xr3:uid="{5BD83012-469D-4202-9584-AA182CDF11F9}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="55">
+    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="61">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="54">
+    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="60">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="53">
+    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="59">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2154,36 +2184,36 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="52" headerRowBorderDxfId="51" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="58" headerRowBorderDxfId="57" tableBorderDxfId="56">
   <autoFilter ref="A12:I13" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0F421990-E775-4F35-92AF-6BA19E0E8AEE}" name="index"/>
-    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="49">
+    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="55">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="48">
+    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="54">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0,4, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="47">
+    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="53">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="46">
+    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="52">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{E0783723-9246-4BF6-A5DA-E000EA1E5E87}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="45">
+    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="51">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="44">
+    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="50">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="43">
+    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="49">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2192,44 +2222,44 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:R42" totalsRowShown="0" headerRowDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:R42" totalsRowShown="0" headerRowDxfId="48">
   <autoFilter ref="A2:R42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="18">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="41"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="40">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="47"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="46">
       <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="39">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="45">
       <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="38">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="44">
       <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="37">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="43">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="36">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="42">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="35">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="41">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="34">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="40">
       <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="33">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="39">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="32">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="38">
       <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="31">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="37">
       <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="30">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="36">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="29">
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="35">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
       OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
       IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
@@ -2241,19 +2271,19 @@
       )
   )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="28">
+    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="34">
       <calculatedColumnFormula>AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="27">
+    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="33">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", " --range_x -12 13 --range_y -22 22 ", IF(table_7_1[[#This Row],[hguide]]="CD", " --range_x -12 13 --range_y -18 25 ", IF(table_7_1[[#This Row],[hguide]]="A", " --range_x -12 13 --range_y -22 20 ", IF(table_7_1[[#This Row],[hguide]]="B", " --range_x -12 13 --range_y -20 16 ", NA())))), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{891739FF-B093-4EE5-A0A2-20948C58CB96}" name="universal_layout_legend_pos_x" dataDxfId="26">
+    <tableColumn id="17" xr3:uid="{891739FF-B093-4EE5-A0A2-20948C58CB96}" name="universal_layout_legend_pos_x" dataDxfId="32">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 12, IF(table_7_1[[#This Row],[hguide]]="A", 12, IF(table_7_1[[#This Row],[hguide]]="B", 12, IF(table_7_1[[#This Row],[hguide]]="CD", 12, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="25">
+    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="31">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/individual/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="24">
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="30">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], IF(NOT(ISNA(table_7_1[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_1[[#This Row],[universal_layout_legend_pos_x]], "")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2262,38 +2292,38 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:K60" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:K60" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A44:K60" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="22"/>
-    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="21">
+    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="27">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="20">
+    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="26">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="19">
+    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="25">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="18">
+    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="24">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="17">
+    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="23">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="16">
+    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="22">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="15">
+    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_legend_pos_x" dataDxfId="14">
+    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_legend_pos_x" dataDxfId="20">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_legend_pos_x]:[universal_layout_legend_pos_x]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="13">
+    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="19">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="12">
+    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="18">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], IF(NOT(ISNA(table_7_2[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_2[[#This Row],[universal_layout_legend_pos_x]], "")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2302,38 +2332,38 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:K64" totalsRowShown="0" headerRowDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:K64" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="A62:K64" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="15">
       <calculatedColumnFormula>OFFSET(table_4_2[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="8">
+    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="14">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="7">
+    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="13">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="6">
+    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="12">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="5">
+    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="11">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="4">
+    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="10">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="3">
+    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_legend_pos_x" dataDxfId="2">
+    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_legend_pos_x" dataDxfId="8">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_legend_pos_x]:[universal_layout_legend_pos_x]], 37 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="1">
+    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="7">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="0">
+    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="6">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], IF(NOT(ISNA(table_7_3[[#This Row],[universal_layout_legend_pos_x]])), _xlfn.CONCAT(" --universal_layout_legend_pos_x ", table_7_3[[#This Row],[universal_layout_legend_pos_x]], "")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2342,10 +2372,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="198">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="202">
   <autoFilter ref="A1:O173" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}"/>
   <tableColumns count="15">
-    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="197"/>
+    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="201"/>
     <tableColumn id="1" xr3:uid="{5C1CDEE9-AAC7-4E12-B88F-1314CF422335}" name="library"/>
     <tableColumn id="2" xr3:uid="{D4B174CF-F774-4DA7-B75D-573BC94EE10F}" name="cell"/>
     <tableColumn id="3" xr3:uid="{83898EC9-96DA-46D4-B0B8-F68C7607DCF2}" name="control"/>
@@ -2353,25 +2383,25 @@
     <tableColumn id="5" xr3:uid="{81A143FE-8E74-4182-8124-E697DD5A7C62}" name="hguide"/>
     <tableColumn id="6" xr3:uid="{4A316E6A-69F3-4B78-9C01-4675AEB656FA}" name="treatment"/>
     <tableColumn id="7" xr3:uid="{25B8E763-346D-4756-8B58-D3C8CB103545}" name="strand"/>
-    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="196">
+    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="200">
       <calculatedColumnFormula array="1">IF(E2="2DSB", IF(H2="R1", 67, 46), IF(E2="1DSB", IF(H2="R1", 67, 46), IF(E2="2DSBanti", IF(H2="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="195">
+    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="199">
       <calculatedColumnFormula>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="194">
+    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="198">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="193">
+    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="197">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="192">
+    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="196">
       <calculatedColumnFormula>VLOOKUP(INT(MID(table_1[[#This Row],[library]], 4, 10)), table_1_2[#All], IF(table_1[[#This Row],[strand]]="R1", 3, 4))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="191">
+    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="195">
       <calculatedColumnFormula>IF(LEFT(table_1[[#This Row],[dsb_type]], 1) = "2", 50, 130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="190">
+    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="194">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2380,38 +2410,38 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="189">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="193">
   <autoFilter ref="A1:S41" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="188"/>
-    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="187">
+    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="192"/>
+    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="191">
       <calculatedColumnFormula>OFFSET(table_1[ref], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="186">
+    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="190">
       <calculatedColumnFormula>OFFSET(table_1[control], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="185">
+    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="189">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="184">
+    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="188">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="183">
+    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="187">
       <calculatedColumnFormula>OFFSET(table_1[cell], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="182">
+    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="186">
       <calculatedColumnFormula>OFFSET(table_1[strand], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="181">
+    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="185">
       <calculatedColumnFormula>OFFSET(table_1[treatment], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="180">
+    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="184">
       <calculatedColumnFormula>OFFSET(table_1[hguide], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="179">
+    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="183">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_1[[#This Row],[cell]], "_", table_2_1[[#This Row],[hguide]], "_", table_2_1[[#This Row],[strand]], "_", table_2_1[[#This Row],[treatment]], IF(table_2_1[[#This Row],[control]]&lt;&gt;"none",_xlfn.CONCAT("_", table_2_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="178">
+    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="182">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{3F29C0D1-58A3-430E-AAAA-9F679DCA46D6}" name="input_2">
@@ -2423,19 +2453,19 @@
     <tableColumn id="20" xr3:uid="{28521A62-94B3-4C7C-AF90-F4E2F4163D29}" name="input_4">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="177">
+    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="181">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="176">
+    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="180">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="175">
+    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="179">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="174">
+    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="178">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="173">
+    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="177">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2447,41 +2477,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}" name="table_2_2" displayName="table_2_2" ref="A44:M56" totalsRowShown="0">
   <autoFilter ref="A44:M56" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="172"/>
-    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="171">
+    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="176"/>
+    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="175">
       <calculatedColumnFormula>OFFSET(table_1[ref], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="170">
+    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="174">
       <calculatedColumnFormula>OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="169">
+    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="173">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="168">
+    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="172">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="167">
+    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="171">
       <calculatedColumnFormula>OFFSET(table_1[cell], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="166">
+    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="170">
       <calculatedColumnFormula>OFFSET(table_1[strand], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="165">
+    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="169">
       <calculatedColumnFormula>OFFSET(table_1[treatment], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="164">
+    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="168">
       <calculatedColumnFormula>OFFSET(table_1[hguide], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="163">
+    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="167">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_2[[#This Row],[cell]], "_", table_2_2[[#This Row],[hguide]], "_", table_2_2[[#This Row],[strand]], "_", table_2_2[[#This Row],[treatment]], "_nodsb")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="162">
+    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="166">
       <calculatedColumnFormula>OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="161">
+    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="165">
       <calculatedColumnFormula>OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="160">
+    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="164">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2490,47 +2520,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="159">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="163">
   <autoFilter ref="A1:N41" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="158"/>
-    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="157">
+    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="162"/>
+    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="161">
       <calculatedColumnFormula>OFFSET(table_2_1[output_dir], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="156">
+    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="160">
       <calculatedColumnFormula>OFFSET(table_2_1[control], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="155">
+    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="159">
       <calculatedColumnFormula>OFFSET(table_2_1[ref], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="154">
+    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="158">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="153">
+    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="157">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="152">
+    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="156">
       <calculatedColumnFormula array="1">IF(table_3_1[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_1[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_1[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="151">
+    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="155">
       <calculatedColumnFormula>OFFSET(table_2_1[strand], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="150">
+    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="154">
       <calculatedColumnFormula>MID(OFFSET(table_2_1[hguide], table_3_1[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="149">
+    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="153">
       <calculatedColumnFormula>OFFSET(table_2_1[cell], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="148">
+    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="152">
       <calculatedColumnFormula>OFFSET(table_2_1[treatment], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DB6998A3-1431-4DDD-8DA0-525B805BF436}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="147">
+    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="151">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="146">
+    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="150">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2539,47 +2569,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="145">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="149">
   <autoFilter ref="A43:N55" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="144"/>
-    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="143">
+    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="148"/>
+    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="147">
       <calculatedColumnFormula>OFFSET(table_2_2[output_dir], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="142">
+    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="146">
       <calculatedColumnFormula>OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="141">
+    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="145">
       <calculatedColumnFormula>OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="140">
+    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="144">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_pos], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="139">
+    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="143">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_type], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="138">
+    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="142">
       <calculatedColumnFormula array="1">IF(table_3_2[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_2[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_2[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="137">
+    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="141">
       <calculatedColumnFormula>OFFSET(table_2_2[strand], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="136">
+    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="140">
       <calculatedColumnFormula>MID(OFFSET(table_2_2[hguide], table_3_2[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="135">
+    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="139">
       <calculatedColumnFormula>OFFSET(table_2_2[cell], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="134">
+    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="138">
       <calculatedColumnFormula>OFFSET(table_2_2[treatment], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{142C480D-E258-4979-A008-3940A3FE78E4}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="133">
+    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="137">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="132">
+    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="136">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2588,38 +2618,38 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="131">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="135">
   <autoFilter ref="A1:K17" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="130"/>
-    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="129">
+    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="134"/>
+    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="133">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="128">
+    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="132">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="127">
+    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="131">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="126">
+    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="130">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="125">
+    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="129">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="124">
+    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="128">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_1[[#This Row],[treatment_1]], "_", table_4_1[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="123">
+    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="127">
       <calculatedColumnFormula>SUBSTITUTE(table_4_1[[#This Row],[dir_1]], table_4_1[[#This Row],[treatment_1]], table_4_1[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="122">
+    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="126">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="121">
+    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="125">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_1[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_1[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_1[[#This Row],[dir_out]], " --subst_type ", table_4_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="120">
+    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="124">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_1[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2628,38 +2658,38 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="123">
   <autoFilter ref="A20:K22" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="118"/>
-    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="117">
+    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="122"/>
+    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="121">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_4_anti_offset + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="116">
+    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="120">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="115">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="119">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="114">
+    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="118">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="113">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="117">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="112">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="116">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_2[[#This Row],[treatment_1]], "_", table_4_2[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="111">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="115">
       <calculatedColumnFormula>SUBSTITUTE(table_4_2[[#This Row],[dir_1]], table_4_2[[#This Row],[treatment_1]], table_4_2[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="110">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="114">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_2[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_2[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_2[[#This Row],[dir_out]], " --subst_type ", table_4_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="109">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="113">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_2[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2668,38 +2698,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="108">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="112">
   <autoFilter ref="A25:K33" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="107"/>
-    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="106">
+    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="111"/>
+    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="110">
       <calculatedColumnFormula>OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="105">
+    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="109">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="104">
+    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="108">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="103">
+    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="107">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="102">
+    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="106">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="101">
+    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="105">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_3[[#This Row],[treatment_1]], "_", table_4_3[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="100">
+    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="104">
       <calculatedColumnFormula>SUBSTITUTE(table_4_3[[#This Row],[dir_1]], table_4_3[[#This Row],[treatment_1]], table_4_3[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="99">
+    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="103">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="98">
+    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="102">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_3[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_3[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_3[[#This Row],[dir_out]], " --subst_type ", table_4_3[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="97">
+    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="101">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_3[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_3[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4713,7 +4743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F1EACD-27DC-4973-8E3A-9162F610D9C4}">
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B157" workbookViewId="0">
+    <sheetView topLeftCell="B157" workbookViewId="0">
       <selection activeCell="O173" sqref="O173"/>
     </sheetView>
   </sheetViews>
@@ -22787,10 +22817,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FCC207B-A9CD-4866-A17E-A3EE763F139F}">
-  <dimension ref="A1:M58"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="A58" sqref="A58"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22804,11 +22834,11 @@
     <col min="10" max="10" width="12.140625" customWidth="1"/>
     <col min="11" max="11" width="12.85546875" customWidth="1"/>
     <col min="12" max="12" width="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="51" customWidth="1"/>
-    <col min="14" max="14" width="22.7109375" customWidth="1"/>
+    <col min="13" max="13" width="12.42578125" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>112</v>
       </c>
@@ -22846,10 +22876,16 @@
         <v>105</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -22898,11 +22934,19 @@
         <v>with</v>
       </c>
       <c r="M2" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_sense -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N2" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O2" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_sense -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -22951,11 +22995,19 @@
         <v>with</v>
       </c>
       <c r="M3" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_branch -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N3" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O3" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_branch -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -23004,11 +23056,19 @@
         <v>with</v>
       </c>
       <c r="M4" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_cmv -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N4" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O4" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_cmv -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -23057,11 +23117,19 @@
         <v>with</v>
       </c>
       <c r="M5" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_sense -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N5" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O5" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_sense -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -23110,11 +23178,19 @@
         <v>with</v>
       </c>
       <c r="M6" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_branch -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N6" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O6" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_branch -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -23163,11 +23239,19 @@
         <v>with</v>
       </c>
       <c r="M7" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_cmv -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N7" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O7" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_cmv -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -23216,11 +23300,19 @@
         <v>with</v>
       </c>
       <c r="M8" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_sense -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N8" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O8" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_sense -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -23269,11 +23361,19 @@
         <v>with</v>
       </c>
       <c r="M9" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_branch -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N9" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O9" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_branch -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -23322,11 +23422,19 @@
         <v>with</v>
       </c>
       <c r="M10" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_cmv -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N10" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O10" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_cmv -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -23375,11 +23483,19 @@
         <v>with</v>
       </c>
       <c r="M11" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_sense -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N11" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O11" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_sense -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -23428,11 +23544,19 @@
         <v>with</v>
       </c>
       <c r="M12" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_branch -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N12" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O12" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_branch -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -23481,11 +23605,19 @@
         <v>with</v>
       </c>
       <c r="M13" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_cmv -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N13" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O13" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_cmv -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -23534,11 +23666,19 @@
         <v>with</v>
       </c>
       <c r="M14" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N14" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O14" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>14</v>
       </c>
@@ -23587,11 +23727,19 @@
         <v>with</v>
       </c>
       <c r="M15" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N15" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O15" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -23640,11 +23788,19 @@
         <v>with</v>
       </c>
       <c r="M16" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N16" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O16" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -23693,11 +23849,19 @@
         <v>with</v>
       </c>
       <c r="M17" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N17" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O17" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -23746,11 +23910,19 @@
         <v>with</v>
       </c>
       <c r="M18" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N18" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O18" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -23799,11 +23971,19 @@
         <v>with</v>
       </c>
       <c r="M19" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N19" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O19" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -23852,11 +24032,19 @@
         <v>with</v>
       </c>
       <c r="M20" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N20" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O20" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -23905,11 +24093,19 @@
         <v>with</v>
       </c>
       <c r="M21" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N21" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O21" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -23958,11 +24154,19 @@
         <v>with</v>
       </c>
       <c r="M22" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N22" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O22" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -24011,11 +24215,19 @@
         <v>with</v>
       </c>
       <c r="M23" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N23" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O23" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -24064,11 +24276,19 @@
         <v>with</v>
       </c>
       <c r="M24" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N24" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O24" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>24</v>
       </c>
@@ -24117,11 +24337,19 @@
         <v>with</v>
       </c>
       <c r="M25" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N25" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O25" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>25</v>
       </c>
@@ -24170,11 +24398,19 @@
         <v>with</v>
       </c>
       <c r="M26" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>absolute</v>
+      </c>
+      <c r="N26" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O26" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/histogram_3d/ -lt absolute</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>26</v>
       </c>
@@ -24223,11 +24459,19 @@
         <v>with</v>
       </c>
       <c r="M27" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>absolute</v>
+      </c>
+      <c r="N27" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O27" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/histogram_3d/ -lt absolute</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>27</v>
       </c>
@@ -24276,11 +24520,19 @@
         <v>with</v>
       </c>
       <c r="M28" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>absolute</v>
+      </c>
+      <c r="N28" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O28" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/histogram_3d/ -lt absolute</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>28</v>
       </c>
@@ -24329,11 +24581,19 @@
         <v>with</v>
       </c>
       <c r="M29" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>absolute</v>
+      </c>
+      <c r="N29" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O29" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/histogram_3d/ -lt absolute</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>29</v>
       </c>
@@ -24382,11 +24642,19 @@
         <v>with</v>
       </c>
       <c r="M30" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>absolute</v>
+      </c>
+      <c r="N30" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O30" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/histogram_3d/ -lt absolute</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -24435,11 +24703,19 @@
         <v>with</v>
       </c>
       <c r="M31" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>absolute</v>
+      </c>
+      <c r="N31" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O31" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/histogram_3d/ -lt absolute</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -24488,11 +24764,19 @@
         <v>with</v>
       </c>
       <c r="M32" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>absolute</v>
+      </c>
+      <c r="N32" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O32" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/histogram_3d/ -rp  -lt absolute</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>32</v>
       </c>
@@ -24541,11 +24825,19 @@
         <v>with</v>
       </c>
       <c r="M33" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>absolute</v>
+      </c>
+      <c r="N33" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O33" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/histogram_3d/ -rp  -lt absolute</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -24594,11 +24886,19 @@
         <v>with</v>
       </c>
       <c r="M34" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>absolute</v>
+      </c>
+      <c r="N34" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O34" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/histogram_3d/ -rp  -lt absolute</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>34</v>
       </c>
@@ -24647,11 +24947,19 @@
         <v>with</v>
       </c>
       <c r="M35" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>absolute</v>
+      </c>
+      <c r="N35" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O35" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/histogram_3d/ -rp  -lt absolute</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>35</v>
       </c>
@@ -24700,11 +25008,19 @@
         <v>with</v>
       </c>
       <c r="M36" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>absolute</v>
+      </c>
+      <c r="N36" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O36" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/histogram_3d/ -rp  -lt absolute</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>36</v>
       </c>
@@ -24753,11 +25069,19 @@
         <v>with</v>
       </c>
       <c r="M37" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>absolute</v>
+      </c>
+      <c r="N37" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O37" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/histogram_3d/ -rp  -lt absolute</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>37</v>
       </c>
@@ -24806,11 +25130,19 @@
         <v>with</v>
       </c>
       <c r="M38" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R1_antisense -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N38" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O38" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R1_antisense -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>38</v>
       </c>
@@ -24859,11 +25191,19 @@
         <v>with</v>
       </c>
       <c r="M39" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R1_splicing -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N39" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O39" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R1_splicing -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>39</v>
       </c>
@@ -24912,11 +25252,19 @@
         <v>with</v>
       </c>
       <c r="M40" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R2_antisense -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N40" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O40" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R2_antisense -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>40</v>
       </c>
@@ -24965,11 +25313,19 @@
         <v>with</v>
       </c>
       <c r="M41" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R2_splicing -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N41" t="str">
+        <f ca="1">IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O41" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R2_splicing -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>112</v>
       </c>
@@ -25007,10 +25363,16 @@
         <v>105</v>
       </c>
       <c r="M43" t="s">
+        <v>189</v>
+      </c>
+      <c r="N43" t="s">
+        <v>190</v>
+      </c>
+      <c r="O43" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>1</v>
       </c>
@@ -25059,11 +25421,19 @@
         <v>with</v>
       </c>
       <c r="M44" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense_nodsb -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N44" t="str">
+        <f ca="1">IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O44" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense_nodsb -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2</v>
       </c>
@@ -25112,11 +25482,19 @@
         <v>with</v>
       </c>
       <c r="M45" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch_nodsb -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N45" t="str">
+        <f ca="1">IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O45" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch_nodsb -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>3</v>
       </c>
@@ -25165,11 +25543,19 @@
         <v>with</v>
       </c>
       <c r="M46" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv_nodsb -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N46" t="str">
+        <f ca="1">IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O46" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv_nodsb -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>4</v>
       </c>
@@ -25218,11 +25604,19 @@
         <v>with</v>
       </c>
       <c r="M47" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense_nodsb -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N47" t="str">
+        <f ca="1">IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O47" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense_nodsb -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>5</v>
       </c>
@@ -25271,11 +25665,19 @@
         <v>with</v>
       </c>
       <c r="M48" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch_nodsb -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N48" t="str">
+        <f ca="1">IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O48" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch_nodsb -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>6</v>
       </c>
@@ -25324,11 +25726,19 @@
         <v>with</v>
       </c>
       <c r="M49" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv_nodsb -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N49" t="str">
+        <f ca="1">IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v/>
+      </c>
+      <c r="O49" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv_nodsb -o plots/histogram_3d/ -lt relative</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>7</v>
       </c>
@@ -25377,11 +25787,19 @@
         <v>with</v>
       </c>
       <c r="M50" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense_nodsb -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N50" t="str">
+        <f ca="1">IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O50" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense_nodsb -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>8</v>
       </c>
@@ -25430,11 +25848,19 @@
         <v>with</v>
       </c>
       <c r="M51" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch_nodsb -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N51" t="str">
+        <f ca="1">IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O51" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch_nodsb -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>9</v>
       </c>
@@ -25483,11 +25909,19 @@
         <v>with</v>
       </c>
       <c r="M52" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv_nodsb -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N52" t="str">
+        <f ca="1">IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O52" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv_nodsb -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>10</v>
       </c>
@@ -25536,11 +25970,19 @@
         <v>with</v>
       </c>
       <c r="M53" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense_nodsb -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N53" t="str">
+        <f ca="1">IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O53" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense_nodsb -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>11</v>
       </c>
@@ -25589,11 +26031,19 @@
         <v>with</v>
       </c>
       <c r="M54" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch_nodsb -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N54" t="str">
+        <f ca="1">IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O54" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch_nodsb -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>12</v>
       </c>
@@ -25642,73 +26092,82 @@
         <v>with</v>
       </c>
       <c r="M55" t="str">
-        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/")</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/histogram_3d/</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+        <f ca="1">IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</f>
+        <v>relative</v>
+      </c>
+      <c r="N55" t="str">
+        <f ca="1">IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</f>
+        <v xml:space="preserve"> -rp </v>
+      </c>
+      <c r="O55" t="str">
+        <f ca="1">_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/histogram_3d/ -rp  -lt relative</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, M2:M41,M44:M55)</f>
-        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_sense -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_branch -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_cmv -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_sense -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_branch -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_cmv -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_sense -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_branch -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_cmv -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_sense -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_branch -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_cmv -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R1_antisense -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R1_splicing -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R2_antisense -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R2_splicing -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense_nodsb -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch_nodsb -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv_nodsb -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense_nodsb -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch_nodsb -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv_nodsb -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense_nodsb -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch_nodsb -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv_nodsb -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense_nodsb -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch_nodsb -o plots/histogram_3d/
-python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/histogram_3d/</v>
+        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, O2:O41,O44:O55)</f>
+        <v>python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_sense -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_branch -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R1_cmv -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_sense -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_branch -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R1_cmv -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_sense -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_branch -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgAB_R2_cmv -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_sense -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_branch -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgAB_R2_cmv -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/histogram_3d/ -lt absolute
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/histogram_3d/ -lt absolute
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/histogram_3d/ -lt absolute
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/histogram_3d/ -lt absolute
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/histogram_3d/ -lt absolute
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/histogram_3d/ -lt absolute
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/histogram_3d/ -rp  -lt absolute
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/histogram_3d/ -rp  -lt absolute
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/histogram_3d/ -rp  -lt absolute
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/histogram_3d/ -rp  -lt absolute
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/histogram_3d/ -rp  -lt absolute
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/histogram_3d/ -rp  -lt absolute
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R1_antisense -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R1_splicing -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R2_antisense -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgCD_R2_splicing -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_sense_nodsb -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_branch_nodsb -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgA_R1_cmv_nodsb -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_sense_nodsb -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_branch_nodsb -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgA_R1_cmv_nodsb -o plots/histogram_3d/ -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_sense_nodsb -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_branch_nodsb -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/WT_sgB_R2_cmv_nodsb -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_sense_nodsb -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_branch_nodsb -o plots/histogram_3d/ -rp  -lt relative
+python 2_graph_processing/make_histogram_3d.py -i libraries_4/KO_sgB_R2_cmv_nodsb -o plots/histogram_3d/ -rp  -lt relative</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="2">

</xml_diff>

<commit_message>
Add new option to make_pptx to control size of images.
</commit_message>
<xml_diff>
--- a/analyze_nhej/libinfo.xlsx
+++ b/analyze_nhej/libinfo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\analyze_nhej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23DA7FEF-035E-4347-9AAD-9956F715789D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEE428E-61FA-4545-B41D-214116FB2F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1562" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="203">
   <si>
     <t>yjl217</t>
   </si>
@@ -691,6 +691,15 @@
   <si>
     <t>universal_layout_max_tick_args</t>
   </si>
+  <si>
+    <t>format</t>
+  </si>
+  <si>
+    <t>individual</t>
+  </si>
+  <si>
+    <t>combined</t>
+  </si>
 </sst>
 </file>
 
@@ -809,22 +818,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FFD19645-61C4-4244-A560-0232B787F38C}"/>
   </cellStyles>
-  <dxfs count="217">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
+  <dxfs count="218">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -937,6 +931,12 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -971,6 +971,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2062,7 +2074,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}" name="table_1_2" displayName="table_1_2" ref="A1:D108" totalsRowShown="0">
   <autoFilter ref="A1:D108" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}"/>
   <tableColumns count="4">
-    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="216">
+    <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="217">
       <calculatedColumnFormula>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{5F63B290-093A-48A3-9AFC-EB2FE27DE630}" name="library"/>
@@ -2074,50 +2086,50 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:O41" totalsRowShown="0" headerRowDxfId="113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:O41" totalsRowShown="0" headerRowDxfId="114">
   <autoFilter ref="A1:O41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="15">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="112"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="111">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="113"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="112">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="110">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="111">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="109">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="110">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="108">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="109">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="107">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="108">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="106">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="107">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="105">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="106">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="104">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="105">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="103">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="104">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="102">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="103">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="101">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="102">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1D971CC2-F378-4E62-9759-F7168770AA64}" name="label_type" dataDxfId="100">
+    <tableColumn id="11" xr3:uid="{1D971CC2-F378-4E62-9759-F7168770AA64}" name="label_type" dataDxfId="101">
       <calculatedColumnFormula>IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{8241431B-CE1C-49A4-B13E-77512D442338}" name="reverse_pos" dataDxfId="99">
+    <tableColumn id="14" xr3:uid="{8241431B-CE1C-49A4-B13E-77512D442338}" name="reverse_pos" dataDxfId="100">
       <calculatedColumnFormula>IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="98">
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="99">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2130,46 +2142,46 @@
   <autoFilter ref="A43:O55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
-    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="97">
+    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="98">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="96">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="97">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="95">
+    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="96">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="94">
+    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="95">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="93">
+    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="94">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="92">
+    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="93">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="91">
+    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="92">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="90">
+    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="91">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="89">
+    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="90">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="88">
+    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="89">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="87">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="88">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{F5E6916D-F1BC-48E0-9E73-728C62F32A69}" name="label_type" dataDxfId="86">
+    <tableColumn id="14" xr3:uid="{F5E6916D-F1BC-48E0-9E73-728C62F32A69}" name="label_type" dataDxfId="87">
       <calculatedColumnFormula>IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{EF50F256-FFB6-49D0-8199-D7AB5C783AD5}" name="reverse_pos" dataDxfId="85">
+    <tableColumn id="15" xr3:uid="{EF50F256-FFB6-49D0-8199-D7AB5C783AD5}" name="reverse_pos" dataDxfId="86">
       <calculatedColumnFormula>IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="84">
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="85">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2178,36 +2190,36 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="83">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="84">
   <autoFilter ref="A3:I4" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="82"/>
-    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="81">
+    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="83"/>
+    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="82">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="80">
+    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="81">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="79">
+    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="80">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="78">
+    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="79">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 12 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="33" xr3:uid="{8FF7E83A-9135-4A64-965C-48368A6C0367}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="77">
+    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="78">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="76">
+    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="77">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="75">
+    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="76">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2216,32 +2228,32 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="74">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="75">
   <autoFilter ref="A7:I9" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="73"/>
-    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="72">
+    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="74"/>
+    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="73">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="71">
+    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="72">
       <calculatedColumnFormula>IF(table_6_4[[#This Row],[hguide]]="A",NA(), IF(var_6_layout = "universal", "1 1 1 1 1 1", NA()))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="70">
+    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="71">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="69">
+    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="70">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" xr3:uid="{5BD83012-469D-4202-9584-AA182CDF11F9}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="68">
+    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="69">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="67">
+    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="68">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="66">
+    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="67">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2250,36 +2262,36 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="65" headerRowBorderDxfId="64" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64">
   <autoFilter ref="A12:I13" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0F421990-E775-4F35-92AF-6BA19E0E8AEE}" name="index"/>
-    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="62">
+    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="63">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="61">
+    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="62">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0,4, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="60">
+    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="61">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="59">
+    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="60">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{E0783723-9246-4BF6-A5DA-E000EA1E5E87}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="58">
+    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="59">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="57">
+    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="58">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="56">
+    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="57">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2288,44 +2300,44 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:AA42" totalsRowShown="0" headerRowDxfId="55">
-  <autoFilter ref="A2:AA42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
-  <tableColumns count="27">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="54"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="53">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:AB42" totalsRowShown="0" headerRowDxfId="56">
+  <autoFilter ref="A2:AB42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
+  <tableColumns count="28">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="55"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="54">
       <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="52">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="53">
       <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="51">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="52">
       <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="50">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="51">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="49">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="50">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="48">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="49">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="47">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="48">
       <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="46">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="47">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="45">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="46">
       <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="44">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="45">
       <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="43">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="44">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="42">
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="43">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
       OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
       IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
@@ -2337,16 +2349,16 @@
       )
   )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="41">
+    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="42">
       <calculatedColumnFormula>AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{2D7A10AC-1675-4E76-989F-888C0D89C117}" name="range_x0" dataDxfId="40">
+    <tableColumn id="27" xr3:uid="{2D7A10AC-1675-4E76-989F-888C0D89C117}" name="range_x0" dataDxfId="41">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -12, IF(table_7_1[[#This Row],[hguide]]="CD", -12, IF(table_7_1[[#This Row],[hguide]]="A", -12, IF(table_7_1[[#This Row],[hguide]]="B", -12, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{CD6660D4-A656-4F48-89BD-45D3BAC7EE11}" name="range_x1" dataDxfId="39">
+    <tableColumn id="26" xr3:uid="{CD6660D4-A656-4F48-89BD-45D3BAC7EE11}" name="range_x1" dataDxfId="40">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 13, IF(table_7_1[[#This Row],[hguide]]="CD", 13, IF(table_7_1[[#This Row],[hguide]]="A", 13, IF(table_7_1[[#This Row],[hguide]]="B", 13, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{EFB5F04D-FC42-47A6-83B6-18FC45D14ABE}" name="range_y0" dataDxfId="2">
+    <tableColumn id="28" xr3:uid="{EFB5F04D-FC42-47A6-83B6-18FC45D14ABE}" name="range_y0" dataDxfId="39">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="18" xr3:uid="{FCD7272B-07C5-4D80-8B2B-EFDF0948D1A3}" name="range_y1" dataDxfId="38">
@@ -2362,19 +2374,20 @@
     <tableColumn id="23" xr3:uid="{010D8635-D593-4849-BEA6-27994308E467}" name="universal_layout_x_axis_args" dataDxfId="35">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[show_universal_layout_x_axes]], _xlfn.CONCAT(" --universal_layout_x_axis_deletion_y_pos ", table_7_1[[#This Row],[range_y0]] + 1.5, " --universal_layout_x_axis_insertion_y_pos ", table_7_1[[#This Row],[range_y1]] - 0.5, " --universal_layout_x_axis_x_range ", table_7_1[[#This Row],[range_x0]] + 0.5, " ", table_7_1[[#This Row],[range_x1]] - 1.5), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{5BFAE794-32B2-4D0D-B4C9-47939AA6DF3D}" name="universal_layout_max_tick_insertion" dataDxfId="9">
+    <tableColumn id="17" xr3:uid="{5BFAE794-32B2-4D0D-B4C9-47939AA6DF3D}" name="universal_layout_max_tick_insertion" dataDxfId="34">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 7, IF(table_7_1[[#This Row],[hguide]]="CD", 8, IF(table_7_1[[#This Row],[hguide]]="A", 6, IF(table_7_1[[#This Row],[hguide]]="B", 5, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{BDF49305-2112-4726-89DD-C9F4FFED50C5}" name="universal_layout_max_tick_deletion" dataDxfId="8">
+    <tableColumn id="19" xr3:uid="{BDF49305-2112-4726-89DD-C9F4FFED50C5}" name="universal_layout_max_tick_deletion" dataDxfId="33">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{9E5CCD08-C11E-4294-860A-FDFE3FE422F8}" name="universal_layout_max_tick_args" dataDxfId="7">
+    <tableColumn id="20" xr3:uid="{9E5CCD08-C11E-4294-860A-FDFE3FE422F8}" name="universal_layout_max_tick_args" dataDxfId="32">
       <calculatedColumnFormula>IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_deletion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_deletion]], " --universal_layout_y_axis_insertion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_insertion]]), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="34">
-      <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/individual/", var_7_ext)</calculatedColumnFormula>
+    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="3">
+      <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="6">
+    <tableColumn id="21" xr3:uid="{C5B2A575-6AC4-403E-AE67-1624B7F60F7E}" name="format"/>
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="31">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2383,45 +2396,46 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:N60" totalsRowShown="0" headerRowDxfId="33">
-  <autoFilter ref="A44:N60" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:O60" totalsRowShown="0" headerRowDxfId="30">
+  <autoFilter ref="A44:O60" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="28">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="30">
+    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="27">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="29">
+    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="26">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="28">
+    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="25">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="27">
+    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="24">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="26">
+    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="23">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="22">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{0EB304B9-B5C9-435B-99CC-6F02D04A5268}" name="universal_layout_y_axis_args" dataDxfId="24">
+    <tableColumn id="12" xr3:uid="{0EB304B9-B5C9-435B-99CC-6F02D04A5268}" name="universal_layout_y_axis_args" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_y_axis_args]:[universal_layout_y_axis_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{EADBB7DC-9D40-44C2-8742-A17A0EB899C3}" name="show_universal_layout_x_axes"/>
-    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_x_axis_args" dataDxfId="10">
+    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_x_axis_args" dataDxfId="20">
       <calculatedColumnFormula>IF(table_7_2[[#This Row],[show_universal_layout_x_axes]], OFFSET(table_7_1[[universal_layout_x_axis_args]:[universal_layout_x_axis_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{641C7B24-D16A-472B-B06C-7348DDBC60AA}" name="universal_layout_max_tick_args" dataDxfId="5">
+    <tableColumn id="14" xr3:uid="{641C7B24-D16A-472B-B06C-7348DDBC60AA}" name="universal_layout_max_tick_args" dataDxfId="19">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_max_tick_args]:[universal_layout_max_tick_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="23">
-      <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="2">
+      <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="4">
+    <tableColumn id="15" xr3:uid="{8B58B2DF-3EB7-4D4E-A96D-1BED892121E3}" name="format"/>
+    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="18">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2430,45 +2444,46 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:N64" totalsRowShown="0" headerRowDxfId="22">
-  <autoFilter ref="A62:N64" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}"/>
-  <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:O64" totalsRowShown="0" headerRowDxfId="17">
+  <autoFilter ref="A62:O64" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}"/>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="16"/>
+    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="15">
       <calculatedColumnFormula>OFFSET(table_4_2[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="19">
+    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="14">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="18">
+    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="13">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="17">
+    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="12">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="16">
+    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="11">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="15">
+    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="10">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="14">
+    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BF1D3FB1-D45A-4909-BA3E-BB6993D39E6E}" name="universal_layout_y_axis_args" dataDxfId="13">
+    <tableColumn id="12" xr3:uid="{BF1D3FB1-D45A-4909-BA3E-BB6993D39E6E}" name="universal_layout_y_axis_args" dataDxfId="8">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_y_axis_args]:[universal_layout_y_axis_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{8D9288FF-05A5-4B58-AC7F-2C4096A25202}" name="show_universal_layout_x_axes" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_x_axis_args" dataDxfId="1">
+    <tableColumn id="13" xr3:uid="{8D9288FF-05A5-4B58-AC7F-2C4096A25202}" name="show_universal_layout_x_axes" dataDxfId="7"/>
+    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_x_axis_args" dataDxfId="6">
       <calculatedColumnFormula>IF(table_7_3[[#This Row],[show_universal_layout_x_axes]], OFFSET(table_7_1[[universal_layout_x_axis_args]:[universal_layout_x_axis_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{FD5F951D-27C2-4E6B-B33F-D83C250C9CC4}" name="universal_layout_max_tick_args" dataDxfId="0">
+    <tableColumn id="14" xr3:uid="{FD5F951D-27C2-4E6B-B33F-D83C250C9CC4}" name="universal_layout_max_tick_args" dataDxfId="5">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_max_tick_args]:[universal_layout_max_tick_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="12">
-      <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</calculatedColumnFormula>
+    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="0">
+      <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_3[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="3">
+    <tableColumn id="15" xr3:uid="{0AB61192-5C37-4578-ADFD-BAE568B914C5}" name="format" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="4">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], " ", table_7_3[[#This Row],[universal_layout_y_axis_args]], " ", table_7_3[[#This Row],[universal_layout_x_axis_args]], " ", table_7_3[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2477,10 +2492,10 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="215">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}" name="table_1" displayName="table_1" ref="A1:O173" totalsRowShown="0" headerRowDxfId="216">
   <autoFilter ref="A1:O173" xr:uid="{22A90416-B904-4D3D-A6DB-EFCB9FD1EAED}"/>
   <tableColumns count="15">
-    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="214"/>
+    <tableColumn id="15" xr3:uid="{A06DA701-31D6-44A5-8655-82CAD7E3082B}" name="index" dataDxfId="215"/>
     <tableColumn id="1" xr3:uid="{5C1CDEE9-AAC7-4E12-B88F-1314CF422335}" name="library"/>
     <tableColumn id="2" xr3:uid="{D4B174CF-F774-4DA7-B75D-573BC94EE10F}" name="cell"/>
     <tableColumn id="3" xr3:uid="{83898EC9-96DA-46D4-B0B8-F68C7607DCF2}" name="control"/>
@@ -2488,25 +2503,25 @@
     <tableColumn id="5" xr3:uid="{81A143FE-8E74-4182-8124-E697DD5A7C62}" name="hguide"/>
     <tableColumn id="6" xr3:uid="{4A316E6A-69F3-4B78-9C01-4675AEB656FA}" name="treatment"/>
     <tableColumn id="7" xr3:uid="{25B8E763-346D-4756-8B58-D3C8CB103545}" name="strand"/>
-    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="213">
+    <tableColumn id="8" xr3:uid="{4B708639-BB19-4DC1-A57D-214FA0EFB1EA}" name="dsb_pos" dataDxfId="214">
       <calculatedColumnFormula array="1">IF(E2="2DSB", IF(H2="R1", 67, 46), IF(E2="1DSB", IF(H2="R1", 67, 46), IF(E2="2DSBanti", IF(H2="R1", 50, 47), NA))) + IF(table_1[[#This Row],[control]]="30bpDown", 30, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="212">
+    <tableColumn id="9" xr3:uid="{CCF6021C-1B60-4954-A92E-3F2848564215}" name="file_in" dataDxfId="213">
       <calculatedColumnFormula>IF(OR(table_1[[#This Row],[control]]="none", table_1[[#This Row],[control]]="30bpDown"), _xlfn.CONCAT(table_1[[#This Row],[library]], IF(table_1[[#This Row],[dsb_type]] = "2DSBanti", "_anti", ""), "_",table_1[[#This Row],[strand]],"_", IF(LEFT(table_1[[#This Row],[dsb_type]], 1)="2","2DSBs", table_1[[#This Row],[hguide]]), ".sam"), _xlfn.CONCAT(table_1[[#This Row],[library]], "_NHEJ_", IF(table_1[[#This Row],[hguide]]="sgA", "hg39", IF(table_1[[#This Row],[hguide]]="sgB", "hg42", "2DSB")), "_", table_1[[#This Row],[strand]], ".sam"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="211">
+    <tableColumn id="10" xr3:uid="{58220462-2A11-4DAD-A247-C0871AFCFDB4}" name="file_out" dataDxfId="212">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[library]], "_", table_1[[#This Row],[cell]], "_", table_1[[#This Row],[hguide]], "_", table_1[[#This Row],[strand]], "_", table_1[[#This Row],[treatment]], IF(table_1[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="210">
+    <tableColumn id="11" xr3:uid="{775EE7A9-3C78-4568-BF98-500DE451177C}" name="ref" dataDxfId="211">
       <calculatedColumnFormula>_xlfn.CONCAT(table_1[[#This Row],[dsb_type]],"_", table_1[[#This Row],[strand]],"_", table_1[[#This Row],[treatment]], ".fa")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="209">
+    <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="210">
       <calculatedColumnFormula>VLOOKUP(INT(MID(table_1[[#This Row],[library]], 4, 10)), table_1_2[#All], IF(table_1[[#This Row],[strand]]="R1", 3, 4))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="208">
+    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="209">
       <calculatedColumnFormula>IF(LEFT(table_1[[#This Row],[dsb_type]], 1) = "2", 50, 130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="207">
+    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="208">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2515,38 +2530,38 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="206">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="207">
   <autoFilter ref="A1:S41" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="205"/>
-    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="204">
+    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="206"/>
+    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="205">
       <calculatedColumnFormula>OFFSET(table_1[ref], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="203">
+    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="204">
       <calculatedColumnFormula>OFFSET(table_1[control], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="202">
+    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="203">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="201">
+    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="202">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="200">
+    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="201">
       <calculatedColumnFormula>OFFSET(table_1[cell], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="199">
+    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="200">
       <calculatedColumnFormula>OFFSET(table_1[strand], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="198">
+    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="199">
       <calculatedColumnFormula>OFFSET(table_1[treatment], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="197">
+    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="198">
       <calculatedColumnFormula>OFFSET(table_1[hguide], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="196">
+    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="197">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_1[[#This Row],[cell]], "_", table_2_1[[#This Row],[hguide]], "_", table_2_1[[#This Row],[strand]], "_", table_2_1[[#This Row],[treatment]], IF(table_2_1[[#This Row],[control]]&lt;&gt;"none",_xlfn.CONCAT("_", table_2_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="195">
+    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="196">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{3F29C0D1-58A3-430E-AAAA-9F679DCA46D6}" name="input_2">
@@ -2558,19 +2573,19 @@
     <tableColumn id="20" xr3:uid="{28521A62-94B3-4C7C-AF90-F4E2F4163D29}" name="input_4">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="194">
+    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="195">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="193">
+    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="194">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="192">
+    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="193">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="191">
+    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="192">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="190">
+    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="191">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2582,41 +2597,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}" name="table_2_2" displayName="table_2_2" ref="A44:M56" totalsRowShown="0">
   <autoFilter ref="A44:M56" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="189"/>
-    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="188">
+    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="190"/>
+    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="189">
       <calculatedColumnFormula>OFFSET(table_1[ref], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="187">
+    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="188">
       <calculatedColumnFormula>OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="186">
+    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="187">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="185">
+    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="186">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="184">
+    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="185">
       <calculatedColumnFormula>OFFSET(table_1[cell], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="183">
+    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="184">
       <calculatedColumnFormula>OFFSET(table_1[strand], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="182">
+    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="183">
       <calculatedColumnFormula>OFFSET(table_1[treatment], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="181">
+    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="182">
       <calculatedColumnFormula>OFFSET(table_1[hguide], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="180">
+    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="181">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_2[[#This Row],[cell]], "_", table_2_2[[#This Row],[hguide]], "_", table_2_2[[#This Row],[strand]], "_", table_2_2[[#This Row],[treatment]], "_nodsb")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="179">
+    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="180">
       <calculatedColumnFormula>OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="178">
+    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="179">
       <calculatedColumnFormula>OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="177">
+    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="178">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2625,47 +2640,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="176">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="177">
   <autoFilter ref="A1:N41" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="175"/>
-    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="174">
+    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="176"/>
+    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="175">
       <calculatedColumnFormula>OFFSET(table_2_1[output_dir], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="173">
+    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="174">
       <calculatedColumnFormula>OFFSET(table_2_1[control], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="172">
+    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="173">
       <calculatedColumnFormula>OFFSET(table_2_1[ref], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="171">
+    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="172">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="170">
+    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="171">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="169">
+    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="170">
       <calculatedColumnFormula array="1">IF(table_3_1[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_1[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_1[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="168">
+    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="169">
       <calculatedColumnFormula>OFFSET(table_2_1[strand], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="167">
+    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="168">
       <calculatedColumnFormula>MID(OFFSET(table_2_1[hguide], table_3_1[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="166">
+    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="167">
       <calculatedColumnFormula>OFFSET(table_2_1[cell], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="165">
+    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="166">
       <calculatedColumnFormula>OFFSET(table_2_1[treatment], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DB6998A3-1431-4DDD-8DA0-525B805BF436}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="164">
+    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="165">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="163">
+    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="164">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2674,47 +2689,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="162">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="163">
   <autoFilter ref="A43:N55" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="161"/>
-    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="160">
+    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="162"/>
+    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="161">
       <calculatedColumnFormula>OFFSET(table_2_2[output_dir], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="159">
+    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="160">
       <calculatedColumnFormula>OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="158">
+    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="159">
       <calculatedColumnFormula>OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="157">
+    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="158">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_pos], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="156">
+    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="157">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_type], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="155">
+    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="156">
       <calculatedColumnFormula array="1">IF(table_3_2[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_2[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_2[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="154">
+    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="155">
       <calculatedColumnFormula>OFFSET(table_2_2[strand], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="153">
+    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="154">
       <calculatedColumnFormula>MID(OFFSET(table_2_2[hguide], table_3_2[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="152">
+    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="153">
       <calculatedColumnFormula>OFFSET(table_2_2[cell], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="151">
+    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="152">
       <calculatedColumnFormula>OFFSET(table_2_2[treatment], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{142C480D-E258-4979-A008-3940A3FE78E4}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="150">
+    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="151">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="149">
+    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="150">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2723,38 +2738,38 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="148">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="149">
   <autoFilter ref="A1:K17" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="147"/>
-    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="146">
+    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="148"/>
+    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="147">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="145">
+    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="146">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="144">
+    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="145">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="143">
+    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="144">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="142">
+    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="143">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="141">
+    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="142">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_1[[#This Row],[treatment_1]], "_", table_4_1[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="140">
+    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="141">
       <calculatedColumnFormula>SUBSTITUTE(table_4_1[[#This Row],[dir_1]], table_4_1[[#This Row],[treatment_1]], table_4_1[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="139">
+    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="140">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="138">
+    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="139">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_1[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_1[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_1[[#This Row],[dir_out]], " --subst_type ", table_4_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="137">
+    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="138">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_1[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2763,38 +2778,38 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="136">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="137">
   <autoFilter ref="A20:K22" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="135"/>
-    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="134">
+    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="136"/>
+    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="135">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_4_anti_offset + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="133">
+    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="134">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="132">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="133">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="131">
+    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="132">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="130">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="131">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="129">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="130">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_2[[#This Row],[treatment_1]], "_", table_4_2[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="128">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="129">
       <calculatedColumnFormula>SUBSTITUTE(table_4_2[[#This Row],[dir_1]], table_4_2[[#This Row],[treatment_1]], table_4_2[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="127">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="128">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_2[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_2[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_2[[#This Row],[dir_out]], " --subst_type ", table_4_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="126">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="127">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_2[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2803,38 +2818,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="125">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="126">
   <autoFilter ref="A25:K33" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="124"/>
-    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="123">
+    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="125"/>
+    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="124">
       <calculatedColumnFormula>OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="122">
+    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="123">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="121">
+    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="122">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="120">
+    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="121">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="119">
+    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="120">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="118">
+    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="119">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_3[[#This Row],[treatment_1]], "_", table_4_3[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="117">
+    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="118">
       <calculatedColumnFormula>SUBSTITUTE(table_4_3[[#This Row],[dir_1]], table_4_3[[#This Row],[treatment_1]], table_4_3[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="116">
+    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="117">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="115">
+    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="116">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_3[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_3[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_3[[#This Row],[dir_out]], " --subst_type ", table_4_3[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="114">
+    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="115">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_3[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_3[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -26661,10 +26676,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
-  <dimension ref="A1:AA67"/>
+  <dimension ref="A1:AB67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="L64" sqref="L64"/>
+    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
+      <selection activeCell="M64" sqref="M64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26683,7 +26698,7 @@
     <col min="14" max="14" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>174</v>
       </c>
@@ -26716,7 +26731,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>112</v>
       </c>
@@ -26796,10 +26811,13 @@
         <v>139</v>
       </c>
       <c r="AA2" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="AB2" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -26908,15 +26926,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="Z3" t="str">
-        <f t="shared" ref="Z3:Z42" si="1">_xlfn.CONCAT(graphs, "/", var_7_layout, "/individual/", var_7_ext)</f>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA3" t="str">
+      <c r="AA3" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB3" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5   --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 21.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -27025,15 +27046,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="Z4" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA4" t="str">
+      <c r="AA4" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB4" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -27142,15 +27166,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="Z5" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA5" t="str">
+      <c r="AA5" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB5" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -27259,15 +27286,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="Z6" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA6" t="str">
+      <c r="AA6" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB6" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5   --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 21.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -27376,15 +27406,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="Z7" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA7" t="str">
+      <c r="AA7" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB7" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
@@ -27493,15 +27526,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="Z8" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA8" t="str">
+      <c r="AA8" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB8" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
@@ -27610,15 +27646,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="Z9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA9" t="str">
+      <c r="AA9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -27727,15 +27766,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="Z10" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA10" t="str">
+      <c r="AA10" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB10" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -27844,15 +27886,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="Z11" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA11" t="str">
+      <c r="AA11" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB11" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
@@ -27961,15 +28006,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="Z12" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA12" t="str">
+      <c r="AA12" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB12" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
@@ -28078,15 +28126,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="Z13" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA13" t="str">
+      <c r="AA13" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB13" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
@@ -28195,15 +28246,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="Z14" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA14" t="str">
+      <c r="AA14" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB14" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
@@ -28312,15 +28366,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="Z15" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA15" t="str">
+      <c r="AA15" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB15" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5   --universal_layout_x_axis_deletion_y_pos -21.5 --universal_layout_x_axis_insertion_y_pos 19.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
@@ -28429,15 +28486,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="Z16" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA16" t="str">
+      <c r="AA16" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB16" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
@@ -28546,15 +28606,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="Z17" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA17" t="str">
+      <c r="AA17" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB17" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -28663,15 +28726,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="Z18" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA18" t="str">
+      <c r="AA18" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB18" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5   --universal_layout_x_axis_deletion_y_pos -21.5 --universal_layout_x_axis_insertion_y_pos 19.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -28780,15 +28846,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="Z19" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA19" t="str">
+      <c r="AA19" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB19" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -28897,15 +28966,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="Z20" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA20" t="str">
+      <c r="AA20" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB20" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -29014,15 +29086,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="Z21" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA21" t="str">
+      <c r="AA21" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB21" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -29131,15 +29206,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="Z22" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA22" t="str">
+      <c r="AA22" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB22" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -29248,15 +29326,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="Z23" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA23" t="str">
+      <c r="AA23" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB23" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -29365,15 +29446,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="Z24" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA24" t="str">
+      <c r="AA24" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB24" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -29482,15 +29566,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="Z25" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA25" t="str">
+      <c r="AA25" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB25" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -29599,15 +29686,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="Z26" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA26" t="str">
+      <c r="AA26" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB26" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -29716,15 +29806,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="Z27" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA27" s="9" t="str">
+      <c r="AA27" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB27" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -29833,15 +29926,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="Z28" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA28" s="9" t="str">
+      <c r="AA28" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB28" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -29950,15 +30046,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="Z29" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA29" s="9" t="str">
+      <c r="AA29" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB29" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -30067,15 +30166,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="Z30" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA30" s="9" t="str">
+      <c r="AA30" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB30" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -30184,15 +30286,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="Z31" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA31" s="9" t="str">
+      <c r="AA31" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB31" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -30301,15 +30406,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="Z32" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA32" s="9" t="str">
+      <c r="AA32" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB32" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -30418,15 +30526,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="Z33" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA33" s="9" t="str">
+      <c r="AA33" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB33" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -30535,15 +30646,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="Z34" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA34" s="9" t="str">
+      <c r="AA34" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB34" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -30652,15 +30766,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="Z35" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA35" s="9" t="str">
+      <c r="AA35" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB35" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -30769,15 +30886,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="Z36" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA36" s="9" t="str">
+      <c r="AA36" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB36" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -30886,15 +31006,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="Z37" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA37" s="9" t="str">
+      <c r="AA37" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB37" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -31003,15 +31126,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="Z38" s="9" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA38" s="9" t="str">
+      <c r="AA38" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB38" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -31120,15 +31246,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
       <c r="Z39" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA39" t="str">
+      <c r="AA39" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB39" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5   --universal_layout_x_axis_deletion_y_pos -16.5 --universal_layout_x_axis_insertion_y_pos 26.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -31237,15 +31366,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
       <c r="Z40" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA40" t="str">
+      <c r="AA40" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB40" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -31354,15 +31486,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
       <c r="Z41" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA41" t="str">
+      <c r="AA41" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB41" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>40</v>
       </c>
@@ -31471,15 +31606,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
       <c r="Z42" t="str">
-        <f t="shared" si="1"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/individual/png</v>
       </c>
-      <c r="AA42" t="str">
+      <c r="AA42" t="s">
+        <v>201</v>
+      </c>
+      <c r="AB42" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>112</v>
       </c>
@@ -31520,10 +31658,13 @@
         <v>139</v>
       </c>
       <c r="N44" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O44" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>1</v>
       </c>
@@ -31571,15 +31712,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="M45" s="2" t="str">
-        <f t="shared" ref="M45:M60" si="2">_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</f>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N45" t="str">
+      <c r="N45" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="O45" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>2</v>
       </c>
@@ -31627,15 +31771,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="M46" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N46" s="2" t="str">
+      <c r="N46" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="O46" s="2" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>3</v>
       </c>
@@ -31683,15 +31830,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="M47" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N47" t="str">
+      <c r="N47" t="s">
+        <v>202</v>
+      </c>
+      <c r="O47" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>4</v>
       </c>
@@ -31739,15 +31889,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="M48" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N48" t="str">
+      <c r="N48" t="s">
+        <v>202</v>
+      </c>
+      <c r="O48" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>5</v>
       </c>
@@ -31795,15 +31948,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="M49" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N49" t="str">
+      <c r="N49" t="s">
+        <v>202</v>
+      </c>
+      <c r="O49" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>6</v>
       </c>
@@ -31851,15 +32007,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="M50" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N50" t="str">
+      <c r="N50" t="s">
+        <v>202</v>
+      </c>
+      <c r="O50" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>7</v>
       </c>
@@ -31907,15 +32066,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="M51" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N51" t="str">
+      <c r="N51" t="s">
+        <v>202</v>
+      </c>
+      <c r="O51" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>8</v>
       </c>
@@ -31963,15 +32125,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
       <c r="M52" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N52" t="str">
+      <c r="N52" t="s">
+        <v>202</v>
+      </c>
+      <c r="O52" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>9</v>
       </c>
@@ -32019,15 +32184,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="M53" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N53" t="str">
+      <c r="N53" t="s">
+        <v>202</v>
+      </c>
+      <c r="O53" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>10</v>
       </c>
@@ -32075,15 +32243,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="M54" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N54" t="str">
+      <c r="N54" t="s">
+        <v>202</v>
+      </c>
+      <c r="O54" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>11</v>
       </c>
@@ -32131,15 +32302,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="M55" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N55" t="str">
+      <c r="N55" t="s">
+        <v>202</v>
+      </c>
+      <c r="O55" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>12</v>
       </c>
@@ -32187,15 +32361,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
       <c r="M56" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N56" t="str">
+      <c r="N56" t="s">
+        <v>202</v>
+      </c>
+      <c r="O56" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>13</v>
       </c>
@@ -32243,15 +32420,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="M57" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N57" t="str">
+      <c r="N57" t="s">
+        <v>202</v>
+      </c>
+      <c r="O57" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>14</v>
       </c>
@@ -32299,15 +32479,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="M58" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N58" t="str">
+      <c r="N58" t="s">
+        <v>202</v>
+      </c>
+      <c r="O58" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>15</v>
       </c>
@@ -32355,15 +32538,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="M59" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N59" t="str">
+      <c r="N59" t="s">
+        <v>202</v>
+      </c>
+      <c r="O59" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>16</v>
       </c>
@@ -32411,15 +32597,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
       <c r="M60" t="str">
-        <f t="shared" si="2"/>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N60" t="str">
+      <c r="N60" t="s">
+        <v>202</v>
+      </c>
+      <c r="O60" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>112</v>
       </c>
@@ -32460,10 +32649,13 @@
         <v>139</v>
       </c>
       <c r="N62" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="O62" s="1" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>1</v>
       </c>
@@ -32511,15 +32703,18 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
       <c r="M63" s="2" t="str">
-        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</f>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_3[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N63" t="str">
+      <c r="N63" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="O63" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], " ", table_7_3[[#This Row],[universal_layout_y_axis_args]], " ", table_7_3[[#This Row],[universal_layout_x_axis_args]], " ", table_7_3[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>2</v>
       </c>
@@ -32567,10 +32762,13 @@
         <v xml:space="preserve"> --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
       <c r="M64" s="2" t="str">
-        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/combined/", var_7_ext)</f>
+        <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_3[[#This Row],[format]], "/", var_7_ext)</f>
         <v>plots/graphs/universal/combined/png</v>
       </c>
-      <c r="N64" s="2" t="str">
+      <c r="N64" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="O64" s="2" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], " ", table_7_3[[#This Row],[universal_layout_y_axis_args]], " ", table_7_3[[#This Row],[universal_layout_x_axis_args]], " ", table_7_3[[#This Row],[universal_layout_max_tick_args]])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
@@ -32582,7 +32780,7 @@
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
-        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, AA3:AA26,AA39:AA42, table_7_2[command], table_7_3[command])</f>
+        <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, AB3:AB26,AB39:AB42, table_7_2[command], table_7_3[command])</f>
         <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5   --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 21.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
 python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
 python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7

</xml_diff>

<commit_message>
Add script for generating interactive graphs.
</commit_message>
<xml_diff>
--- a/analyze_nhej/libinfo.xlsx
+++ b/analyze_nhej/libinfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\analyze_nhej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EEE428E-61FA-4545-B41D-214116FB2F86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E3D80A-163C-49F5-861A-6A42A1F26B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
@@ -623,9 +623,6 @@
     <t>layout</t>
   </si>
   <si>
-    <t>png</t>
-  </si>
-  <si>
     <t>full_command</t>
   </si>
   <si>
@@ -699,6 +696,9 @@
   </si>
   <si>
     <t>combined</t>
+  </si>
+  <si>
+    <t>html</t>
   </si>
 </sst>
 </file>
@@ -862,12 +862,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -937,6 +931,9 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -971,6 +968,9 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -2383,11 +2383,11 @@
     <tableColumn id="20" xr3:uid="{9E5CCD08-C11E-4294-860A-FDFE3FE422F8}" name="universal_layout_max_tick_args" dataDxfId="32">
       <calculatedColumnFormula>IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_deletion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_deletion]], " --universal_layout_y_axis_insertion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_insertion]]), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="3">
+    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="31">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="21" xr3:uid="{C5B2A575-6AC4-403E-AE67-1624B7F60F7E}" name="format"/>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="31">
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="30">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2396,46 +2396,46 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:O60" totalsRowShown="0" headerRowDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:O60" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A44:O60" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="28">
+    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="27">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="27">
+    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="26">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="26">
+    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="25">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="25">
+    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="24">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="24">
+    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="23">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="23">
+    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="22">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="22">
+    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{0EB304B9-B5C9-435B-99CC-6F02D04A5268}" name="universal_layout_y_axis_args" dataDxfId="21">
+    <tableColumn id="12" xr3:uid="{0EB304B9-B5C9-435B-99CC-6F02D04A5268}" name="universal_layout_y_axis_args" dataDxfId="20">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_y_axis_args]:[universal_layout_y_axis_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{EADBB7DC-9D40-44C2-8742-A17A0EB899C3}" name="show_universal_layout_x_axes"/>
-    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_x_axis_args" dataDxfId="20">
+    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_x_axis_args" dataDxfId="19">
       <calculatedColumnFormula>IF(table_7_2[[#This Row],[show_universal_layout_x_axes]], OFFSET(table_7_1[[universal_layout_x_axis_args]:[universal_layout_x_axis_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{641C7B24-D16A-472B-B06C-7348DDBC60AA}" name="universal_layout_max_tick_args" dataDxfId="19">
+    <tableColumn id="14" xr3:uid="{641C7B24-D16A-472B-B06C-7348DDBC60AA}" name="universal_layout_max_tick_args" dataDxfId="18">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_max_tick_args]:[universal_layout_max_tick_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="17">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{8B58B2DF-3EB7-4D4E-A96D-1BED892121E3}" name="format"/>
-    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="18">
+    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="16">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2444,46 +2444,46 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:O64" totalsRowShown="0" headerRowDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:O64" totalsRowShown="0" headerRowDxfId="15">
   <autoFilter ref="A62:O64" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="16"/>
-    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="15">
+    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="13">
       <calculatedColumnFormula>OFFSET(table_4_2[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="14">
+    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="12">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="13">
+    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="11">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="12">
+    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="10">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="11">
+    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="10">
+    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="8">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="7">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BF1D3FB1-D45A-4909-BA3E-BB6993D39E6E}" name="universal_layout_y_axis_args" dataDxfId="8">
+    <tableColumn id="12" xr3:uid="{BF1D3FB1-D45A-4909-BA3E-BB6993D39E6E}" name="universal_layout_y_axis_args" dataDxfId="6">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_y_axis_args]:[universal_layout_y_axis_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{8D9288FF-05A5-4B58-AC7F-2C4096A25202}" name="show_universal_layout_x_axes" dataDxfId="7"/>
-    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_x_axis_args" dataDxfId="6">
+    <tableColumn id="13" xr3:uid="{8D9288FF-05A5-4B58-AC7F-2C4096A25202}" name="show_universal_layout_x_axes" dataDxfId="5"/>
+    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_x_axis_args" dataDxfId="4">
       <calculatedColumnFormula>IF(table_7_3[[#This Row],[show_universal_layout_x_axes]], OFFSET(table_7_1[[universal_layout_x_axis_args]:[universal_layout_x_axis_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{FD5F951D-27C2-4E6B-B33F-D83C250C9CC4}" name="universal_layout_max_tick_args" dataDxfId="5">
+    <tableColumn id="14" xr3:uid="{FD5F951D-27C2-4E6B-B33F-D83C250C9CC4}" name="universal_layout_max_tick_args" dataDxfId="3">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_max_tick_args]:[universal_layout_max_tick_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="2">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_3[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{0AB61192-5C37-4578-ADFD-BAE568B914C5}" name="format" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="4">
+    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="0">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], " ", table_7_3[[#This Row],[universal_layout_y_axis_args]], " ", table_7_3[[#This Row],[universal_layout_x_axis_args]], " ", table_7_3[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -3211,7 +3211,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -13583,7 +13583,7 @@
         <v>1</v>
       </c>
       <c r="D162" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E162" t="s">
         <v>124</v>
@@ -13637,7 +13637,7 @@
         <v>1</v>
       </c>
       <c r="D163" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E163" t="s">
         <v>124</v>
@@ -13691,7 +13691,7 @@
         <v>1</v>
       </c>
       <c r="D164" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E164" t="s">
         <v>124</v>
@@ -13745,7 +13745,7 @@
         <v>14</v>
       </c>
       <c r="D165" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E165" t="s">
         <v>124</v>
@@ -13799,7 +13799,7 @@
         <v>14</v>
       </c>
       <c r="D166" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E166" t="s">
         <v>124</v>
@@ -13853,7 +13853,7 @@
         <v>14</v>
       </c>
       <c r="D167" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E167" t="s">
         <v>124</v>
@@ -13907,7 +13907,7 @@
         <v>1</v>
       </c>
       <c r="D168" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E168" t="s">
         <v>124</v>
@@ -13961,7 +13961,7 @@
         <v>1</v>
       </c>
       <c r="D169" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E169" t="s">
         <v>124</v>
@@ -14015,7 +14015,7 @@
         <v>1</v>
       </c>
       <c r="D170" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E170" t="s">
         <v>124</v>
@@ -14069,7 +14069,7 @@
         <v>14</v>
       </c>
       <c r="D171" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E171" t="s">
         <v>124</v>
@@ -14123,7 +14123,7 @@
         <v>14</v>
       </c>
       <c r="D172" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E172" t="s">
         <v>124</v>
@@ -14177,7 +14177,7 @@
         <v>14</v>
       </c>
       <c r="D173" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E173" t="s">
         <v>124</v>
@@ -14222,7 +14222,7 @@
     </row>
     <row r="175" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B175" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="176" spans="1:15" x14ac:dyDescent="0.25">
@@ -18262,7 +18262,7 @@
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H58" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.25">
@@ -21410,7 +21410,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -21472,7 +21472,7 @@
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
@@ -22853,7 +22853,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
@@ -22889,7 +22889,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -22996,10 +22996,10 @@
         <v>105</v>
       </c>
       <c r="M1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>168</v>
@@ -25483,10 +25483,10 @@
         <v>105</v>
       </c>
       <c r="M43" t="s">
+        <v>187</v>
+      </c>
+      <c r="N43" t="s">
         <v>188</v>
-      </c>
-      <c r="N43" t="s">
-        <v>189</v>
       </c>
       <c r="O43" t="s">
         <v>168</v>
@@ -26226,7 +26226,7 @@
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -26328,7 +26328,7 @@
         <v>176</v>
       </c>
       <c r="B1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
@@ -26339,7 +26339,7 @@
         <v>87</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>134</v>
@@ -26421,7 +26421,7 @@
         <v>87</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>134</v>
@@ -26629,7 +26629,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -26678,8 +26678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:AB67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
-      <selection activeCell="M64" sqref="M64"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26709,7 +26709,7 @@
         <v>175</v>
       </c>
       <c r="D1" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>176</v>
@@ -26719,13 +26719,13 @@
         <v>universal</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H1">
         <v>2400</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="J1">
         <v>1800</v>
@@ -26772,46 +26772,46 @@
         <v>171</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="S2" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="U2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="Z2" s="1" t="s">
         <v>139</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AB2" s="1" t="s">
         <v>168</v>
@@ -26927,14 +26927,14 @@
       </c>
       <c r="Z3" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB3" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5   --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 21.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5   --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 21.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
@@ -27047,14 +27047,14 @@
       </c>
       <c r="Z4" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB4" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
@@ -27167,14 +27167,14 @@
       </c>
       <c r="Z5" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB5" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -27287,14 +27287,14 @@
       </c>
       <c r="Z6" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB6" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5   --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 21.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5   --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 21.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -27407,14 +27407,14 @@
       </c>
       <c r="Z7" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA7" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB7" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -27527,14 +27527,14 @@
       </c>
       <c r="Z8" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB8" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -27647,14 +27647,14 @@
       </c>
       <c r="Z9" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
@@ -27767,14 +27767,14 @@
       </c>
       <c r="Z10" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB10" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -27887,14 +27887,14 @@
       </c>
       <c r="Z11" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB11" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -28007,14 +28007,14 @@
       </c>
       <c r="Z12" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB12" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.25">
@@ -28127,14 +28127,14 @@
       </c>
       <c r="Z13" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA13" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB13" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
@@ -28247,14 +28247,14 @@
       </c>
       <c r="Z14" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB14" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -28367,14 +28367,14 @@
       </c>
       <c r="Z15" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB15" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5   --universal_layout_x_axis_deletion_y_pos -21.5 --universal_layout_x_axis_insertion_y_pos 19.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5   --universal_layout_x_axis_deletion_y_pos -21.5 --universal_layout_x_axis_insertion_y_pos 19.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -28487,14 +28487,14 @@
       </c>
       <c r="Z16" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA16" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB16" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
@@ -28607,14 +28607,14 @@
       </c>
       <c r="Z17" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB17" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="18" spans="1:28" x14ac:dyDescent="0.25">
@@ -28727,14 +28727,14 @@
       </c>
       <c r="Z18" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB18" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5   --universal_layout_x_axis_deletion_y_pos -21.5 --universal_layout_x_axis_insertion_y_pos 19.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5   --universal_layout_x_axis_deletion_y_pos -21.5 --universal_layout_x_axis_insertion_y_pos 19.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="19" spans="1:28" x14ac:dyDescent="0.25">
@@ -28847,14 +28847,14 @@
       </c>
       <c r="Z19" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB19" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="20" spans="1:28" x14ac:dyDescent="0.25">
@@ -28967,14 +28967,14 @@
       </c>
       <c r="Z20" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA20" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB20" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="21" spans="1:28" x14ac:dyDescent="0.25">
@@ -29087,14 +29087,14 @@
       </c>
       <c r="Z21" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB21" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="22" spans="1:28" x14ac:dyDescent="0.25">
@@ -29207,14 +29207,14 @@
       </c>
       <c r="Z22" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB22" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="23" spans="1:28" x14ac:dyDescent="0.25">
@@ -29327,14 +29327,14 @@
       </c>
       <c r="Z23" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB23" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="24" spans="1:28" x14ac:dyDescent="0.25">
@@ -29447,14 +29447,14 @@
       </c>
       <c r="Z24" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB24" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="25" spans="1:28" x14ac:dyDescent="0.25">
@@ -29567,14 +29567,14 @@
       </c>
       <c r="Z25" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB25" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="26" spans="1:28" x14ac:dyDescent="0.25">
@@ -29687,14 +29687,14 @@
       </c>
       <c r="Z26" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB26" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="27" spans="1:28" x14ac:dyDescent="0.25">
@@ -29807,14 +29807,14 @@
       </c>
       <c r="Z27" s="9" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA27" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB27" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_30bpDown -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
@@ -29927,14 +29927,14 @@
       </c>
       <c r="Z28" s="9" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA28" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB28" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch_30bpDown -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="29" spans="1:28" x14ac:dyDescent="0.25">
@@ -30047,14 +30047,14 @@
       </c>
       <c r="Z29" s="9" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA29" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB29" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv_30bpDown -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="30" spans="1:28" x14ac:dyDescent="0.25">
@@ -30167,14 +30167,14 @@
       </c>
       <c r="Z30" s="9" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA30" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB30" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_30bpDown -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="31" spans="1:28" x14ac:dyDescent="0.25">
@@ -30287,14 +30287,14 @@
       </c>
       <c r="Z31" s="9" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA31" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB31" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch_30bpDown -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="32" spans="1:28" x14ac:dyDescent="0.25">
@@ -30407,14 +30407,14 @@
       </c>
       <c r="Z32" s="9" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA32" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB32" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv_30bpDown -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="33" spans="1:28" x14ac:dyDescent="0.25">
@@ -30527,14 +30527,14 @@
       </c>
       <c r="Z33" s="9" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA33" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB33" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_30bpDown -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="34" spans="1:28" x14ac:dyDescent="0.25">
@@ -30647,14 +30647,14 @@
       </c>
       <c r="Z34" s="9" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA34" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB34" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch_30bpDown -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="35" spans="1:28" x14ac:dyDescent="0.25">
@@ -30767,14 +30767,14 @@
       </c>
       <c r="Z35" s="9" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA35" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB35" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv_30bpDown -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="36" spans="1:28" x14ac:dyDescent="0.25">
@@ -30887,14 +30887,14 @@
       </c>
       <c r="Z36" s="9" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA36" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB36" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_30bpDown -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="37" spans="1:28" x14ac:dyDescent="0.25">
@@ -31007,14 +31007,14 @@
       </c>
       <c r="Z37" s="9" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA37" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB37" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch_30bpDown -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="38" spans="1:28" x14ac:dyDescent="0.25">
@@ -31127,14 +31127,14 @@
       </c>
       <c r="Z38" s="9" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA38" s="9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB38" s="9" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv_30bpDown -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="39" spans="1:28" x14ac:dyDescent="0.25">
@@ -31247,14 +31247,14 @@
       </c>
       <c r="Z39" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA39" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB39" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5   --universal_layout_x_axis_deletion_y_pos -16.5 --universal_layout_x_axis_insertion_y_pos 26.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5   --universal_layout_x_axis_deletion_y_pos -16.5 --universal_layout_x_axis_insertion_y_pos 26.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
     <row r="40" spans="1:28" x14ac:dyDescent="0.25">
@@ -31367,14 +31367,14 @@
       </c>
       <c r="Z40" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB40" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
     <row r="41" spans="1:28" x14ac:dyDescent="0.25">
@@ -31487,14 +31487,14 @@
       </c>
       <c r="Z41" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA41" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB41" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
     <row r="42" spans="1:28" x14ac:dyDescent="0.25">
@@ -31607,14 +31607,14 @@
       </c>
       <c r="Z42" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/individual/png</v>
+        <v>plots/graphs/universal/individual/html</v>
       </c>
       <c r="AA42" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="AB42" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
     <row r="44" spans="1:28" x14ac:dyDescent="0.25">
@@ -31637,28 +31637,28 @@
         <v>171</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I44" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="J44" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="J44" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="K44" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M44" s="1" t="s">
         <v>139</v>
       </c>
       <c r="N44" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O44" s="1" t="s">
         <v>168</v>
@@ -31713,14 +31713,14 @@
       </c>
       <c r="M45" s="2" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O45" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="46" spans="1:28" x14ac:dyDescent="0.25">
@@ -31772,14 +31772,14 @@
       </c>
       <c r="M46" s="2" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O46" s="2" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="47" spans="1:28" x14ac:dyDescent="0.25">
@@ -31831,14 +31831,14 @@
       </c>
       <c r="M47" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N47" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O47" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="48" spans="1:28" x14ac:dyDescent="0.25">
@@ -31890,14 +31890,14 @@
       </c>
       <c r="M48" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O48" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
@@ -31949,14 +31949,14 @@
       </c>
       <c r="M49" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N49" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O49" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
@@ -32008,14 +32008,14 @@
       </c>
       <c r="M50" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N50" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O50" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
@@ -32067,14 +32067,14 @@
       </c>
       <c r="M51" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N51" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O51" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
@@ -32126,14 +32126,14 @@
       </c>
       <c r="M52" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N52" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O52" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
@@ -32185,14 +32185,14 @@
       </c>
       <c r="M53" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N53" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O53" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
@@ -32244,14 +32244,14 @@
       </c>
       <c r="M54" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N54" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O54" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
@@ -32303,14 +32303,14 @@
       </c>
       <c r="M55" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N55" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O55" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
@@ -32362,14 +32362,14 @@
       </c>
       <c r="M56" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N56" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O56" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
@@ -32421,14 +32421,14 @@
       </c>
       <c r="M57" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N57" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O57" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -32480,14 +32480,14 @@
       </c>
       <c r="M58" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N58" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O58" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
@@ -32539,14 +32539,14 @@
       </c>
       <c r="M59" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N59" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O59" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
@@ -32598,14 +32598,14 @@
       </c>
       <c r="M60" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N60" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O60" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
@@ -32628,28 +32628,28 @@
         <v>171</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="I62" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="J62" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="J62" s="1" t="s">
-        <v>196</v>
-      </c>
       <c r="K62" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M62" s="1" t="s">
         <v>139</v>
       </c>
       <c r="N62" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="O62" s="1" t="s">
         <v>168</v>
@@ -32704,14 +32704,14 @@
       </c>
       <c r="M63" s="2" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_3[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O63" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], " ", table_7_3[[#This Row],[universal_layout_y_axis_args]], " ", table_7_3[[#This Row],[universal_layout_x_axis_args]], " ", table_7_3[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
@@ -32763,70 +32763,70 @@
       </c>
       <c r="M64" s="2" t="str">
         <f>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_3[[#This Row],[format]], "/", var_7_ext)</f>
-        <v>plots/graphs/universal/combined/png</v>
+        <v>plots/graphs/universal/combined/html</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O64" s="2" t="str">
         <f ca="1">_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], " ", table_7_3[[#This Row],[universal_layout_y_axis_args]], " ", table_7_3[[#This Row],[universal_layout_x_axis_args]], " ", table_7_3[[#This Row],[universal_layout_max_tick_args]])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="str">
         <f ca="1">_xlfn.TEXTJOIN(CHAR(10), TRUE, AB3:AB26,AB39:AB42, table_7_2[command], table_7_3[command])</f>
-        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5   --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 21.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5   --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 21.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5   --universal_layout_x_axis_deletion_y_pos -21.5 --universal_layout_x_axis_insertion_y_pos 19.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5   --universal_layout_x_axis_deletion_y_pos -21.5 --universal_layout_x_axis_insertion_y_pos 19.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/universal/individual/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5   --universal_layout_x_axis_deletion_y_pos -16.5 --universal_layout_x_axis_insertion_y_pos 26.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/universal/individual/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSB_AB -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_A -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
-python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/universal/combined/png --layout_dir layouts/universal/1DSB_B -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
-python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/universal/combined/png --layout_dir layouts/universal/2DSBanti_CD -ext png --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
+        <v>python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5   --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 21.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5   --universal_layout_x_axis_deletion_y_pos -20.5 --universal_layout_x_axis_insertion_y_pos 21.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5   --universal_layout_x_axis_deletion_y_pos -21.5 --universal_layout_x_axis_insertion_y_pos 19.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5   --universal_layout_x_axis_deletion_y_pos -21.5 --universal_layout_x_axis_insertion_y_pos 19.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_branch -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_cmv -o plots/graphs/universal/individual/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5   --universal_layout_x_axis_deletion_y_pos -16.5 --universal_layout_x_axis_insertion_y_pos 26.5 --universal_layout_x_axis_x_range -11.5 11.5  --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_splicing -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_splicing -o plots/graphs/universal/individual/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R1_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgAB_R2_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSB_AB -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 22  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 20.5    --universal_layout_y_axis_deletion_max_tick 17 --universal_layout_y_axis_insertion_max_tick 7
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgA_R1_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgA_R1_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_A -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -23 20  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -20.5 18.5    --universal_layout_y_axis_deletion_max_tick 19 --universal_layout_y_axis_insertion_max_tick 6
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgB_R2_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_branch -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
+python 2_graph_processing/plot_graph.py -i libraries_4/KO_sgB_R2_sense_cmv -o plots/graphs/universal/combined/html --layout_dir layouts/universal/1DSB_B -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -22 16  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -19.5 14.5    --universal_layout_y_axis_deletion_max_tick 18 --universal_layout_y_axis_insertion_max_tick 5
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R1_antisense_splicing -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8
+python 2_graph_processing/plot_graph.py -i libraries_4/WT_sgCD_R2_antisense_splicing -o plots/graphs/universal/combined/html --layout_dir layouts/universal/2DSBanti_CD -ext html --layout universal --reverse_complement  --width 2400 --height 1800 --range_x -12 13 --range_y -18 27  --universal_layout_y_axis_x_pos 12 --universal_layout_y_axis_y_range -15.5 25.5    --universal_layout_y_axis_deletion_max_tick 14 --universal_layout_y_axis_insertion_max_tick 8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Make modifications for new antisense data.
</commit_message>
<xml_diff>
--- a/analyze_nhej/libinfo.xlsx
+++ b/analyze_nhej/libinfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\analyze_nhej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8E3D80A-163C-49F5-861A-6A42A1F26B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C30D49-FB63-4CF2-ADD4-60C53E33FF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" firstSheet="2" activeTab="8" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1623" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="211">
   <si>
     <t>yjl217</t>
   </si>
@@ -699,6 +699,30 @@
   </si>
   <si>
     <t>html</t>
+  </si>
+  <si>
+    <t>yjl349</t>
+  </si>
+  <si>
+    <t>yjl350</t>
+  </si>
+  <si>
+    <t>yjl351</t>
+  </si>
+  <si>
+    <t>yjl352</t>
+  </si>
+  <si>
+    <t>yjl353</t>
+  </si>
+  <si>
+    <t>yjl354</t>
+  </si>
+  <si>
+    <t>yjl355</t>
+  </si>
+  <si>
+    <t>yjl356</t>
   </si>
 </sst>
 </file>
@@ -2071,8 +2095,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}" name="table_1_2" displayName="table_1_2" ref="A1:D108" totalsRowShown="0">
-  <autoFilter ref="A1:D108" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}" name="table_1_2" displayName="table_1_2" ref="A1:D116" totalsRowShown="0">
+  <autoFilter ref="A1:D116" xr:uid="{70502F2F-AE2C-4D63-ADF7-F65702652EBF}"/>
   <tableColumns count="4">
     <tableColumn id="2" xr3:uid="{BB99DCDA-08D4-474A-ABC3-5229CEAF80CF}" name="id" dataDxfId="217">
       <calculatedColumnFormula>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</calculatedColumnFormula>
@@ -3221,10 +3245,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5334D33C-3E16-4C4F-BA76-1F06B33FAC0B}">
-  <dimension ref="A1:D108"/>
+  <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D109" sqref="D109:D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4849,6 +4873,126 @@
       </c>
       <c r="D108">
         <v>6372479</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <f>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</f>
+        <v>349</v>
+      </c>
+      <c r="B109" t="s">
+        <v>203</v>
+      </c>
+      <c r="C109">
+        <v>6302370</v>
+      </c>
+      <c r="D109">
+        <v>6161112</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <f>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</f>
+        <v>350</v>
+      </c>
+      <c r="B110" t="s">
+        <v>204</v>
+      </c>
+      <c r="C110">
+        <v>5988345</v>
+      </c>
+      <c r="D110">
+        <v>5856132</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <f>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</f>
+        <v>351</v>
+      </c>
+      <c r="B111" t="s">
+        <v>205</v>
+      </c>
+      <c r="C111">
+        <v>5741048</v>
+      </c>
+      <c r="D111">
+        <v>5613583</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <f>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</f>
+        <v>352</v>
+      </c>
+      <c r="B112" t="s">
+        <v>206</v>
+      </c>
+      <c r="C112">
+        <v>5405939</v>
+      </c>
+      <c r="D112">
+        <v>5281487</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <f>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</f>
+        <v>353</v>
+      </c>
+      <c r="B113" t="s">
+        <v>207</v>
+      </c>
+      <c r="C113">
+        <v>4177291</v>
+      </c>
+      <c r="D113">
+        <v>4062558</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <f>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</f>
+        <v>354</v>
+      </c>
+      <c r="B114" t="s">
+        <v>208</v>
+      </c>
+      <c r="C114">
+        <v>4647120</v>
+      </c>
+      <c r="D114">
+        <v>4535123</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <f>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</f>
+        <v>355</v>
+      </c>
+      <c r="B115" t="s">
+        <v>209</v>
+      </c>
+      <c r="C115">
+        <v>4405688</v>
+      </c>
+      <c r="D115">
+        <v>4280724</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <f>INT(MID(table_1_2[[#This Row],[library]], 4, 10))</f>
+        <v>356</v>
+      </c>
+      <c r="B116" t="s">
+        <v>210</v>
+      </c>
+      <c r="C116">
+        <v>5054324</v>
+      </c>
+      <c r="D116">
+        <v>4926338</v>
       </c>
     </row>
   </sheetData>
@@ -4863,8 +5007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F1EACD-27DC-4973-8E3A-9162F610D9C4}">
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView topLeftCell="B157" workbookViewId="0">
-      <selection activeCell="O173" sqref="O173"/>
+    <sheetView topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A153" sqref="A153:XFD153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -26678,7 +26822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1375107-D76A-4386-B771-6693BBF75061}">
   <dimension ref="A1:AB67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update the library data files for generating scripts.
</commit_message>
<xml_diff>
--- a/analyze_nhej/libinfo.xlsx
+++ b/analyze_nhej/libinfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\analyze_nhej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C30D49-FB63-4CF2-ADD4-60C53E33FF70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6A790A-B591-463D-ACD6-329F1AC175D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
   <sheets>
     <sheet name="globals" sheetId="3" r:id="rId1"/>
@@ -3247,7 +3247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5334D33C-3E16-4C4F-BA76-1F06B33FAC0B}">
   <dimension ref="A1:D116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+    <sheetView topLeftCell="A100" workbookViewId="0">
       <selection activeCell="D109" sqref="D109:D116"/>
     </sheetView>
   </sheetViews>
@@ -5007,8 +5007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F1EACD-27DC-4973-8E3A-9162F610D9C4}">
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A153" sqref="A153:XFD153"/>
+    <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
+      <selection activeCell="J146" sqref="J146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5024,7 +5024,7 @@
     <col min="9" max="9" width="25.140625" customWidth="1"/>
     <col min="10" max="10" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="31.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" customWidth="1"/>
     <col min="13" max="13" width="13.28515625" customWidth="1"/>
     <col min="14" max="14" width="22.28515625" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
Add more data to script generation. Start generate scripts.
</commit_message>
<xml_diff>
--- a/analyze_nhej/libinfo.xlsx
+++ b/analyze_nhej/libinfo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tchan\Code\SCMB_Project\RNA-mediated_DSB_repair\analyze_nhej\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6A790A-B591-463D-ACD6-329F1AC175D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEA7241-B263-4CFF-97D1-3329D5D766FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{2091B41C-DDD2-4E50-B30A-30FF3CA370E5}"/>
   </bookViews>
@@ -843,6 +843,9 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{FFD19645-61C4-4244-A560-0232B787F38C}"/>
   </cellStyles>
   <dxfs count="218">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -2052,9 +2055,6 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
@@ -2110,50 +2110,50 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:O41" totalsRowShown="0" headerRowDxfId="114">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}" name="table_5_1" displayName="table_5_1" ref="A1:O41" totalsRowShown="0" headerRowDxfId="115">
   <autoFilter ref="A1:O41" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="15">
-    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="113"/>
-    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="112">
+    <tableColumn id="25" xr3:uid="{43F57146-0E56-46F3-A0E3-717A41010F4A}" name="index" dataDxfId="114"/>
+    <tableColumn id="1" xr3:uid="{B0B3F6B0-7577-49AC-B865-1E873B4DC53C}" name="dir" dataDxfId="113">
       <calculatedColumnFormula>table_3_1[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="111">
+    <tableColumn id="13" xr3:uid="{D04F356F-9288-416D-ACDA-6BFE128B70D7}" name="control" dataDxfId="112">
       <calculatedColumnFormula>table_3_1[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="110">
+    <tableColumn id="2" xr3:uid="{9C168B22-F534-40D4-947C-918239C33FD9}" name="ref" dataDxfId="111">
       <calculatedColumnFormula>table_3_1[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="109">
+    <tableColumn id="3" xr3:uid="{6F64477B-0C66-4251-9156-22307A6D70A0}" name="dsb_pos" dataDxfId="110">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="108">
+    <tableColumn id="4" xr3:uid="{D037F4F2-543F-4D7D-AB36-0B253FD61B0D}" name="dsb_type" dataDxfId="109">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="107">
+    <tableColumn id="12" xr3:uid="{407AC5E6-13CB-409A-8E78-64B8CC121882}" name="dsb_type_command" dataDxfId="108">
       <calculatedColumnFormula>table_3_1[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="106">
+    <tableColumn id="5" xr3:uid="{1A24C844-2A10-4394-818F-0C25A569B414}" name="strand" dataDxfId="107">
       <calculatedColumnFormula>table_3_1[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="105">
+    <tableColumn id="6" xr3:uid="{4F0A02F9-5555-489E-BA41-E3CBF81D1114}" name="hguide" dataDxfId="106">
       <calculatedColumnFormula>table_3_1[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="104">
+    <tableColumn id="7" xr3:uid="{FAE741F2-7C1B-41F2-8875-9F7A2EF40A54}" name="cell" dataDxfId="105">
       <calculatedColumnFormula>table_3_1[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="103">
+    <tableColumn id="8" xr3:uid="{FE3ED128-2534-43D1-9244-11AB1FB57650}" name="treatment" dataDxfId="104">
       <calculatedColumnFormula>table_3_1[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="102">
+    <tableColumn id="9" xr3:uid="{65ACBC9C-0EC8-4074-B310-05F4B70BFAD5}" name="subst_type" dataDxfId="103">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1D971CC2-F378-4E62-9759-F7168770AA64}" name="label_type" dataDxfId="101">
+    <tableColumn id="11" xr3:uid="{1D971CC2-F378-4E62-9759-F7168770AA64}" name="label_type" dataDxfId="102">
       <calculatedColumnFormula>IF(table_5_1[[#This Row],[control]]="30bpDown", "absolute", "relative")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{8241431B-CE1C-49A4-B13E-77512D442338}" name="reverse_pos" dataDxfId="100">
+    <tableColumn id="14" xr3:uid="{8241431B-CE1C-49A4-B13E-77512D442338}" name="reverse_pos" dataDxfId="101">
       <calculatedColumnFormula>IF(table_5_1[[#This Row],[strand]]="R2", " -rp ", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="99">
+    <tableColumn id="10" xr3:uid="{F80F6FB9-4F35-4819-8285-D77131C6EFCE}" name="command" dataDxfId="100">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_1[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_1[[#This Row],[reverse_pos]], " -lt ", table_5_1[[#This Row],[label_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2166,46 +2166,46 @@
   <autoFilter ref="A43:O55" xr:uid="{D74A5276-1A50-4DA1-9131-9669404C8622}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{8AC09A63-4226-4C75-8801-68CF93C0F078}" name="index"/>
-    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="98">
+    <tableColumn id="2" xr3:uid="{77584C42-D70C-48A4-979A-F4DEA0B31542}" name="dir" dataDxfId="99">
       <calculatedColumnFormula>table_3_2[[#This Row],[dir]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="97">
+    <tableColumn id="3" xr3:uid="{483E3D73-4059-4B65-84EC-5DC4E7008F35}" name="control" dataDxfId="98">
       <calculatedColumnFormula>table_3_2[[#This Row],[control]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="96">
+    <tableColumn id="4" xr3:uid="{5859A8DB-4C52-4451-BBB6-C6BEBF497540}" name="ref" dataDxfId="97">
       <calculatedColumnFormula>table_3_2[[#This Row],[ref]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="95">
+    <tableColumn id="5" xr3:uid="{06FC4099-C18C-436C-B1E6-9739B71C7F22}" name="dsb_pos" dataDxfId="96">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_pos]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="94">
+    <tableColumn id="6" xr3:uid="{8F043A8E-C5E7-4596-AE13-3E495C6DB33E}" name="dsb_type" dataDxfId="95">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="93">
+    <tableColumn id="7" xr3:uid="{E2DB136E-6FA9-4095-8B91-F094974333AF}" name="dsb_type_command" dataDxfId="94">
       <calculatedColumnFormula>table_3_2[[#This Row],[dsb_type_command]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="92">
+    <tableColumn id="8" xr3:uid="{55CDC54E-3E43-4365-B1C9-5359F747A157}" name="strand" dataDxfId="93">
       <calculatedColumnFormula>table_3_2[[#This Row],[strand]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="91">
+    <tableColumn id="9" xr3:uid="{056BD8A0-CC40-4C61-9F22-EE7382045F66}" name="hguide" dataDxfId="92">
       <calculatedColumnFormula>table_3_2[[#This Row],[hguide]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="90">
+    <tableColumn id="10" xr3:uid="{489E156D-888A-4DDC-BB23-A4721D588249}" name="cell" dataDxfId="91">
       <calculatedColumnFormula>table_3_2[[#This Row],[cell]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="89">
+    <tableColumn id="11" xr3:uid="{0F1B5F9E-B10D-4258-9052-90BCDC89F0B0}" name="treatment" dataDxfId="90">
       <calculatedColumnFormula>table_3_2[[#This Row],[treatment]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="88">
+    <tableColumn id="12" xr3:uid="{A2723EF6-80E8-4D8D-A6DC-7556C1996222}" name="subst_type" dataDxfId="89">
       <calculatedColumnFormula>"with"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{F5E6916D-F1BC-48E0-9E73-728C62F32A69}" name="label_type" dataDxfId="87">
+    <tableColumn id="14" xr3:uid="{F5E6916D-F1BC-48E0-9E73-728C62F32A69}" name="label_type" dataDxfId="88">
       <calculatedColumnFormula>IF(table_5_2[[#This Row],[control]]="30bpDown", "absolute", "relative")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{EF50F256-FFB6-49D0-8199-D7AB5C783AD5}" name="reverse_pos" dataDxfId="86">
+    <tableColumn id="15" xr3:uid="{EF50F256-FFB6-49D0-8199-D7AB5C783AD5}" name="reverse_pos" dataDxfId="87">
       <calculatedColumnFormula>IF(table_5_2[[#This Row],[strand]]="R2", " -rp ", "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="85">
+    <tableColumn id="13" xr3:uid="{02531CCA-6CDE-42BA-80E3-31C0F97A3546}" name="command" dataDxfId="86">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_histogram_3d.py ", "-i ", libraries_4, "/", table_5_2[[#This Row],[dir]], " -o ", histogram_3d, "/", table_5_2[[#This Row],[reverse_pos]], " -lt ", table_5_2[[#This Row],[label_type]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2214,36 +2214,36 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="84">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}" name="table_6_3" displayName="table_6_3" ref="A3:I4" totalsRowShown="0" headerRowDxfId="85">
   <autoFilter ref="A3:I4" xr:uid="{C8C4C06E-000E-41C5-BD07-871BB3291C48}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="83"/>
-    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="82">
+    <tableColumn id="25" xr3:uid="{D7EEB429-5A34-4903-8247-E1BD5C0098AE}" name="index" dataDxfId="84"/>
+    <tableColumn id="18" xr3:uid="{BACD6182-9E09-4A02-A171-8DFCB7543380}" name="dir" dataDxfId="83">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="81">
+    <tableColumn id="2" xr3:uid="{39C35B5A-7D06-4895-BF0F-A803A5F94E2E}" name="reverse_complement" dataDxfId="82">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 12, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="80">
+    <tableColumn id="13" xr3:uid="{F617BC3E-90A8-4E63-B2A4-EAC9DE705FC7}" name="control" dataDxfId="81">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="79">
+    <tableColumn id="4" xr3:uid="{8E20D9FC-49B1-428A-AC5E-AEDADB1473AC}" name="dsb_type" dataDxfId="80">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], 12 * (table_6_3[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="33" xr3:uid="{8FF7E83A-9135-4A64-965C-48368A6C0367}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], 12 * (table_6_3[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="78">
+    <tableColumn id="9" xr3:uid="{FB278FFE-A956-4B0C-8CC3-6A0324CBCA11}" name="subst_type" dataDxfId="79">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="77">
+    <tableColumn id="19" xr3:uid="{E4089767-2E77-4296-9392-7BCD64E1E62D}" name="dir_out" dataDxfId="78">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_3[[#This Row],[dsb_type]], "_", table_6_3[[#This Row],[hguide]], IF(table_6_3[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_3[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="76">
+    <tableColumn id="10" xr3:uid="{8BD09F85-30B0-46CA-A0E3-2CC4F3FB2BD0}" name="command" dataDxfId="77">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_3[[#This Row],[dir]], IF(NOT(ISNA(table_6_3[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_3[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_3[[#This Row],[dir_out]], " --subst_type ", table_6_3[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2252,32 +2252,32 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}" name="table_6_4" displayName="table_6_4" ref="A7:I9" totalsRowShown="0" headerRowDxfId="76">
   <autoFilter ref="A7:I9" xr:uid="{43CAA14F-D870-4D8C-8372-DFAF0C2B719D}"/>
   <tableColumns count="9">
-    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="74"/>
-    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="73">
+    <tableColumn id="25" xr3:uid="{4FA5A2E4-C9F7-4673-98E1-BCCE618B100D}" name="index" dataDxfId="75"/>
+    <tableColumn id="18" xr3:uid="{155653FE-38BD-4542-A5AE-2B40B0FD52C7}" name="dir" dataDxfId="74">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 6, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="72">
+    <tableColumn id="34" xr3:uid="{05E960C2-864E-41C3-A84E-DF767C09AA42}" name="reverse_complement" dataDxfId="73">
       <calculatedColumnFormula>IF(table_6_4[[#This Row],[hguide]]="A",NA(), IF(var_6_layout = "universal", "1 1 1 1 1 1", NA()))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="71">
+    <tableColumn id="13" xr3:uid="{9EA58FA8-5496-4600-905A-95909513339B}" name="control" dataDxfId="72">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="70">
+    <tableColumn id="4" xr3:uid="{46390A5F-98AD-4211-85B4-A4DD8E31C40C}" name="dsb_type" dataDxfId="71">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="35" xr3:uid="{5BD83012-469D-4202-9584-AA182CDF11F9}" name="hguide">
       <calculatedColumnFormula array="1">OFFSET(table_3_1[[hguide]:[hguide]], var_6_1dsb_offset + 6 * (table_6_4[[#This Row],[index]:[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="69">
+    <tableColumn id="9" xr3:uid="{123049FA-F284-452C-8FDD-63F409D9967F}" name="subst_type" dataDxfId="70">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="68">
+    <tableColumn id="19" xr3:uid="{CFCDDB26-095C-4395-82E2-37B45B0CDEAD}" name="dir_out" dataDxfId="69">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_4[[#This Row],[dsb_type]], "_", table_6_4[[#This Row],[hguide]], IF(table_6_4[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_4[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="67">
+    <tableColumn id="10" xr3:uid="{DC6C9CBA-5796-4FFE-878D-BB47DC276187}" name="command" dataDxfId="68">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_4[[#This Row],[dir]], IF(NOT(ISNA(table_6_4[[#This Row],[reverse_complement]])), _xlfn.CONCAT(" -rc ", table_6_4[[#This Row],[reverse_complement]]), ""), " -o ", layouts, "/", table_6_4[[#This Row],[dir_out]], " --subst_type ", table_6_4[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2286,36 +2286,36 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="66" headerRowBorderDxfId="65" tableBorderDxfId="64">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}" name="table_6_5" displayName="table_6_5" ref="A12:I13" totalsRowShown="0" headerRowDxfId="67" headerRowBorderDxfId="66" tableBorderDxfId="65">
   <autoFilter ref="A12:I13" xr:uid="{F5E44D84-0923-4099-A9D7-D0D16C2D6571}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0F421990-E775-4F35-92AF-6BA19E0E8AEE}" name="index"/>
-    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="63">
+    <tableColumn id="2" xr3:uid="{81FE7256-F482-4A2C-902D-871C80C1D881}" name="dir" dataDxfId="64">
       <calculatedColumnFormula array="1">TRIM(SUBSTITUTE(_xlfn.CONCAT(" ", _xlfn.TEXTJOIN(" ", TRUE, OFFSET(table_3_1[[dir]:[dir]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0, 4, 1))), " ", _xlfn.CONCAT(" ", libraries_4, "/")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="62">
+    <tableColumn id="3" xr3:uid="{E9F8E6A0-B4A7-475B-9ED2-9F2A4A9EB628}" name="strand" dataDxfId="63">
       <calculatedColumnFormula array="1">_xlfn.TEXTJOIN(
   " ",
   TRUE,
   IF(OFFSET(table_3_1[[strand]:[strand]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]:[index]] - 1), 0,4, 1) = "R1", 0, 1)
 )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="61">
+    <tableColumn id="6" xr3:uid="{70821CEE-FFC4-44AB-ACF6-DA81A4B053E6}" name="control" dataDxfId="62">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="60">
+    <tableColumn id="5" xr3:uid="{FA9180EA-3AA0-451A-ACAC-78776C7CB75D}" name="dsb_type" dataDxfId="61">
       <calculatedColumnFormula>OFFSET(table_3_1[dsb_type], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="8" xr3:uid="{E0783723-9246-4BF6-A5DA-E000EA1E5E87}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="59">
+    <tableColumn id="4" xr3:uid="{DE820E4E-FF8B-435B-B07F-D397029AF597}" name="hguide" dataDxfId="60">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], var_6_anti_offset + 4 * (table_6_5[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="58">
+    <tableColumn id="9" xr3:uid="{3D97DBDD-03E9-4A6C-BADA-D01B27A8EE51}" name="dir_out" dataDxfId="59">
       <calculatedColumnFormula>_xlfn.CONCAT(var_6_layout, "/", table_6_5[[#This Row],[dsb_type]], "_", table_6_5[[#This Row],[hguide]], IF(table_6_5[[#This Row],[control]]&lt;&gt;"none", _xlfn.CONCAT("_", table_6_5[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="57">
+    <tableColumn id="10" xr3:uid="{5E7626AE-E376-4C60-BA64-B24F95580083}" name="command" dataDxfId="58">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_common_layout.py ", "-i ", table_6_5[[#This Row],[dir]], " -rc ", table_6_5[[#This Row],[strand]], " -o ", layouts, "/", table_6_5[[#This Row],[dir_out]], " --subst_type ", table_6_5[[#This Row],[subst_type]], " --layout ", var_6_layout)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2324,44 +2324,44 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:AB42" totalsRowShown="0" headerRowDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{86CE8E4A-18BF-427A-81F0-F9655767A016}" name="table_7_1" displayName="table_7_1" ref="A2:AB42" totalsRowShown="0" headerRowDxfId="57">
   <autoFilter ref="A2:AB42" xr:uid="{73BF8355-0AB0-4422-8F65-2A32E222946E}"/>
   <tableColumns count="28">
-    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="55"/>
-    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="54">
+    <tableColumn id="25" xr3:uid="{C323C376-24D3-4404-9E0F-6E9361862271}" name="index" dataDxfId="56"/>
+    <tableColumn id="1" xr3:uid="{AC070029-7A36-442E-A851-71CD7EB80F28}" name="dir" dataDxfId="55">
       <calculatedColumnFormula>OFFSET(table_3_1[[dir]:[dir]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="53">
+    <tableColumn id="13" xr3:uid="{6A4B6748-6DA2-44B2-95C1-9C2BF9C21AC6}" name="control" dataDxfId="54">
       <calculatedColumnFormula>OFFSET(table_3_1[[control]:[control]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="52">
+    <tableColumn id="2" xr3:uid="{46183BCF-754C-4289-9E28-8DB2FB5F3E2E}" name="ref" dataDxfId="53">
       <calculatedColumnFormula>OFFSET(table_3_1[[ref]:[ref]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="51">
+    <tableColumn id="3" xr3:uid="{01CE35D5-BD5A-4DBE-911A-523BA86E9558}" name="dsb_pos" dataDxfId="52">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_pos]:[dsb_pos]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="50">
+    <tableColumn id="4" xr3:uid="{0171B01F-9599-42EC-9AD8-75EE9608FE15}" name="dsb_type" dataDxfId="51">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type]:[dsb_type]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="49">
+    <tableColumn id="12" xr3:uid="{2D9967F2-F905-4DDC-BC13-BE494C96FD78}" name="dsb_type_command" dataDxfId="50">
       <calculatedColumnFormula>OFFSET(table_3_1[[dsb_type_command]:[dsb_type_command]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="48">
+    <tableColumn id="5" xr3:uid="{B8E237AE-E973-40A0-86E3-7BF5DEC7FC87}" name="strand" dataDxfId="49">
       <calculatedColumnFormula>OFFSET(table_3_1[[strand]:[strand]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="47">
+    <tableColumn id="6" xr3:uid="{647E20CB-AEBC-4627-AE45-391FD9784E21}" name="hguide" dataDxfId="48">
       <calculatedColumnFormula>OFFSET(table_3_1[[hguide]:[hguide]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="46">
+    <tableColumn id="7" xr3:uid="{EAED7BDD-3E55-428C-8CC0-D27D2F2EF394}" name="cell" dataDxfId="47">
       <calculatedColumnFormula>OFFSET(table_3_1[[cell]:[cell]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="45">
+    <tableColumn id="8" xr3:uid="{8D720D5E-95C1-4847-85D5-656085769184}" name="treatment" dataDxfId="46">
       <calculatedColumnFormula>OFFSET(table_3_1[[treatment]:[treatment]], table_7_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="44">
+    <tableColumn id="9" xr3:uid="{D6F4320B-CD2D-4288-B9EC-64E8C7BA2DDE}" name="subst_type" dataDxfId="45">
       <calculatedColumnFormula>"without"</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="43">
+    <tableColumn id="14" xr3:uid="{C107BDC5-6E3A-4EAC-9D60-3D3C790CFE24}" name="common_layout_dir" dataDxfId="44">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[dsb_type]]="2DSBanti",
       OFFSET(table_6_5[[dir_out]:[dir_out]], 0, 0, 1, 1),
       IF(table_7_1[[#This Row],[dsb_type]] = "2DSB",
@@ -2373,45 +2373,45 @@
       )
   )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="42">
+    <tableColumn id="11" xr3:uid="{7AF47D8C-A10C-454A-8FE8-6D4A4FFD2B60}" name="reverse_complement" dataDxfId="43">
       <calculatedColumnFormula>AND(table_7_1[[#This Row],[strand]] = "R2", OR(var_7_layout = "universal", var_7_layout = "fractal", AND(var_7_layout = "radial", table_7_1[[#This Row],[dsb_type]] &lt;&gt; "1DSB")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{2D7A10AC-1675-4E76-989F-888C0D89C117}" name="range_x0" dataDxfId="41">
+    <tableColumn id="27" xr3:uid="{2D7A10AC-1675-4E76-989F-888C0D89C117}" name="range_x0" dataDxfId="42">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -12, IF(table_7_1[[#This Row],[hguide]]="CD", -12, IF(table_7_1[[#This Row],[hguide]]="A", -12, IF(table_7_1[[#This Row],[hguide]]="B", -12, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{CD6660D4-A656-4F48-89BD-45D3BAC7EE11}" name="range_x1" dataDxfId="40">
+    <tableColumn id="26" xr3:uid="{CD6660D4-A656-4F48-89BD-45D3BAC7EE11}" name="range_x1" dataDxfId="41">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 13, IF(table_7_1[[#This Row],[hguide]]="CD", 13, IF(table_7_1[[#This Row],[hguide]]="A", 13, IF(table_7_1[[#This Row],[hguide]]="B", 13, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{EFB5F04D-FC42-47A6-83B6-18FC45D14ABE}" name="range_y0" dataDxfId="39">
+    <tableColumn id="28" xr3:uid="{EFB5F04D-FC42-47A6-83B6-18FC45D14ABE}" name="range_y0" dataDxfId="40">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", -22, IF(table_7_1[[#This Row],[hguide]]="CD", -18, IF(table_7_1[[#This Row],[hguide]]="A", -23, IF(table_7_1[[#This Row],[hguide]]="B", -22, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{FCD7272B-07C5-4D80-8B2B-EFDF0948D1A3}" name="range_y1" dataDxfId="38">
+    <tableColumn id="18" xr3:uid="{FCD7272B-07C5-4D80-8B2B-EFDF0948D1A3}" name="range_y1" dataDxfId="39">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 22, IF(table_7_1[[#This Row],[hguide]]="CD", 27, IF(table_7_1[[#This Row],[hguide]]="A", 20, IF(table_7_1[[#This Row],[hguide]]="B", 16, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="37">
+    <tableColumn id="15" xr3:uid="{0D90823C-DABB-4D5B-952B-ECA267C2D98A}" name="range_args" dataDxfId="38">
       <calculatedColumnFormula>IF(var_7_layout="universal", _xlfn.CONCAT("--range_x ", table_7_1[[#This Row],[range_x0]], " ", table_7_1[[#This Row],[range_x1]], " --range_y ", table_7_1[[#This Row],[range_y0]], " ", table_7_1[[#This Row],[range_y1]]), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{862E4B1D-E776-4C82-956F-64077E0EAD63}" name="universal_layout_y_axis_args" dataDxfId="36">
+    <tableColumn id="29" xr3:uid="{862E4B1D-E776-4C82-956F-64077E0EAD63}" name="universal_layout_y_axis_args" dataDxfId="37">
       <calculatedColumnFormula>IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_x_pos ", table_7_1[[#This Row],[range_x1]] - 1, " --universal_layout_y_axis_y_range ", table_7_1[[#This Row],[range_y0]] + 2.5, " ", table_7_1[[#This Row],[range_y1]] - 1.5, " "), "")</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{80C9383B-6A26-4051-B986-65C11BA3AFE0}" name="show_universal_layout_x_axes"/>
-    <tableColumn id="23" xr3:uid="{010D8635-D593-4849-BEA6-27994308E467}" name="universal_layout_x_axis_args" dataDxfId="35">
+    <tableColumn id="23" xr3:uid="{010D8635-D593-4849-BEA6-27994308E467}" name="universal_layout_x_axis_args" dataDxfId="36">
       <calculatedColumnFormula>IF(table_7_1[[#This Row],[show_universal_layout_x_axes]], _xlfn.CONCAT(" --universal_layout_x_axis_deletion_y_pos ", table_7_1[[#This Row],[range_y0]] + 1.5, " --universal_layout_x_axis_insertion_y_pos ", table_7_1[[#This Row],[range_y1]] - 0.5, " --universal_layout_x_axis_x_range ", table_7_1[[#This Row],[range_x0]] + 0.5, " ", table_7_1[[#This Row],[range_x1]] - 1.5), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{5BFAE794-32B2-4D0D-B4C9-47939AA6DF3D}" name="universal_layout_max_tick_insertion" dataDxfId="34">
+    <tableColumn id="17" xr3:uid="{5BFAE794-32B2-4D0D-B4C9-47939AA6DF3D}" name="universal_layout_max_tick_insertion" dataDxfId="35">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 7, IF(table_7_1[[#This Row],[hguide]]="CD", 8, IF(table_7_1[[#This Row],[hguide]]="A", 6, IF(table_7_1[[#This Row],[hguide]]="B", 5, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{BDF49305-2112-4726-89DD-C9F4FFED50C5}" name="universal_layout_max_tick_deletion" dataDxfId="33">
+    <tableColumn id="19" xr3:uid="{BDF49305-2112-4726-89DD-C9F4FFED50C5}" name="universal_layout_max_tick_deletion" dataDxfId="34">
       <calculatedColumnFormula>IF(var_7_layout="universal", IF(table_7_1[[#This Row],[hguide]]="AB", 17, IF(table_7_1[[#This Row],[hguide]]="CD", 14, IF(table_7_1[[#This Row],[hguide]]="A", 19, IF(table_7_1[[#This Row],[hguide]]="B", 18, NA())))), NA())</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{9E5CCD08-C11E-4294-860A-FDFE3FE422F8}" name="universal_layout_max_tick_args" dataDxfId="32">
+    <tableColumn id="20" xr3:uid="{9E5CCD08-C11E-4294-860A-FDFE3FE422F8}" name="universal_layout_max_tick_args" dataDxfId="33">
       <calculatedColumnFormula>IF(var_7_layout="universal", _xlfn.CONCAT(" --universal_layout_y_axis_deletion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_deletion]], " --universal_layout_y_axis_insertion_max_tick ", table_7_1[[#This Row],[universal_layout_max_tick_insertion]]), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="31">
+    <tableColumn id="16" xr3:uid="{680D5200-6ABF-4323-82E5-C6AF5DA257FD}" name="output_dir" dataDxfId="32">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_1[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="21" xr3:uid="{C5B2A575-6AC4-403E-AE67-1624B7F60F7E}" name="format"/>
-    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="30">
+    <tableColumn id="10" xr3:uid="{927D810C-70D6-4266-8FCE-04D49787D147}" name="command" dataDxfId="31">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_1[[#This Row],[dir]], " -o ", table_7_1[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_1[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_1[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_1[[#This Row],[range_args]], " ", table_7_1[[#This Row],[universal_layout_y_axis_args]], " ", table_7_1[[#This Row],[universal_layout_x_axis_args]], " ", table_7_1[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2420,46 +2420,46 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:O60" totalsRowShown="0" headerRowDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}" name="table_7_2" displayName="table_7_2" ref="A44:O60" totalsRowShown="0" headerRowDxfId="30">
   <autoFilter ref="A44:O60" xr:uid="{E155FABF-AFCB-4399-AD96-6241BA80EFED}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="28"/>
-    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="27">
+    <tableColumn id="1" xr3:uid="{B2B7DB73-4221-4AF0-A850-325F3752E3E0}" name="index" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{7CBFD0EC-49AE-431E-A905-A56D19FE8F5B}" name="dir" dataDxfId="28">
       <calculatedColumnFormula>OFFSET(table_4_1[], table_7_2[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="26">
+    <tableColumn id="3" xr3:uid="{8B726DB7-A763-4D99-9E71-D69E0FA3D7BF}" name="strand" dataDxfId="27">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="25">
+    <tableColumn id="5" xr3:uid="{E7E8C40B-8285-4EE4-A61D-1F147432D708}" name="hguide" dataDxfId="26">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="24">
+    <tableColumn id="7" xr3:uid="{64B9691C-2BDA-4EE7-B149-7349BFA40A22}" name="dsb_type" dataDxfId="25">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="23">
+    <tableColumn id="2" xr3:uid="{46F7ABEC-3D59-449F-B3B9-3B53D4C4E17C}" name="common_layout_dir" dataDxfId="24">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="22">
+    <tableColumn id="8" xr3:uid="{BFEA7E87-08AD-4F58-8B7D-A592368549F0}" name="reverse_complement" dataDxfId="23">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="21">
+    <tableColumn id="9" xr3:uid="{928832B4-7BAB-42E7-88BC-BB633DA53A2E}" name="range_args" dataDxfId="22">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{0EB304B9-B5C9-435B-99CC-6F02D04A5268}" name="universal_layout_y_axis_args" dataDxfId="20">
+    <tableColumn id="12" xr3:uid="{0EB304B9-B5C9-435B-99CC-6F02D04A5268}" name="universal_layout_y_axis_args" dataDxfId="21">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_y_axis_args]:[universal_layout_y_axis_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="13" xr3:uid="{EADBB7DC-9D40-44C2-8742-A17A0EB899C3}" name="show_universal_layout_x_axes"/>
-    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_x_axis_args" dataDxfId="19">
+    <tableColumn id="11" xr3:uid="{E157268B-09A6-4B13-AD6D-24B6BD4C0B56}" name="universal_layout_x_axis_args" dataDxfId="20">
       <calculatedColumnFormula>IF(table_7_2[[#This Row],[show_universal_layout_x_axes]], OFFSET(table_7_1[[universal_layout_x_axis_args]:[universal_layout_x_axis_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{641C7B24-D16A-472B-B06C-7348DDBC60AA}" name="universal_layout_max_tick_args" dataDxfId="18">
+    <tableColumn id="14" xr3:uid="{641C7B24-D16A-472B-B06C-7348DDBC60AA}" name="universal_layout_max_tick_args" dataDxfId="19">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_max_tick_args]:[universal_layout_max_tick_args]], 3 * QUOTIENT(table_7_2[[#This Row],[index]] - 1, 2) + MOD(table_7_2[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="17">
+    <tableColumn id="10" xr3:uid="{28F0CC58-CEE1-4245-A4B6-361813C46856}" name="output_dir" dataDxfId="18">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_2[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="15" xr3:uid="{8B58B2DF-3EB7-4D4E-A96D-1BED892121E3}" name="format"/>
-    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="16">
+    <tableColumn id="6" xr3:uid="{FEA012AC-7DC4-4D11-9B59-A05887E08F6E}" name="command" dataDxfId="17">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_2[[#This Row],[dir]], " -o ", table_7_2[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_2[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_2[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_2[[#This Row],[range_args]], " ", table_7_2[[#This Row],[universal_layout_y_axis_args]], " ", table_7_2[[#This Row],[universal_layout_x_axis_args]], " ", table_7_2[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2468,46 +2468,46 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:O64" totalsRowShown="0" headerRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}" name="table_7_3" displayName="table_7_3" ref="A62:O64" totalsRowShown="0" headerRowDxfId="16">
   <autoFilter ref="A62:O64" xr:uid="{BE9A0328-D472-47BB-96EE-6A945E4CAD3B}"/>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{E718984E-FC22-4321-9162-791892D20032}" name="index" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{A71ABC91-B291-4CD9-A2A1-F6CA41CEE59E}" name="dir" dataDxfId="14">
       <calculatedColumnFormula>OFFSET(table_4_2[], table_7_3[[#This Row],[index]] - 1, _xlfn.XMATCH("dir_out", table_4_1[#Headers], 0, 1) - 1, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="12">
+    <tableColumn id="3" xr3:uid="{8D7F2EAB-990D-439F-AE1F-6FB6AFC6C4B1}" name="strand" dataDxfId="13">
       <calculatedColumnFormula>OFFSET(table_7_1[[strand]:[strand]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="11">
+    <tableColumn id="5" xr3:uid="{B8ABFFB9-C4F5-4866-8F37-B49F31C44F20}" name="hguide" dataDxfId="12">
       <calculatedColumnFormula>OFFSET(table_7_1[[hguide]:[hguide]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="10">
+    <tableColumn id="7" xr3:uid="{3835BF64-C6A9-440B-96F5-A2332AB91438}" name="dsb_type" dataDxfId="11">
       <calculatedColumnFormula>OFFSET(table_7_1[[dsb_type]:[dsb_type]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="9">
+    <tableColumn id="2" xr3:uid="{C07D080E-B5A2-43FC-84BA-BCBD008F3B26}" name="common_layout_dir" dataDxfId="10">
       <calculatedColumnFormula>OFFSET(table_7_1[[common_layout_dir]:[common_layout_dir]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="8">
+    <tableColumn id="8" xr3:uid="{6E360CD4-3BFD-4CC3-A93F-137C46B62651}" name="reverse_complement" dataDxfId="9">
       <calculatedColumnFormula>OFFSET(table_7_1[[reverse_complement]:[reverse_complement]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="7">
+    <tableColumn id="9" xr3:uid="{A1862EF0-F072-4796-964D-7EDA8C8787B0}" name="range_args" dataDxfId="8">
       <calculatedColumnFormula>OFFSET(table_7_1[[range_args]:[range_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BF1D3FB1-D45A-4909-BA3E-BB6993D39E6E}" name="universal_layout_y_axis_args" dataDxfId="6">
+    <tableColumn id="12" xr3:uid="{BF1D3FB1-D45A-4909-BA3E-BB6993D39E6E}" name="universal_layout_y_axis_args" dataDxfId="7">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_y_axis_args]:[universal_layout_y_axis_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{8D9288FF-05A5-4B58-AC7F-2C4096A25202}" name="show_universal_layout_x_axes" dataDxfId="5"/>
-    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_x_axis_args" dataDxfId="4">
+    <tableColumn id="13" xr3:uid="{8D9288FF-05A5-4B58-AC7F-2C4096A25202}" name="show_universal_layout_x_axes" dataDxfId="6"/>
+    <tableColumn id="11" xr3:uid="{312C98E0-05A4-4DD6-86F6-6BFBF9058DC2}" name="universal_layout_x_axis_args" dataDxfId="5">
       <calculatedColumnFormula>IF(table_7_3[[#This Row],[show_universal_layout_x_axes]], OFFSET(table_7_1[[universal_layout_x_axis_args]:[universal_layout_x_axis_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 2), 0, 1, 1), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{FD5F951D-27C2-4E6B-B33F-D83C250C9CC4}" name="universal_layout_max_tick_args" dataDxfId="3">
+    <tableColumn id="14" xr3:uid="{FD5F951D-27C2-4E6B-B33F-D83C250C9CC4}" name="universal_layout_max_tick_args" dataDxfId="4">
       <calculatedColumnFormula>OFFSET(table_7_1[[universal_layout_max_tick_args]:[universal_layout_max_tick_args]], 36 + 2 * QUOTIENT(table_7_3[[#This Row],[index]] - 1, 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="2">
+    <tableColumn id="10" xr3:uid="{28284CC2-E402-4A85-83F5-4FC36722329E}" name="output_dir" dataDxfId="3">
       <calculatedColumnFormula>_xlfn.CONCAT(graphs, "/", var_7_layout, "/", table_7_3[[#This Row],[format]], "/", var_7_ext)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{0AB61192-5C37-4578-ADFD-BAE568B914C5}" name="format" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="0">
+    <tableColumn id="15" xr3:uid="{0AB61192-5C37-4578-ADFD-BAE568B914C5}" name="format" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{D5ADEB9F-0405-4E9D-BDA9-7ECD31E23490}" name="command" dataDxfId="1">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/plot_graph.py ", "-i ", libraries_4, "/", table_7_3[[#This Row],[dir]], " -o ", table_7_3[[#This Row],[output_dir]], IF(var_7_common_layout, _xlfn.CONCAT(" --layout_dir ", layouts, "/", table_7_3[[#This Row],[common_layout_dir]]), ""), " -ext ", var_7_ext, " --layout ", var_7_layout, IF(table_7_3[[#This Row],[reverse_complement]], " --reverse_complement ", ""), " --width ", var_7_width, " --height ", var_7_height, " ",  table_7_3[[#This Row],[range_args]], " ", table_7_3[[#This Row],[universal_layout_y_axis_args]], " ", table_7_3[[#This Row],[universal_layout_x_axis_args]], " ", table_7_3[[#This Row],[universal_layout_max_tick_args]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2542,10 +2542,10 @@
     <tableColumn id="12" xr3:uid="{5B945FB6-D054-40C4-AAEF-BB50B19F8936}" name="total_reads" dataDxfId="210">
       <calculatedColumnFormula>VLOOKUP(INT(MID(table_1[[#This Row],[library]], 4, 10)), table_1_2[#All], IF(table_1[[#This Row],[strand]]="R1", 3, 4))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="209">
+    <tableColumn id="13" xr3:uid="{66485B06-471E-47D3-BA91-FC751F58FA5A}" name="min_length" dataDxfId="0">
       <calculatedColumnFormula>IF(LEFT(table_1[[#This Row],[dsb_type]], 1) = "2", 50, 130)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="208">
+    <tableColumn id="14" xr3:uid="{DF3C46EA-690D-4E6A-99CF-BBC2B2F74AFF}" name="command_filter_nhej" dataDxfId="209">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/filter_nhej.py", " -sam ", libraries_1, "/", table_1[[#This Row],[file_in]], " -ref ref_seq/", table_1[[#This Row],[ref]], " -o ", libraries_2, "/", table_1[[#This Row],[file_out]], ".tsv", " --min_length ", table_1[[#This Row],[min_length]], " -dsb ", table_1[[#This Row],[dsb_pos]], " --quiet")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2554,38 +2554,38 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="207">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}" name="table_2_1" displayName="table_2_1" ref="A1:S41" totalsRowShown="0" headerRowDxfId="208">
   <autoFilter ref="A1:S41" xr:uid="{DE05925F-1FF6-4367-AF1E-BAECCA464E36}"/>
   <tableColumns count="19">
-    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="206"/>
-    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="205">
+    <tableColumn id="1" xr3:uid="{C373869E-A92E-4B06-B8E5-C5A873420ED4}" name="index" dataDxfId="207"/>
+    <tableColumn id="2" xr3:uid="{A28AAC50-FA09-494A-B052-8489F07A5A70}" name="ref" dataDxfId="206">
       <calculatedColumnFormula>OFFSET(table_1[ref], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="204">
+    <tableColumn id="18" xr3:uid="{07D57089-9737-4983-8884-C4ACCDCFF6CB}" name="control" dataDxfId="205">
       <calculatedColumnFormula>OFFSET(table_1[control], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="203">
+    <tableColumn id="19" xr3:uid="{C6423FEA-272F-48D3-BC6A-909FCA937DA9}" name="dsb_type" dataDxfId="204">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="202">
+    <tableColumn id="3" xr3:uid="{B8F61088-5FFA-4860-BF4E-1BFB301A31D9}" name="dsb_pos" dataDxfId="203">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="201">
+    <tableColumn id="4" xr3:uid="{524D5B3D-BB20-420D-B7E9-93A7F77CA728}" name="cell" dataDxfId="202">
       <calculatedColumnFormula>OFFSET(table_1[cell], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="200">
+    <tableColumn id="5" xr3:uid="{CC918D20-5D79-4223-9717-2CA0EFFA213F}" name="strand" dataDxfId="201">
       <calculatedColumnFormula>OFFSET(table_1[strand], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="199">
+    <tableColumn id="6" xr3:uid="{B2851465-D533-4787-80C4-E844BB2ABB8C}" name="treatment" dataDxfId="200">
       <calculatedColumnFormula>OFFSET(table_1[treatment], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="198">
+    <tableColumn id="7" xr3:uid="{849BE448-7739-4815-A2C5-5843F62D83D7}" name="hguide" dataDxfId="199">
       <calculatedColumnFormula>OFFSET(table_1[hguide], 4 * (table_2_1[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="197">
+    <tableColumn id="8" xr3:uid="{343716D9-C3A9-4F90-A58A-42B1B9C79EBF}" name="output_dir" dataDxfId="198">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_1[[#This Row],[cell]], "_", table_2_1[[#This Row],[hguide]], "_", table_2_1[[#This Row],[strand]], "_", table_2_1[[#This Row],[treatment]], IF(table_2_1[[#This Row],[control]]&lt;&gt;"none",_xlfn.CONCAT("_", table_2_1[[#This Row],[control]]), ""))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="196">
+    <tableColumn id="9" xr3:uid="{D29558AA-D418-4CDD-81AE-A987E7BC501D}" name="input_1" dataDxfId="197">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="22" xr3:uid="{3F29C0D1-58A3-430E-AAAA-9F679DCA46D6}" name="input_2">
@@ -2597,19 +2597,19 @@
     <tableColumn id="20" xr3:uid="{28521A62-94B3-4C7C-AF90-F4E2F4163D29}" name="input_4">
       <calculatedColumnFormula array="1">OFFSET(table_1[[file_out]:[file_out]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 11, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="195">
+    <tableColumn id="10" xr3:uid="{E2ABF5A3-B032-47F7-9141-9F269EFD9D49}" name="total_reads_1" dataDxfId="196">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="194">
+    <tableColumn id="12" xr3:uid="{C7B1BE14-3BD6-413B-8575-DE9712F9761A}" name="total_reads_2" dataDxfId="195">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="193">
+    <tableColumn id="14" xr3:uid="{6A8CE344-45B9-42E3-95D8-8EB6A485D968}" name="total_reads_3" dataDxfId="194">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="192">
+    <tableColumn id="16" xr3:uid="{AC170216-9CAE-43B8-A8E2-8FE1529F6D55}" name="total_reads_4" dataDxfId="193">
       <calculatedColumnFormula array="1">OFFSET(table_1[[total_reads]:[total_reads]], 4 * (table_2_1[[#This Row],[index]:[index]] - 1) + COLUMN() - 15, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="191">
+    <tableColumn id="17" xr3:uid="{A285A0DD-6F6D-404D-AE2A-0D1FC3DDB459}" name="command" dataDxfId="192">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_1[[#This Row],[input_1]], ".tsv ", libraries_2, "/",table_2_1[[#This Row],[input_2]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_3]], ".tsv ", libraries_2, "/", table_2_1[[#This Row],[input_4]], ".tsv --total_reads ", table_2_1[[#This Row],[total_reads_1]], " ", table_2_1[[#This Row],[total_reads_2]], " ", table_2_1[[#This Row],[total_reads_3]], " ", table_2_1[[#This Row],[total_reads_4]], " -o ", libraries_3, "/", table_2_1[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2621,41 +2621,41 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}" name="table_2_2" displayName="table_2_2" ref="A44:M56" totalsRowShown="0">
   <autoFilter ref="A44:M56" xr:uid="{7D969AC7-2D2F-45B0-BA99-D174130B0A52}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="190"/>
-    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="189">
+    <tableColumn id="1" xr3:uid="{D612E3DF-AA8E-4EE0-9306-7903B4821992}" name="index" dataDxfId="191"/>
+    <tableColumn id="2" xr3:uid="{B00239B6-16E0-4472-B8C9-F25D625D21DD}" name="ref" dataDxfId="190">
       <calculatedColumnFormula>OFFSET(table_1[ref], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="188">
+    <tableColumn id="3" xr3:uid="{47FE94A7-C208-4138-B063-127D4AE215A0}" name="control" dataDxfId="189">
       <calculatedColumnFormula>OFFSET(table_1[control], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="187">
+    <tableColumn id="4" xr3:uid="{43B4F550-AB35-4206-AAAB-820BBA723DEA}" name="dsb_type" dataDxfId="188">
       <calculatedColumnFormula>OFFSET(table_1[dsb_type], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="186">
+    <tableColumn id="5" xr3:uid="{7233C674-8249-48C9-814C-599A94DF6097}" name="dsb_pos" dataDxfId="187">
       <calculatedColumnFormula>OFFSET(table_1[dsb_pos], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="185">
+    <tableColumn id="6" xr3:uid="{8FD419DF-3888-4BC8-ACF7-F31E7AB24754}" name="cell" dataDxfId="186">
       <calculatedColumnFormula>OFFSET(table_1[cell], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="184">
+    <tableColumn id="7" xr3:uid="{612FF909-1004-49E1-BC8F-F65A8C97EEFC}" name="strand" dataDxfId="185">
       <calculatedColumnFormula>OFFSET(table_1[strand], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="183">
+    <tableColumn id="8" xr3:uid="{C57AB4D7-F308-46D6-8F19-069619F8CF1B}" name="treatment" dataDxfId="184">
       <calculatedColumnFormula>OFFSET(table_1[treatment], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="182">
+    <tableColumn id="9" xr3:uid="{27DAC4C9-BDB2-4621-A4F1-0094D063284E}" name="hguide" dataDxfId="183">
       <calculatedColumnFormula>OFFSET(table_1[hguide], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="181">
+    <tableColumn id="10" xr3:uid="{E0E9E8C1-4E85-4EFB-8220-84140FBAAF8E}" name="output_dir" dataDxfId="182">
       <calculatedColumnFormula>_xlfn.CONCAT(table_2_2[[#This Row],[cell]], "_", table_2_2[[#This Row],[hguide]], "_", table_2_2[[#This Row],[strand]], "_", table_2_2[[#This Row],[treatment]], "_nodsb")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="180">
+    <tableColumn id="11" xr3:uid="{CAC474F1-3930-4766-B491-65C86C5752E8}" name="input" dataDxfId="181">
       <calculatedColumnFormula>OFFSET(table_1[file_out], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="179">
+    <tableColumn id="12" xr3:uid="{BB84920E-3487-4670-93ED-5671EACD3061}" name="total_reads" dataDxfId="180">
       <calculatedColumnFormula>OFFSET(table_1[total_reads], table_2_2[[#This Row],[index]] +  var_2_nodsb_offset - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="178">
+    <tableColumn id="13" xr3:uid="{0CE6DAF6-0C4C-4EC5-8FE5-9B3840A02412}" name="command" dataDxfId="179">
       <calculatedColumnFormula>_xlfn.CONCAT("python 1_process_nhej/combine_repeats.py -i ", libraries_2, "/", table_2_2[[#This Row],[input]], ".tsv ", " --total_reads ", table_2_2[[#This Row],[total_reads]], " -o ", libraries_3, "/", table_2_2[[#This Row],[output_dir]], ".tsv", " --quiet ")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2664,47 +2664,47 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="177">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}" name="table_3_1" displayName="table_3_1" ref="A1:N41" totalsRowShown="0" headerRowDxfId="178">
   <autoFilter ref="A1:N41" xr:uid="{5C7BFDB7-8825-4FA5-A5E3-550303D41F99}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="176"/>
-    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="175">
+    <tableColumn id="25" xr3:uid="{93D2F09B-24D5-4FE1-BF34-C037E361889F}" name="index" dataDxfId="177"/>
+    <tableColumn id="1" xr3:uid="{2F28DC66-449D-4F81-AA63-8F24B25F33D1}" name="dir" dataDxfId="176">
       <calculatedColumnFormula>OFFSET(table_2_1[output_dir], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="174">
+    <tableColumn id="13" xr3:uid="{3DF6F698-1F9A-4B05-A310-657CCFCE9F66}" name="control" dataDxfId="175">
       <calculatedColumnFormula>OFFSET(table_2_1[control], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="173">
+    <tableColumn id="2" xr3:uid="{362C2395-52F7-4A62-B7BA-2DD97ED5E6FB}" name="ref" dataDxfId="174">
       <calculatedColumnFormula>OFFSET(table_2_1[ref], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="172">
+    <tableColumn id="3" xr3:uid="{5F0895D9-2EF2-4524-8BC7-15A33FE68636}" name="dsb_pos" dataDxfId="173">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_pos], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="171">
+    <tableColumn id="4" xr3:uid="{C6D28829-46E6-4D97-8EA4-0AD12EF6CF10}" name="dsb_type" dataDxfId="172">
       <calculatedColumnFormula>OFFSET(table_2_1[dsb_type], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="170">
+    <tableColumn id="12" xr3:uid="{E8B2E211-C273-4602-86F0-60EA4259B7A4}" name="dsb_type_command" dataDxfId="171">
       <calculatedColumnFormula array="1">IF(table_3_1[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_1[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_1[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="169">
+    <tableColumn id="5" xr3:uid="{15578E86-B7BE-4D8E-8FD4-E6C9C4F35C9C}" name="strand" dataDxfId="170">
       <calculatedColumnFormula>OFFSET(table_2_1[strand], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="168">
+    <tableColumn id="6" xr3:uid="{3366AC40-6578-4797-B607-19265E7DBF5C}" name="hguide" dataDxfId="169">
       <calculatedColumnFormula>MID(OFFSET(table_2_1[hguide], table_3_1[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="167">
+    <tableColumn id="7" xr3:uid="{554F4E79-98DE-474B-A5C8-D4B536772E95}" name="cell" dataDxfId="168">
       <calculatedColumnFormula>OFFSET(table_2_1[cell], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="166">
+    <tableColumn id="8" xr3:uid="{32FC5061-DD85-4234-9ED8-FEAF6D9E3BC0}" name="treatment" dataDxfId="167">
       <calculatedColumnFormula>OFFSET(table_2_1[treatment], table_3_1[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{DB6998A3-1431-4DDD-8DA0-525B805BF436}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="165">
+    <tableColumn id="10" xr3:uid="{367B0912-E7A8-4430-962D-4F79EE14E5EA}" name="command_main_data" dataDxfId="166">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_1[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_1[[#This Row],[dir]], " -ref ref_seq/", table_3_1[[#This Row],[ref]], " -dsb ", table_3_1[[#This Row],[dsb_pos]], " --dsb_type ",table_3_1[[#This Row],[dsb_type_command]], " --strand ", table_3_1[[#This Row],[strand]], " --hguide ", table_3_1[[#This Row],[hguide]], " --cell ", table_3_1[[#This Row],[cell]], " --treatment ", table_3_1[[#This Row],[treatment]], " --subst_type ", table_3_1[[#This Row],[subst_type]], " --control ", table_3_1[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="164">
+    <tableColumn id="11" xr3:uid="{4A65279E-321E-4E3E-8383-26D448C2012F}" name="command_graph_data" dataDxfId="165">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_1[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2713,47 +2713,47 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="163">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}" name="table_3_2" displayName="table_3_2" ref="A43:N55" totalsRowShown="0" headerRowDxfId="164">
   <autoFilter ref="A43:N55" xr:uid="{D5160C95-D2BA-47CB-B22B-E91EC7D3F498}"/>
   <tableColumns count="14">
-    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="162"/>
-    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="161">
+    <tableColumn id="25" xr3:uid="{B2894846-EBB9-47DC-8DE1-7F1DA571A0B9}" name="index" dataDxfId="163"/>
+    <tableColumn id="1" xr3:uid="{98269DFC-71F0-4066-B063-59597431C1C3}" name="dir" dataDxfId="162">
       <calculatedColumnFormula>OFFSET(table_2_2[output_dir], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="160">
+    <tableColumn id="13" xr3:uid="{EB55B964-D8E2-4E0C-B7CF-07043E026664}" name="control" dataDxfId="161">
       <calculatedColumnFormula>OFFSET(table_2_2[control], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="159">
+    <tableColumn id="2" xr3:uid="{7A83EC55-03CE-4608-92D6-6F1C53B539FE}" name="ref" dataDxfId="160">
       <calculatedColumnFormula>OFFSET(table_2_2[ref], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="158">
+    <tableColumn id="3" xr3:uid="{13E984FC-9FD2-479F-AB4C-B74DDF5FD234}" name="dsb_pos" dataDxfId="159">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_pos], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="157">
+    <tableColumn id="4" xr3:uid="{EF0F2447-2FA1-4517-A5CE-D8DDAAC8D3F2}" name="dsb_type" dataDxfId="158">
       <calculatedColumnFormula>OFFSET(table_2_2[dsb_type], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="156">
+    <tableColumn id="12" xr3:uid="{A1849AE1-952B-42B5-99EE-20BD2E4C5A6A}" name="dsb_type_command" dataDxfId="157">
       <calculatedColumnFormula array="1">IF(table_3_2[[#This Row],[dsb_type]]="2DSB", "2", IF(table_3_2[[#This Row],[dsb_type]]="2DSBanti", "2a", IF(table_3_2[[#This Row],[dsb_type]]="1DSB", "1", NA)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="155">
+    <tableColumn id="5" xr3:uid="{625E12FC-BF17-4E65-99DB-EDD53FEF055D}" name="strand" dataDxfId="156">
       <calculatedColumnFormula>OFFSET(table_2_2[strand], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="154">
+    <tableColumn id="6" xr3:uid="{0ABF747E-328F-4A80-85AA-4AF871C860C1}" name="hguide" dataDxfId="155">
       <calculatedColumnFormula>MID(OFFSET(table_2_2[hguide], table_3_2[[#This Row],[index]] - 1, 0, 1, 1), 3, 100)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="153">
+    <tableColumn id="7" xr3:uid="{29D6C48B-05B8-42C6-88A9-0939BC454FE0}" name="cell" dataDxfId="154">
       <calculatedColumnFormula>OFFSET(table_2_2[cell], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="152">
+    <tableColumn id="8" xr3:uid="{BD269EBE-94A9-4B57-B984-C7566AC259DE}" name="treatment" dataDxfId="153">
       <calculatedColumnFormula>OFFSET(table_2_2[treatment], table_3_2[[#This Row],[index]] - 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="9" xr3:uid="{142C480D-E258-4979-A008-3940A3FE78E4}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="151">
+    <tableColumn id="10" xr3:uid="{19804410-83AB-479E-A819-2D7449105C25}" name="command_main_data" dataDxfId="152">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data.py ", "-i ", libraries_3, "/",table_3_2[[#This Row],[dir]], ".tsv -o ", libraries_4, "/", table_3_2[[#This Row],[dir]], " -ref ref_seq/", table_3_2[[#This Row],[ref]], " -dsb ", table_3_2[[#This Row],[dsb_pos]], " --dsb_type ",table_3_2[[#This Row],[dsb_type_command]], " --strand ", table_3_2[[#This Row],[strand]], " --hguide ", table_3_2[[#This Row],[hguide]], " --cell ", table_3_2[[#This Row],[cell]], " --treatment ", table_3_2[[#This Row],[treatment]], " --subst_type ", table_3_2[[#This Row],[subst_type]], " --control ", table_3_2[[#This Row],[control]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="150">
+    <tableColumn id="11" xr3:uid="{212A69BD-0F88-401C-957F-8B6EC8E55AED}" name="command_graph_data" dataDxfId="151">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_3_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_3_2[[#This Row],[dir]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2762,38 +2762,38 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="149">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}" name="table_4_1" displayName="table_4_1" ref="A1:K17" totalsRowShown="0" headerRowDxfId="150">
   <autoFilter ref="A1:K17" xr:uid="{3ADBC687-3D92-491E-B36B-6CC1BB3B3380}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="148"/>
-    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="147">
+    <tableColumn id="1" xr3:uid="{B7EC223D-BA24-48F1-9EE3-DC56DEFDE4C2}" name="index" dataDxfId="149"/>
+    <tableColumn id="7" xr3:uid="{D9F1ADDA-18A2-4F81-862D-6B0F786079FF}" name="control" dataDxfId="148">
       <calculatedColumnFormula>OFFSET(table_3_1[control], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="146">
+    <tableColumn id="8" xr3:uid="{0EA5A81F-6EA1-4256-9717-03273165F7BF}" name="treatment_1" dataDxfId="147">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="145">
+    <tableColumn id="2" xr3:uid="{5F6D005A-96D8-4801-93E2-101BAE551BA8}" name="dir_1" dataDxfId="146">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="144">
+    <tableColumn id="9" xr3:uid="{C21D1AF7-7ABE-4181-AA2A-42227869A8DD}" name="treatment_2" dataDxfId="145">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="143">
+    <tableColumn id="3" xr3:uid="{D66426AC-E0B2-4B07-A4D4-5A74AA033E80}" name="dir_2" dataDxfId="144">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], 3 * QUOTIENT(table_4_1[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_1[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="142">
+    <tableColumn id="10" xr3:uid="{0C8146A0-DC77-4DC4-82FF-74F4C74CF33E}" name="treatments_out" dataDxfId="143">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_1[[#This Row],[treatment_1]], "_", table_4_1[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="141">
+    <tableColumn id="4" xr3:uid="{519A6397-7A3C-4009-B8B9-A71C0B3A591B}" name="dir_out" dataDxfId="142">
       <calculatedColumnFormula>SUBSTITUTE(table_4_1[[#This Row],[dir_1]], table_4_1[[#This Row],[treatment_1]], table_4_1[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="140">
+    <tableColumn id="5" xr3:uid="{E1629355-7D02-4819-98A1-EEB3B5FADE18}" name="subst_type" dataDxfId="141">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="139">
+    <tableColumn id="6" xr3:uid="{BC9117A0-CB6F-4D3C-A0E4-BF8395854D9A}" name="command_main_data_combined" dataDxfId="140">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_1[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_1[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_1[[#This Row],[dir_out]], " --subst_type ", table_4_1[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="138">
+    <tableColumn id="11" xr3:uid="{D384013E-9937-4DD8-A36A-43325757359B}" name="command_graph_data" dataDxfId="139">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_1[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_1[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2802,38 +2802,38 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="137">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}" name="table_4_2" displayName="table_4_2" ref="A20:K22" totalsRowShown="0" headerRowDxfId="138">
   <autoFilter ref="A20:K22" xr:uid="{44E39C67-02E4-4910-8670-BA7FFCEEEAF8}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="136"/>
-    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="135">
+    <tableColumn id="1" xr3:uid="{7F5A3A15-751D-407C-A035-61B2605E693F}" name="index" dataDxfId="137"/>
+    <tableColumn id="7" xr3:uid="{45863AB0-FD32-49FE-B4BF-F8EE865F7604}" name="control" dataDxfId="136">
       <calculatedColumnFormula>OFFSET(table_3_1[control], var_4_anti_offset + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="134">
+    <tableColumn id="8" xr3:uid="{CD16648D-267E-410B-A366-3E12367C037C}" name="treatment_1" dataDxfId="135">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="133">
+    <tableColumn id="2" xr3:uid="{10C9F90E-86FD-4BFE-939E-298FD6F69F12}" name="dir_1" dataDxfId="134">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="132">
+    <tableColumn id="9" xr3:uid="{7AB3E4AB-F43B-4FDE-96D7-FBBB4A8B83BE}" name="treatment_2" dataDxfId="133">
       <calculatedColumnFormula>OFFSET(table_3_1[treatment], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="131">
+    <tableColumn id="3" xr3:uid="{BF948A3E-9649-41BF-A7E7-57BFDE810FE9}" name="dir_2" dataDxfId="132">
       <calculatedColumnFormula>OFFSET(table_3_1[dir], var_4_anti_offset - 1 + 2 * (table_4_2[[#This Row],[index]] - 1) + 1, 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="130">
+    <tableColumn id="10" xr3:uid="{378119E5-F021-4785-A653-4D632F029AA6}" name="treatments_out" dataDxfId="131">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_2[[#This Row],[treatment_1]], "_", table_4_2[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="129">
+    <tableColumn id="4" xr3:uid="{AE1A14DC-D0C9-4818-B8CC-09A571E73BC2}" name="dir_out" dataDxfId="130">
       <calculatedColumnFormula>SUBSTITUTE(table_4_2[[#This Row],[dir_1]], table_4_2[[#This Row],[treatment_1]], table_4_2[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{F29DAC4E-FEC5-4C1D-AAC1-7CE19E401F25}" name="subst_type">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="128">
+    <tableColumn id="6" xr3:uid="{DC4E99F4-97AB-4553-A5FB-D20D3D487947}" name="command_main_data_combined" dataDxfId="129">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_2[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_2[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_2[[#This Row],[dir_out]], " --subst_type ", table_4_2[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="127">
+    <tableColumn id="11" xr3:uid="{E19D3001-2E76-4CC2-BF33-D0465C77D538}" name="command_graph_data" dataDxfId="128">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_2[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_2[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2842,38 +2842,38 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}" name="table_4_3" displayName="table_4_3" ref="A25:K33" totalsRowShown="0" headerRowDxfId="127">
   <autoFilter ref="A25:K33" xr:uid="{7D35E6FC-E7CD-464B-90E4-DB03DC258109}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="125"/>
-    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="124">
+    <tableColumn id="1" xr3:uid="{33AF3495-7432-4F03-9832-525A370EADEC}" name="index" dataDxfId="126"/>
+    <tableColumn id="7" xr3:uid="{3D66515C-5022-4D48-A834-4320DA4E73F6}" name="control" dataDxfId="125">
       <calculatedColumnFormula>OFFSET(table_3_2[control], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="123">
+    <tableColumn id="8" xr3:uid="{294B17A9-F0F9-42CA-8342-55C00648E3A5}" name="treatment_1" dataDxfId="124">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="122">
+    <tableColumn id="2" xr3:uid="{E13C38CF-C105-4AB5-8602-7D32E688C737}" name="dir_1" dataDxfId="123">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="121">
+    <tableColumn id="9" xr3:uid="{15B3CC7F-2A3C-4026-8417-A9DD21E4F004}" name="treatment_2" dataDxfId="122">
       <calculatedColumnFormula>OFFSET(table_3_2[treatment], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="120">
+    <tableColumn id="3" xr3:uid="{FF7D9AD3-1A35-4013-88AE-0C00465033CD}" name="dir_2" dataDxfId="121">
       <calculatedColumnFormula>OFFSET(table_3_2[dir], 3 * QUOTIENT(table_4_3[[#This Row],[index]] - 1, 2) + 1 + MOD(table_4_3[[#This Row],[index]] - 1, 2), 0, 1, 1)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="119">
+    <tableColumn id="10" xr3:uid="{9353B2D3-0D23-4FBB-AFEC-EB68549160F4}" name="treatments_out" dataDxfId="120">
       <calculatedColumnFormula>_xlfn.CONCAT(table_4_3[[#This Row],[treatment_1]], "_", table_4_3[[#This Row],[treatment_2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="118">
+    <tableColumn id="4" xr3:uid="{77F1D6F0-DE95-4E63-9E7E-D3CA3CF85F37}" name="dir_out" dataDxfId="119">
       <calculatedColumnFormula>SUBSTITUTE(table_4_3[[#This Row],[dir_1]], table_4_3[[#This Row],[treatment_1]], table_4_3[[#This Row],[treatments_out]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="117">
+    <tableColumn id="5" xr3:uid="{BBF4F840-178E-461E-8C17-36D699EDE038}" name="subst_type" dataDxfId="118">
       <calculatedColumnFormula>subst_type</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="116">
+    <tableColumn id="6" xr3:uid="{9434BF8B-81C5-43DF-BCB7-FA7146BF2FE8}" name="command_main_data_combined" dataDxfId="117">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_main_data_combined.py", " -i ", libraries_4, "/", table_4_3[[#This Row],[dir_1]], " ", libraries_4, "/", table_4_3[[#This Row],[dir_2]], " -o ", libraries_4, "/", table_4_3[[#This Row],[dir_out]], " --subst_type ", table_4_3[[#This Row],[subst_type]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="115">
+    <tableColumn id="11" xr3:uid="{1ABF0B7B-4ECE-42BF-A7D8-EA13E98144EE}" name="command_graph_data" dataDxfId="116">
       <calculatedColumnFormula>_xlfn.CONCAT("python 2_graph_processing/make_graph_data.py", " --subst_type ", table_4_3[[#This Row],[subst_type]], " -dir ", libraries_4, "/", table_4_3[[#This Row],[dir_out]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5007,8 +5007,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40F1EACD-27DC-4973-8E3A-9162F610D9C4}">
   <dimension ref="A1:O176"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C133" workbookViewId="0">
-      <selection activeCell="J146" sqref="J146"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N119" sqref="N119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>